<commit_message>
corretta applicabilità sul file xls
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB98CF1-4888-4A6E-AD4A-2E1D4F4A6C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5A32A5-71C5-4E3C-9856-3B039ABAB2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="718">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4652,14 +4652,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W770"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="Q191" sqref="Q191:Q192"/>
+      <selection pane="bottomRight" activeCell="J191" sqref="J191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5111,7 +5110,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="31">
         <v>30</v>
       </c>
@@ -5266,7 +5265,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
         <v>33</v>
       </c>
@@ -5303,7 +5302,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="31">
         <v>34</v>
       </c>
@@ -5340,7 +5339,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="31">
         <v>35</v>
       </c>
@@ -5490,7 +5489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="31">
         <v>38</v>
       </c>
@@ -5645,7 +5644,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="31">
         <v>41</v>
       </c>
@@ -5682,7 +5681,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="31">
         <v>42</v>
       </c>
@@ -5719,7 +5718,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="31">
         <v>43</v>
       </c>
@@ -5872,7 +5871,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="31">
         <v>46</v>
       </c>
@@ -6029,7 +6028,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="31">
         <v>49</v>
       </c>
@@ -6068,7 +6067,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="31">
         <v>50</v>
       </c>
@@ -6107,7 +6106,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="31">
         <v>51</v>
       </c>
@@ -8672,7 +8671,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="31">
         <v>94</v>
       </c>
@@ -8711,7 +8710,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="31">
         <v>95</v>
       </c>
@@ -8750,7 +8749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="31">
         <v>96</v>
       </c>
@@ -8789,7 +8788,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="31">
         <v>97</v>
       </c>
@@ -8826,7 +8825,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="31">
         <v>98</v>
       </c>
@@ -8863,7 +8862,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="31">
         <v>99</v>
       </c>
@@ -8900,7 +8899,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="31">
         <v>100</v>
       </c>
@@ -8937,7 +8936,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="31">
         <v>101</v>
       </c>
@@ -8974,7 +8973,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="31">
         <v>102</v>
       </c>
@@ -9011,7 +9010,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="31">
         <v>103</v>
       </c>
@@ -9048,7 +9047,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="31">
         <v>104</v>
       </c>
@@ -9085,7 +9084,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="31">
         <v>105</v>
       </c>
@@ -9122,7 +9121,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="31">
         <v>106</v>
       </c>
@@ -9159,7 +9158,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="31">
         <v>107</v>
       </c>
@@ -9196,7 +9195,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="31">
         <v>108</v>
       </c>
@@ -9233,7 +9232,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="31">
         <v>109</v>
       </c>
@@ -9270,7 +9269,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="31">
         <v>110</v>
       </c>
@@ -9307,7 +9306,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="31">
         <v>111</v>
       </c>
@@ -9344,7 +9343,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="31">
         <v>112</v>
       </c>
@@ -9381,7 +9380,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="31">
         <v>113</v>
       </c>
@@ -9418,7 +9417,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="31">
         <v>114</v>
       </c>
@@ -9455,7 +9454,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="31">
         <v>115</v>
       </c>
@@ -9492,7 +9491,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="31">
         <v>116</v>
       </c>
@@ -9529,7 +9528,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="31">
         <v>117</v>
       </c>
@@ -9566,7 +9565,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="31">
         <v>118</v>
       </c>
@@ -9603,7 +9602,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="31">
         <v>119</v>
       </c>
@@ -9640,7 +9639,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="31">
         <v>120</v>
       </c>
@@ -9677,7 +9676,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="31">
         <v>121</v>
       </c>
@@ -9714,7 +9713,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="31">
         <v>122</v>
       </c>
@@ -9751,7 +9750,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="31">
         <v>123</v>
       </c>
@@ -9788,7 +9787,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="31">
         <v>124</v>
       </c>
@@ -9825,7 +9824,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="31">
         <v>125</v>
       </c>
@@ -9862,7 +9861,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="31">
         <v>126</v>
       </c>
@@ -9899,7 +9898,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="31">
         <v>127</v>
       </c>
@@ -9936,7 +9935,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="31">
         <v>128</v>
       </c>
@@ -9973,7 +9972,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="31">
         <v>129</v>
       </c>
@@ -10010,7 +10009,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="31">
         <v>130</v>
       </c>
@@ -10047,7 +10046,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="31">
         <v>131</v>
       </c>
@@ -10084,7 +10083,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="31">
         <v>132</v>
       </c>
@@ -10121,7 +10120,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="31">
         <v>133</v>
       </c>
@@ -10158,7 +10157,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="31">
         <v>134</v>
       </c>
@@ -10195,7 +10194,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="31">
         <v>135</v>
       </c>
@@ -10232,7 +10231,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="31">
         <v>136</v>
       </c>
@@ -10269,7 +10268,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="31">
         <v>137</v>
       </c>
@@ -10306,7 +10305,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="31">
         <v>138</v>
       </c>
@@ -10343,7 +10342,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="31">
         <v>139</v>
       </c>
@@ -10380,7 +10379,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="31">
         <v>140</v>
       </c>
@@ -10417,7 +10416,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="31">
         <v>141</v>
       </c>
@@ -10454,7 +10453,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="31">
         <v>142</v>
       </c>
@@ -10491,7 +10490,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="31">
         <v>143</v>
       </c>
@@ -10528,7 +10527,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="31">
         <v>144</v>
       </c>
@@ -10565,7 +10564,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="31">
         <v>145</v>
       </c>
@@ -10602,7 +10601,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="31">
         <v>146</v>
       </c>
@@ -11701,7 +11700,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="31">
         <v>174</v>
       </c>
@@ -11740,7 +11739,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="149" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="31">
         <v>175</v>
       </c>
@@ -11779,7 +11778,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="150" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="31">
         <v>176</v>
       </c>
@@ -11818,7 +11817,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="31">
         <v>177</v>
       </c>
@@ -11857,7 +11856,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="31">
         <v>178</v>
       </c>
@@ -11896,7 +11895,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="31">
         <v>179</v>
       </c>
@@ -11933,7 +11932,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="31">
         <v>180</v>
       </c>
@@ -11970,7 +11969,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="31">
         <v>181</v>
       </c>
@@ -12007,7 +12006,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="31">
         <v>182</v>
       </c>
@@ -12044,7 +12043,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="31">
         <v>183</v>
       </c>
@@ -12081,7 +12080,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="31">
         <v>184</v>
       </c>
@@ -12118,7 +12117,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="31">
         <v>185</v>
       </c>
@@ -12155,7 +12154,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="31">
         <v>186</v>
       </c>
@@ -12192,7 +12191,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="31">
         <v>187</v>
       </c>
@@ -12229,7 +12228,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="31">
         <v>188</v>
       </c>
@@ -12266,7 +12265,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="31">
         <v>189</v>
       </c>
@@ -12303,7 +12302,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="164" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="31">
         <v>190</v>
       </c>
@@ -12426,7 +12425,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="31">
         <v>417</v>
       </c>
@@ -12463,7 +12462,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="31">
         <v>418</v>
       </c>
@@ -12500,7 +12499,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="31">
         <v>419</v>
       </c>
@@ -12537,7 +12536,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="31">
         <v>423</v>
       </c>
@@ -12574,7 +12573,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="171" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="31">
         <v>424</v>
       </c>
@@ -12611,7 +12610,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="172" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="31">
         <v>425</v>
       </c>
@@ -12648,7 +12647,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="173" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="31">
         <v>426</v>
       </c>
@@ -12685,7 +12684,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="31">
         <v>432</v>
       </c>
@@ -12722,7 +12721,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="175" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="31">
         <v>433</v>
       </c>
@@ -12759,7 +12758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="176" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="31">
         <v>434</v>
       </c>
@@ -12796,7 +12795,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="31">
         <v>435</v>
       </c>
@@ -12833,7 +12832,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="31">
         <v>437</v>
       </c>
@@ -12870,7 +12869,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="31">
         <v>438</v>
       </c>
@@ -12907,7 +12906,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="31">
         <v>440</v>
       </c>
@@ -12944,7 +12943,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="31">
         <v>441</v>
       </c>
@@ -12981,7 +12980,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="31">
         <v>442</v>
       </c>
@@ -13018,7 +13017,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="31">
         <v>443</v>
       </c>
@@ -13055,7 +13054,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="31">
         <v>444</v>
       </c>
@@ -13092,7 +13091,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="31">
         <v>445</v>
       </c>
@@ -13157,7 +13156,9 @@
       <c r="I186" s="42" t="s">
         <v>607</v>
       </c>
-      <c r="J186" s="43"/>
+      <c r="J186" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K186" s="43"/>
       <c r="L186" s="43"/>
       <c r="M186" s="43" t="s">
@@ -13214,7 +13215,9 @@
       <c r="I187" s="42" t="s">
         <v>610</v>
       </c>
-      <c r="J187" s="43"/>
+      <c r="J187" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K187" s="43"/>
       <c r="L187" s="43"/>
       <c r="M187" s="43" t="s">
@@ -13271,7 +13274,9 @@
       <c r="I188" s="42" t="s">
         <v>672</v>
       </c>
-      <c r="J188" s="43"/>
+      <c r="J188" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K188" s="43"/>
       <c r="L188" s="43"/>
       <c r="M188" s="43"/>
@@ -13318,7 +13323,9 @@
       <c r="I189" s="42" t="s">
         <v>675</v>
       </c>
-      <c r="J189" s="43"/>
+      <c r="J189" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K189" s="43"/>
       <c r="L189" s="43"/>
       <c r="M189" s="43"/>
@@ -13365,7 +13372,9 @@
       <c r="I190" s="42" t="s">
         <v>562</v>
       </c>
-      <c r="J190" s="43"/>
+      <c r="J190" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K190" s="43"/>
       <c r="L190" s="43"/>
       <c r="M190" s="43"/>
@@ -13414,7 +13423,9 @@
       <c r="I191" s="42" t="s">
         <v>566</v>
       </c>
-      <c r="J191" s="43"/>
+      <c r="J191" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K191" s="43"/>
       <c r="L191" s="43"/>
       <c r="M191" s="43"/>
@@ -13461,7 +13472,9 @@
       <c r="I192" s="42" t="s">
         <v>537</v>
       </c>
-      <c r="J192" s="43"/>
+      <c r="J192" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K192" s="43"/>
       <c r="L192" s="43"/>
       <c r="M192" s="43"/>
@@ -13488,7 +13501,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="193" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="31">
         <v>454</v>
       </c>
@@ -13525,7 +13538,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="194" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="31">
         <v>455</v>
       </c>
@@ -13562,7 +13575,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="195" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="31">
         <v>456</v>
       </c>
@@ -13599,7 +13612,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="196" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="31">
         <v>457</v>
       </c>
@@ -13636,7 +13649,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="197" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="31">
         <v>458</v>
       </c>
@@ -13673,7 +13686,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="31">
         <v>459</v>
       </c>
@@ -13710,7 +13723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="199" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="31">
         <v>460</v>
       </c>
@@ -18118,16 +18131,7 @@
       <c r="W770" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:W200" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="LAB"/>
-        <filter val="LDO"/>
-        <filter val="RAD"/>
-        <filter val="RSA"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:W200" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -20407,6 +20411,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F560B38A5B3C4B41B1895754B1F1A56A" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="69dc0f489d46816a4b9bb4a327e14425">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca719f03-9e45-4ef4-9920-d156f53157f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7de9a44ff87fdcabda187bbd662e75de" ns2:_="">
     <xsd:import namespace="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
@@ -20578,26 +20601,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20615,32 +20645,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
corretto xls per colonna esito
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5A32A5-71C5-4E3C-9856-3B039ABAB2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04035190-2327-486D-93C8-F7DE54374D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="718">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4655,10 +4655,10 @@
   <dimension ref="A1:W770"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J191" sqref="J191"/>
+      <selection pane="bottomRight" activeCell="T200" sqref="T200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5040,9 +5040,7 @@
       </c>
       <c r="R11" s="43"/>
       <c r="S11" s="43"/>
-      <c r="T11" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T11" s="43"/>
       <c r="U11" s="44"/>
       <c r="V11" s="45" t="s">
         <v>460</v>
@@ -5101,9 +5099,7 @@
       <c r="S12" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T12" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T12" s="43"/>
       <c r="U12" s="44"/>
       <c r="V12" s="45"/>
       <c r="W12" s="43" t="s">
@@ -5197,9 +5193,7 @@
       <c r="S14" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T14" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T14" s="43"/>
       <c r="U14" s="44"/>
       <c r="V14" s="45"/>
       <c r="W14" s="43" t="s">
@@ -5256,9 +5250,7 @@
       <c r="S15" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T15" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T15" s="43"/>
       <c r="U15" s="44"/>
       <c r="V15" s="45"/>
       <c r="W15" s="43" t="s">
@@ -5420,9 +5412,7 @@
       </c>
       <c r="R19" s="43"/>
       <c r="S19" s="43"/>
-      <c r="T19" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T19" s="43"/>
       <c r="U19" s="44"/>
       <c r="V19" s="45" t="s">
         <v>463</v>
@@ -5481,9 +5471,7 @@
       <c r="S20" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T20" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T20" s="43"/>
       <c r="V20" s="45"/>
       <c r="W20" s="43" t="s">
         <v>46</v>
@@ -5576,9 +5564,7 @@
       <c r="S22" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T22" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T22" s="43"/>
       <c r="U22" s="44"/>
       <c r="V22" s="45"/>
       <c r="W22" s="43" t="s">
@@ -5635,9 +5621,7 @@
       <c r="S23" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T23" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T23" s="43"/>
       <c r="U23" s="44"/>
       <c r="V23" s="45"/>
       <c r="W23" s="43" t="s">
@@ -5801,9 +5785,7 @@
       <c r="S27" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T27" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T27" s="43"/>
       <c r="U27" s="44" t="s">
         <v>66</v>
       </c>
@@ -5860,9 +5842,7 @@
       <c r="S28" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T28" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T28" s="43"/>
       <c r="U28" s="44" t="s">
         <v>66</v>
       </c>
@@ -5958,9 +5938,7 @@
       <c r="S30" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T30" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T30" s="43"/>
       <c r="U30" s="44" t="s">
         <v>66</v>
       </c>
@@ -6017,9 +5995,7 @@
       <c r="S31" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T31" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T31" s="43"/>
       <c r="U31" s="44" t="s">
         <v>66</v>
       </c>
@@ -6195,9 +6171,7 @@
       <c r="S35" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T35" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T35" s="43"/>
       <c r="U35" s="44"/>
       <c r="V35" s="45" t="s">
         <v>457</v>
@@ -6256,9 +6230,7 @@
       <c r="S36" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T36" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T36" s="43"/>
       <c r="U36" s="44"/>
       <c r="V36" s="45"/>
       <c r="W36" s="43" t="s">
@@ -6315,9 +6287,7 @@
       <c r="S37" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T37" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T37" s="43"/>
       <c r="U37" s="44"/>
       <c r="V37" s="45" t="s">
         <v>475</v>
@@ -6376,9 +6346,7 @@
       <c r="S38" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T38" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T38" s="43"/>
       <c r="U38" s="44"/>
       <c r="V38" s="45"/>
       <c r="W38" s="43" t="s">
@@ -6435,9 +6403,7 @@
       <c r="S39" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T39" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T39" s="43"/>
       <c r="U39" s="44"/>
       <c r="V39" s="45"/>
       <c r="W39" s="43" t="s">
@@ -6494,9 +6460,7 @@
       <c r="S40" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T40" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T40" s="43"/>
       <c r="U40" s="44"/>
       <c r="V40" s="45"/>
       <c r="W40" s="43" t="s">
@@ -6553,9 +6517,7 @@
       <c r="S41" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T41" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T41" s="43"/>
       <c r="U41" s="44"/>
       <c r="V41" s="45"/>
       <c r="W41" s="43" t="s">
@@ -6612,9 +6574,7 @@
       <c r="S42" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T42" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T42" s="43"/>
       <c r="U42" s="44"/>
       <c r="V42" s="45"/>
       <c r="W42" s="43" t="s">
@@ -6671,9 +6631,7 @@
       <c r="S43" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T43" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T43" s="43"/>
       <c r="U43" s="44"/>
       <c r="V43" s="45"/>
       <c r="W43" s="43" t="s">
@@ -6730,9 +6688,7 @@
       <c r="S44" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T44" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T44" s="43"/>
       <c r="U44" s="44" t="s">
         <v>493</v>
       </c>
@@ -6791,9 +6747,7 @@
       <c r="S45" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T45" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T45" s="43"/>
       <c r="U45" s="44" t="s">
         <v>494</v>
       </c>
@@ -6852,9 +6806,7 @@
       <c r="S46" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T46" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T46" s="43"/>
       <c r="U46" s="44" t="s">
         <v>495</v>
       </c>
@@ -6913,9 +6865,7 @@
       <c r="S47" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T47" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T47" s="43"/>
       <c r="U47" s="44" t="s">
         <v>496</v>
       </c>
@@ -6976,9 +6926,7 @@
       <c r="S48" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T48" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T48" s="43"/>
       <c r="U48" s="44" t="s">
         <v>498</v>
       </c>
@@ -7037,9 +6985,7 @@
       <c r="S49" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T49" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T49" s="43"/>
       <c r="U49" s="44" t="s">
         <v>499</v>
       </c>
@@ -7098,9 +7044,7 @@
       <c r="S50" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T50" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T50" s="43"/>
       <c r="U50" s="44" t="s">
         <v>500</v>
       </c>
@@ -7159,9 +7103,7 @@
       <c r="S51" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T51" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T51" s="43"/>
       <c r="U51" s="44" t="s">
         <v>501</v>
       </c>
@@ -7220,9 +7162,7 @@
       <c r="S52" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T52" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T52" s="43"/>
       <c r="U52" s="44" t="s">
         <v>502</v>
       </c>
@@ -7281,9 +7221,7 @@
       <c r="S53" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T53" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T53" s="43"/>
       <c r="U53" s="44" t="s">
         <v>503</v>
       </c>
@@ -7342,9 +7280,7 @@
       <c r="S54" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T54" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T54" s="43"/>
       <c r="U54" s="44" t="s">
         <v>504</v>
       </c>
@@ -7403,9 +7339,7 @@
       <c r="S55" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T55" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T55" s="43"/>
       <c r="U55" s="44" t="s">
         <v>505</v>
       </c>
@@ -7464,9 +7398,7 @@
       <c r="S56" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T56" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T56" s="43"/>
       <c r="U56" s="44" t="s">
         <v>506</v>
       </c>
@@ -7525,9 +7457,7 @@
       <c r="S57" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T57" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T57" s="43"/>
       <c r="U57" s="44" t="s">
         <v>507</v>
       </c>
@@ -7586,9 +7516,7 @@
       <c r="S58" s="43" t="s">
         <v>583</v>
       </c>
-      <c r="T58" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T58" s="43"/>
       <c r="U58" s="44" t="s">
         <v>508</v>
       </c>
@@ -7647,9 +7575,7 @@
       <c r="S59" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T59" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T59" s="43"/>
       <c r="U59" s="44" t="s">
         <v>509</v>
       </c>
@@ -7708,9 +7634,7 @@
       <c r="S60" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T60" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T60" s="43"/>
       <c r="U60" s="44" t="s">
         <v>510</v>
       </c>
@@ -7769,9 +7693,7 @@
       <c r="S61" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T61" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T61" s="43"/>
       <c r="U61" s="44" t="s">
         <v>511</v>
       </c>
@@ -7830,9 +7752,7 @@
       <c r="S62" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T62" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T62" s="43"/>
       <c r="U62" s="44" t="s">
         <v>512</v>
       </c>
@@ -7891,9 +7811,7 @@
       <c r="S63" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T63" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T63" s="43"/>
       <c r="U63" s="44" t="s">
         <v>513</v>
       </c>
@@ -7952,9 +7870,7 @@
       <c r="S64" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T64" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T64" s="43"/>
       <c r="U64" s="44" t="s">
         <v>514</v>
       </c>
@@ -8013,9 +7929,7 @@
       <c r="S65" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T65" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T65" s="43"/>
       <c r="U65" s="44"/>
       <c r="V65" s="45"/>
       <c r="W65" s="43" t="s">
@@ -8072,9 +7986,7 @@
       <c r="S66" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T66" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T66" s="43"/>
       <c r="U66" s="44"/>
       <c r="V66" s="45"/>
       <c r="W66" s="43" t="s">
@@ -8131,9 +8043,7 @@
       <c r="S67" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T67" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T67" s="43"/>
       <c r="U67" s="44"/>
       <c r="V67" s="45"/>
       <c r="W67" s="43" t="s">
@@ -8190,9 +8100,7 @@
       <c r="S68" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T68" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T68" s="43"/>
       <c r="U68" s="44"/>
       <c r="V68" s="45"/>
       <c r="W68" s="43" t="s">
@@ -8249,9 +8157,7 @@
       <c r="S69" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T69" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T69" s="43"/>
       <c r="U69" s="44"/>
       <c r="V69" s="45"/>
       <c r="W69" s="43" t="s">
@@ -8308,9 +8214,7 @@
       <c r="S70" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T70" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T70" s="43"/>
       <c r="U70" s="44"/>
       <c r="V70" s="45"/>
       <c r="W70" s="43" t="s">
@@ -8367,9 +8271,7 @@
       <c r="S71" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T71" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T71" s="43"/>
       <c r="U71" s="44"/>
       <c r="V71" s="45"/>
       <c r="W71" s="43" t="s">
@@ -8426,9 +8328,7 @@
       <c r="S72" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T72" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T72" s="43"/>
       <c r="U72" s="44"/>
       <c r="V72" s="45"/>
       <c r="W72" s="43" t="s">
@@ -8485,9 +8385,7 @@
       <c r="S73" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T73" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T73" s="43"/>
       <c r="U73" s="44"/>
       <c r="V73" s="45"/>
       <c r="W73" s="43" t="s">
@@ -8544,9 +8442,7 @@
       <c r="S74" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T74" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T74" s="43"/>
       <c r="U74" s="44"/>
       <c r="V74" s="45"/>
       <c r="W74" s="43" t="s">
@@ -8603,9 +8499,7 @@
       <c r="S75" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T75" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T75" s="43"/>
       <c r="U75" s="44"/>
       <c r="V75" s="45"/>
       <c r="W75" s="43" t="s">
@@ -8662,9 +8556,7 @@
       <c r="S76" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T76" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T76" s="43"/>
       <c r="U76" s="44"/>
       <c r="V76" s="45"/>
       <c r="W76" s="43" t="s">
@@ -10688,9 +10580,7 @@
       <c r="S130" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T130" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T130" s="43"/>
       <c r="U130" s="44"/>
       <c r="V130" s="45"/>
       <c r="W130" s="43" t="s">
@@ -10747,9 +10637,7 @@
       <c r="S131" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T131" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T131" s="43"/>
       <c r="U131" s="44"/>
       <c r="V131" s="45"/>
       <c r="W131" s="43" t="s">
@@ -10806,9 +10694,7 @@
       <c r="S132" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T132" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T132" s="43"/>
       <c r="U132" s="44"/>
       <c r="V132" s="45"/>
       <c r="W132" s="43" t="s">
@@ -10865,9 +10751,7 @@
       <c r="S133" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T133" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T133" s="43"/>
       <c r="U133" s="44"/>
       <c r="V133" s="45"/>
       <c r="W133" s="43" t="s">
@@ -10924,9 +10808,7 @@
       <c r="S134" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T134" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T134" s="43"/>
       <c r="U134" s="44"/>
       <c r="V134" s="45"/>
       <c r="W134" s="43" t="s">
@@ -10983,9 +10865,7 @@
       <c r="S135" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T135" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T135" s="43"/>
       <c r="U135" s="44"/>
       <c r="V135" s="45"/>
       <c r="W135" s="43" t="s">
@@ -11042,9 +10922,7 @@
       <c r="S136" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T136" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T136" s="43"/>
       <c r="U136" s="44"/>
       <c r="V136" s="45"/>
       <c r="W136" s="43" t="s">
@@ -11101,9 +10979,7 @@
       <c r="S137" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T137" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T137" s="43"/>
       <c r="U137" s="44"/>
       <c r="V137" s="45"/>
       <c r="W137" s="43" t="s">
@@ -11160,9 +11036,7 @@
       <c r="S138" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T138" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T138" s="43"/>
       <c r="U138" s="44"/>
       <c r="V138" s="45"/>
       <c r="W138" s="43" t="s">
@@ -11219,9 +11093,7 @@
       <c r="S139" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T139" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T139" s="43"/>
       <c r="U139" s="44"/>
       <c r="V139" s="45"/>
       <c r="W139" s="43" t="s">
@@ -11278,9 +11150,7 @@
       <c r="S140" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T140" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T140" s="43"/>
       <c r="U140" s="44"/>
       <c r="V140" s="45"/>
       <c r="W140" s="43" t="s">
@@ -11337,9 +11207,7 @@
       <c r="S141" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T141" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T141" s="43"/>
       <c r="U141" s="44"/>
       <c r="V141" s="45"/>
       <c r="W141" s="43" t="s">
@@ -11396,9 +11264,7 @@
       <c r="S142" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T142" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T142" s="43"/>
       <c r="U142" s="44"/>
       <c r="V142" s="45"/>
       <c r="W142" s="43" t="s">
@@ -11455,9 +11321,7 @@
       <c r="S143" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T143" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T143" s="43"/>
       <c r="U143" s="44"/>
       <c r="V143" s="45"/>
       <c r="W143" s="43" t="s">
@@ -11514,9 +11378,7 @@
       <c r="S144" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T144" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T144" s="43"/>
       <c r="U144" s="44"/>
       <c r="V144" s="45"/>
       <c r="W144" s="43" t="s">
@@ -11573,9 +11435,7 @@
       <c r="S145" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T145" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T145" s="43"/>
       <c r="U145" s="44"/>
       <c r="V145" s="45"/>
       <c r="W145" s="43" t="s">
@@ -11632,9 +11492,7 @@
       <c r="S146" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T146" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T146" s="43"/>
       <c r="U146" s="44"/>
       <c r="V146" s="45"/>
       <c r="W146" s="43" t="s">
@@ -11691,9 +11549,7 @@
       <c r="S147" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T147" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T147" s="43"/>
       <c r="U147" s="44"/>
       <c r="V147" s="45"/>
       <c r="W147" s="43" t="s">
@@ -13810,9 +13666,7 @@
       <c r="S200" s="43" t="s">
         <v>456</v>
       </c>
-      <c r="T200" s="43" t="s">
-        <v>266</v>
-      </c>
+      <c r="T200" s="43"/>
       <c r="U200" s="44"/>
       <c r="V200" s="45"/>
       <c r="W200" s="43" t="s">
@@ -20411,25 +20265,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F560B38A5B3C4B41B1895754B1F1A56A" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="69dc0f489d46816a4b9bb4a327e14425">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca719f03-9e45-4ef4-9920-d156f53157f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7de9a44ff87fdcabda187bbd662e75de" ns2:_="">
     <xsd:import namespace="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
@@ -20601,7 +20436,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -20619,32 +20499,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
fix xls di compilazione
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04035190-2327-486D-93C8-F7DE54374D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5C6F5B-92E0-4965-BDB8-17C6C1EFB9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="718">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3506,7 +3506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -4655,10 +4655,10 @@
   <dimension ref="A1:W770"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="T200" sqref="T200"/>
+      <selection pane="bottomRight" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4977,14 +4977,20 @@
       <c r="M10" s="43" t="s">
         <v>267</v>
       </c>
-      <c r="N10" s="43"/>
+      <c r="N10" s="43" t="s">
+        <v>267</v>
+      </c>
       <c r="O10" s="43"/>
       <c r="P10" s="43" t="s">
         <v>66</v>
       </c>
       <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="43"/>
+      <c r="R10" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="S10" s="43" t="s">
+        <v>456</v>
+      </c>
       <c r="T10" s="43" t="s">
         <v>265</v>
       </c>
@@ -5022,13 +5028,19 @@
         <v>465</v>
       </c>
       <c r="I11" s="42"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
+      <c r="J11" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="K11" s="43" t="s">
+        <v>273</v>
+      </c>
       <c r="L11" s="43"/>
       <c r="M11" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="N11" s="43"/>
+      <c r="N11" s="43" t="s">
+        <v>267</v>
+      </c>
       <c r="O11" s="43" t="s">
         <v>466</v>
       </c>
@@ -5075,8 +5087,12 @@
         <v>522</v>
       </c>
       <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
+      <c r="J12" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="K12" s="43" t="s">
+        <v>273</v>
+      </c>
       <c r="L12" s="43"/>
       <c r="M12" s="43" t="s">
         <v>66</v>
@@ -5169,8 +5185,12 @@
         <v>571</v>
       </c>
       <c r="I14" s="42"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
+      <c r="J14" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="K14" s="43" t="s">
+        <v>273</v>
+      </c>
       <c r="L14" s="43"/>
       <c r="M14" s="43" t="s">
         <v>66</v>
@@ -5226,8 +5246,12 @@
         <v>644</v>
       </c>
       <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
+      <c r="J15" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="K15" s="43" t="s">
+        <v>273</v>
+      </c>
       <c r="L15" s="43"/>
       <c r="M15" s="43" t="s">
         <v>66</v>
@@ -5394,13 +5418,19 @@
         <v>464</v>
       </c>
       <c r="I19" s="42"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
+      <c r="J19" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="K19" s="43" t="s">
+        <v>273</v>
+      </c>
       <c r="L19" s="43"/>
       <c r="M19" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="N19" s="43"/>
+      <c r="N19" s="43" t="s">
+        <v>267</v>
+      </c>
       <c r="O19" s="43" t="s">
         <v>461</v>
       </c>
@@ -5447,8 +5477,12 @@
         <v>525</v>
       </c>
       <c r="I20" s="42"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
+      <c r="J20" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="K20" s="43" t="s">
+        <v>273</v>
+      </c>
       <c r="L20" s="43"/>
       <c r="M20" s="43" t="s">
         <v>66</v>
@@ -5540,8 +5574,12 @@
         <v>573</v>
       </c>
       <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
+      <c r="J22" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="K22" s="43" t="s">
+        <v>273</v>
+      </c>
       <c r="L22" s="43"/>
       <c r="M22" s="43" t="s">
         <v>66</v>
@@ -5597,8 +5635,12 @@
         <v>646</v>
       </c>
       <c r="I23" s="42"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
+      <c r="J23" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="K23" s="43" t="s">
+        <v>273</v>
+      </c>
       <c r="L23" s="43"/>
       <c r="M23" s="43" t="s">
         <v>66</v>
@@ -5763,13 +5805,17 @@
       </c>
       <c r="H27" s="41"/>
       <c r="I27" s="42"/>
-      <c r="J27" s="43"/>
+      <c r="J27" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K27" s="43"/>
       <c r="L27" s="43"/>
       <c r="M27" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="N27" s="43"/>
+      <c r="N27" s="43" t="s">
+        <v>267</v>
+      </c>
       <c r="O27" s="43" t="s">
         <v>458</v>
       </c>
@@ -5818,7 +5864,9 @@
       </c>
       <c r="H28" s="41"/>
       <c r="I28" s="42"/>
-      <c r="J28" s="43"/>
+      <c r="J28" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
       <c r="M28" s="43" t="s">
@@ -5914,7 +5962,9 @@
       </c>
       <c r="H30" s="41"/>
       <c r="I30" s="42"/>
-      <c r="J30" s="43"/>
+      <c r="J30" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K30" s="43"/>
       <c r="L30" s="43"/>
       <c r="M30" s="43" t="s">
@@ -5971,7 +6021,9 @@
       </c>
       <c r="H31" s="41"/>
       <c r="I31" s="42"/>
-      <c r="J31" s="43"/>
+      <c r="J31" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K31" s="43"/>
       <c r="L31" s="43"/>
       <c r="M31" s="43" t="s">
@@ -6147,7 +6199,9 @@
         <v>454</v>
       </c>
       <c r="I35" s="42"/>
-      <c r="J35" s="43"/>
+      <c r="J35" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K35" s="43"/>
       <c r="L35" s="43"/>
       <c r="M35" s="43" t="s">
@@ -6206,7 +6260,9 @@
         <v>470</v>
       </c>
       <c r="I36" s="42"/>
-      <c r="J36" s="43"/>
+      <c r="J36" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K36" s="43"/>
       <c r="L36" s="43"/>
       <c r="M36" s="43" t="s">
@@ -6263,7 +6319,9 @@
         <v>474</v>
       </c>
       <c r="I37" s="42"/>
-      <c r="J37" s="43"/>
+      <c r="J37" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K37" s="43"/>
       <c r="L37" s="43"/>
       <c r="M37" s="43" t="s">
@@ -6322,7 +6380,9 @@
         <v>479</v>
       </c>
       <c r="I38" s="42"/>
-      <c r="J38" s="43"/>
+      <c r="J38" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K38" s="43"/>
       <c r="L38" s="43"/>
       <c r="M38" s="43" t="s">
@@ -6379,7 +6439,9 @@
         <v>481</v>
       </c>
       <c r="I39" s="42"/>
-      <c r="J39" s="43"/>
+      <c r="J39" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K39" s="43"/>
       <c r="L39" s="43"/>
       <c r="M39" s="43" t="s">
@@ -6436,7 +6498,9 @@
         <v>484</v>
       </c>
       <c r="I40" s="42"/>
-      <c r="J40" s="43"/>
+      <c r="J40" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K40" s="43"/>
       <c r="L40" s="43"/>
       <c r="M40" s="43" t="s">
@@ -6493,7 +6557,9 @@
         <v>487</v>
       </c>
       <c r="I41" s="42"/>
-      <c r="J41" s="43"/>
+      <c r="J41" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K41" s="43"/>
       <c r="L41" s="43"/>
       <c r="M41" s="43" t="s">
@@ -6550,7 +6616,9 @@
         <v>490</v>
       </c>
       <c r="I42" s="42"/>
-      <c r="J42" s="43"/>
+      <c r="J42" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K42" s="43"/>
       <c r="L42" s="43"/>
       <c r="M42" s="43" t="s">
@@ -6607,7 +6675,9 @@
         <v>515</v>
       </c>
       <c r="I43" s="42"/>
-      <c r="J43" s="43"/>
+      <c r="J43" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K43" s="43"/>
       <c r="L43" s="43"/>
       <c r="M43" s="43" t="s">
@@ -6664,7 +6734,9 @@
         <v>518</v>
       </c>
       <c r="I44" s="42"/>
-      <c r="J44" s="43"/>
+      <c r="J44" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K44" s="43"/>
       <c r="L44" s="43"/>
       <c r="M44" s="43" t="s">
@@ -6723,7 +6795,9 @@
         <v>520</v>
       </c>
       <c r="I45" s="42"/>
-      <c r="J45" s="43"/>
+      <c r="J45" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K45" s="43"/>
       <c r="L45" s="43"/>
       <c r="M45" s="43" t="s">
@@ -6782,7 +6856,9 @@
         <v>531</v>
       </c>
       <c r="I46" s="42"/>
-      <c r="J46" s="43"/>
+      <c r="J46" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K46" s="43"/>
       <c r="L46" s="43"/>
       <c r="M46" s="43" t="s">
@@ -6841,7 +6917,9 @@
         <v>542</v>
       </c>
       <c r="I47" s="42"/>
-      <c r="J47" s="43"/>
+      <c r="J47" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K47" s="43"/>
       <c r="L47" s="43"/>
       <c r="M47" s="43" t="s">
@@ -6902,7 +6980,9 @@
         <v>545</v>
       </c>
       <c r="I48" s="42"/>
-      <c r="J48" s="43"/>
+      <c r="J48" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K48" s="43"/>
       <c r="L48" s="43"/>
       <c r="M48" s="43" t="s">
@@ -6961,7 +7041,9 @@
         <v>548</v>
       </c>
       <c r="I49" s="42"/>
-      <c r="J49" s="43"/>
+      <c r="J49" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K49" s="43"/>
       <c r="L49" s="43"/>
       <c r="M49" s="43" t="s">
@@ -7020,7 +7102,9 @@
         <v>551</v>
       </c>
       <c r="I50" s="42"/>
-      <c r="J50" s="43"/>
+      <c r="J50" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K50" s="43"/>
       <c r="L50" s="43"/>
       <c r="M50" s="43" t="s">
@@ -7079,7 +7163,9 @@
         <v>553</v>
       </c>
       <c r="I51" s="42"/>
-      <c r="J51" s="43"/>
+      <c r="J51" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K51" s="43"/>
       <c r="L51" s="43"/>
       <c r="M51" s="43" t="s">
@@ -7138,7 +7224,9 @@
         <v>556</v>
       </c>
       <c r="I52" s="42"/>
-      <c r="J52" s="43"/>
+      <c r="J52" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K52" s="43"/>
       <c r="L52" s="43"/>
       <c r="M52" s="43" t="s">
@@ -7197,7 +7285,9 @@
         <v>560</v>
       </c>
       <c r="I53" s="42"/>
-      <c r="J53" s="43"/>
+      <c r="J53" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K53" s="43"/>
       <c r="L53" s="43"/>
       <c r="M53" s="43" t="s">
@@ -7256,7 +7346,9 @@
         <v>588</v>
       </c>
       <c r="I54" s="42"/>
-      <c r="J54" s="43"/>
+      <c r="J54" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K54" s="43"/>
       <c r="L54" s="43"/>
       <c r="M54" s="43" t="s">
@@ -7315,7 +7407,9 @@
         <v>591</v>
       </c>
       <c r="I55" s="42"/>
-      <c r="J55" s="43"/>
+      <c r="J55" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K55" s="43"/>
       <c r="L55" s="43"/>
       <c r="M55" s="43" t="s">
@@ -7374,7 +7468,9 @@
         <v>594</v>
       </c>
       <c r="I56" s="42"/>
-      <c r="J56" s="43"/>
+      <c r="J56" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K56" s="43"/>
       <c r="L56" s="43"/>
       <c r="M56" s="43" t="s">
@@ -7433,7 +7529,9 @@
         <v>585</v>
       </c>
       <c r="I57" s="42"/>
-      <c r="J57" s="43"/>
+      <c r="J57" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K57" s="43"/>
       <c r="L57" s="43"/>
       <c r="M57" s="43" t="s">
@@ -7492,7 +7590,9 @@
         <v>576</v>
       </c>
       <c r="I58" s="42"/>
-      <c r="J58" s="43"/>
+      <c r="J58" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K58" s="43"/>
       <c r="L58" s="43"/>
       <c r="M58" s="43" t="s">
@@ -7551,7 +7651,9 @@
         <v>578</v>
       </c>
       <c r="I59" s="42"/>
-      <c r="J59" s="43"/>
+      <c r="J59" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K59" s="43"/>
       <c r="L59" s="43"/>
       <c r="M59" s="43" t="s">
@@ -7610,7 +7712,9 @@
         <v>581</v>
       </c>
       <c r="I60" s="42"/>
-      <c r="J60" s="43"/>
+      <c r="J60" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K60" s="43"/>
       <c r="L60" s="43"/>
       <c r="M60" s="43" t="s">
@@ -7669,7 +7773,9 @@
         <v>597</v>
       </c>
       <c r="I61" s="42"/>
-      <c r="J61" s="43"/>
+      <c r="J61" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K61" s="43"/>
       <c r="L61" s="43"/>
       <c r="M61" s="43" t="s">
@@ -7728,7 +7834,9 @@
         <v>600</v>
       </c>
       <c r="I62" s="42"/>
-      <c r="J62" s="43"/>
+      <c r="J62" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K62" s="43"/>
       <c r="L62" s="43"/>
       <c r="M62" s="43" t="s">
@@ -7787,7 +7895,9 @@
         <v>602</v>
       </c>
       <c r="I63" s="42"/>
-      <c r="J63" s="43"/>
+      <c r="J63" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K63" s="43"/>
       <c r="L63" s="43"/>
       <c r="M63" s="43" t="s">
@@ -7846,7 +7956,9 @@
         <v>617</v>
       </c>
       <c r="I64" s="42"/>
-      <c r="J64" s="43"/>
+      <c r="J64" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K64" s="43"/>
       <c r="L64" s="43"/>
       <c r="M64" s="43" t="s">
@@ -7905,7 +8017,9 @@
         <v>604</v>
       </c>
       <c r="I65" s="42"/>
-      <c r="J65" s="43"/>
+      <c r="J65" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K65" s="43"/>
       <c r="L65" s="43"/>
       <c r="M65" s="43" t="s">
@@ -7962,7 +8076,9 @@
         <v>614</v>
       </c>
       <c r="I66" s="42"/>
-      <c r="J66" s="43"/>
+      <c r="J66" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K66" s="43"/>
       <c r="L66" s="43"/>
       <c r="M66" s="43" t="s">
@@ -8019,7 +8135,9 @@
         <v>621</v>
       </c>
       <c r="I67" s="42"/>
-      <c r="J67" s="43"/>
+      <c r="J67" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K67" s="43"/>
       <c r="L67" s="43"/>
       <c r="M67" s="43" t="s">
@@ -8076,7 +8194,9 @@
         <v>665</v>
       </c>
       <c r="I68" s="42"/>
-      <c r="J68" s="43"/>
+      <c r="J68" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K68" s="43"/>
       <c r="L68" s="43"/>
       <c r="M68" s="43" t="s">
@@ -8133,7 +8253,9 @@
         <v>623</v>
       </c>
       <c r="I69" s="42"/>
-      <c r="J69" s="43"/>
+      <c r="J69" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K69" s="43"/>
       <c r="L69" s="43"/>
       <c r="M69" s="43" t="s">
@@ -8190,7 +8312,9 @@
         <v>626</v>
       </c>
       <c r="I70" s="42"/>
-      <c r="J70" s="43"/>
+      <c r="J70" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K70" s="43"/>
       <c r="L70" s="43"/>
       <c r="M70" s="43" t="s">
@@ -8247,7 +8371,9 @@
         <v>662</v>
       </c>
       <c r="I71" s="42"/>
-      <c r="J71" s="43"/>
+      <c r="J71" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K71" s="43"/>
       <c r="L71" s="43"/>
       <c r="M71" s="43" t="s">
@@ -8304,7 +8430,9 @@
         <v>629</v>
       </c>
       <c r="I72" s="42"/>
-      <c r="J72" s="43"/>
+      <c r="J72" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K72" s="43"/>
       <c r="L72" s="43"/>
       <c r="M72" s="43" t="s">
@@ -8361,7 +8489,9 @@
         <v>632</v>
       </c>
       <c r="I73" s="42"/>
-      <c r="J73" s="43"/>
+      <c r="J73" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K73" s="43"/>
       <c r="L73" s="43"/>
       <c r="M73" s="43" t="s">
@@ -8418,7 +8548,9 @@
         <v>639</v>
       </c>
       <c r="I74" s="42"/>
-      <c r="J74" s="43"/>
+      <c r="J74" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K74" s="43"/>
       <c r="L74" s="43"/>
       <c r="M74" s="43" t="s">
@@ -8475,7 +8607,9 @@
         <v>642</v>
       </c>
       <c r="I75" s="42"/>
-      <c r="J75" s="43"/>
+      <c r="J75" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K75" s="43"/>
       <c r="L75" s="43"/>
       <c r="M75" s="43" t="s">
@@ -8532,7 +8666,9 @@
         <v>668</v>
       </c>
       <c r="I76" s="42"/>
-      <c r="J76" s="43"/>
+      <c r="J76" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K76" s="43"/>
       <c r="L76" s="43"/>
       <c r="M76" s="43" t="s">
@@ -10556,7 +10692,9 @@
         <v>650</v>
       </c>
       <c r="I130" s="42"/>
-      <c r="J130" s="43"/>
+      <c r="J130" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K130" s="43"/>
       <c r="L130" s="43"/>
       <c r="M130" s="43" t="s">
@@ -10613,7 +10751,9 @@
         <v>652</v>
       </c>
       <c r="I131" s="42"/>
-      <c r="J131" s="43"/>
+      <c r="J131" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K131" s="43"/>
       <c r="L131" s="43"/>
       <c r="M131" s="43" t="s">
@@ -10670,7 +10810,9 @@
         <v>655</v>
       </c>
       <c r="I132" s="42"/>
-      <c r="J132" s="43"/>
+      <c r="J132" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K132" s="43"/>
       <c r="L132" s="43"/>
       <c r="M132" s="43" t="s">
@@ -10727,7 +10869,9 @@
         <v>658</v>
       </c>
       <c r="I133" s="42"/>
-      <c r="J133" s="43"/>
+      <c r="J133" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K133" s="43"/>
       <c r="L133" s="43"/>
       <c r="M133" s="43" t="s">
@@ -10784,7 +10928,9 @@
         <v>660</v>
       </c>
       <c r="I134" s="42"/>
-      <c r="J134" s="43"/>
+      <c r="J134" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K134" s="43"/>
       <c r="L134" s="43"/>
       <c r="M134" s="43" t="s">
@@ -10841,7 +10987,9 @@
         <v>678</v>
       </c>
       <c r="I135" s="42"/>
-      <c r="J135" s="43"/>
+      <c r="J135" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K135" s="43"/>
       <c r="L135" s="43"/>
       <c r="M135" s="43" t="s">
@@ -10898,7 +11046,9 @@
         <v>681</v>
       </c>
       <c r="I136" s="42"/>
-      <c r="J136" s="43"/>
+      <c r="J136" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K136" s="43"/>
       <c r="L136" s="43"/>
       <c r="M136" s="43" t="s">
@@ -10955,7 +11105,9 @@
         <v>683</v>
       </c>
       <c r="I137" s="42"/>
-      <c r="J137" s="43"/>
+      <c r="J137" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K137" s="43"/>
       <c r="L137" s="43"/>
       <c r="M137" s="43" t="s">
@@ -11012,7 +11164,9 @@
         <v>686</v>
       </c>
       <c r="I138" s="42"/>
-      <c r="J138" s="43"/>
+      <c r="J138" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K138" s="43"/>
       <c r="L138" s="43"/>
       <c r="M138" s="43" t="s">
@@ -11069,7 +11223,9 @@
         <v>690</v>
       </c>
       <c r="I139" s="42"/>
-      <c r="J139" s="43"/>
+      <c r="J139" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K139" s="43"/>
       <c r="L139" s="43"/>
       <c r="M139" s="43" t="s">
@@ -11126,7 +11282,9 @@
         <v>693</v>
       </c>
       <c r="I140" s="42"/>
-      <c r="J140" s="43"/>
+      <c r="J140" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K140" s="43"/>
       <c r="L140" s="43"/>
       <c r="M140" s="43" t="s">
@@ -11183,7 +11341,9 @@
         <v>695</v>
       </c>
       <c r="I141" s="42"/>
-      <c r="J141" s="43"/>
+      <c r="J141" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K141" s="43"/>
       <c r="L141" s="43"/>
       <c r="M141" s="43" t="s">
@@ -11240,7 +11400,9 @@
         <v>697</v>
       </c>
       <c r="I142" s="42"/>
-      <c r="J142" s="43"/>
+      <c r="J142" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K142" s="43"/>
       <c r="L142" s="43"/>
       <c r="M142" s="43" t="s">
@@ -11297,7 +11459,9 @@
         <v>700</v>
       </c>
       <c r="I143" s="42"/>
-      <c r="J143" s="43"/>
+      <c r="J143" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K143" s="43"/>
       <c r="L143" s="43"/>
       <c r="M143" s="43" t="s">
@@ -11354,7 +11518,9 @@
         <v>703</v>
       </c>
       <c r="I144" s="42"/>
-      <c r="J144" s="43"/>
+      <c r="J144" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K144" s="43"/>
       <c r="L144" s="43"/>
       <c r="M144" s="43" t="s">
@@ -11411,7 +11577,9 @@
         <v>706</v>
       </c>
       <c r="I145" s="42"/>
-      <c r="J145" s="43"/>
+      <c r="J145" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K145" s="43"/>
       <c r="L145" s="43"/>
       <c r="M145" s="43" t="s">
@@ -11468,7 +11636,9 @@
         <v>709</v>
       </c>
       <c r="I146" s="42"/>
-      <c r="J146" s="43"/>
+      <c r="J146" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K146" s="43"/>
       <c r="L146" s="43"/>
       <c r="M146" s="43" t="s">
@@ -11525,7 +11695,9 @@
         <v>712</v>
       </c>
       <c r="I147" s="42"/>
-      <c r="J147" s="43"/>
+      <c r="J147" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K147" s="43"/>
       <c r="L147" s="43"/>
       <c r="M147" s="43" t="s">
@@ -13135,13 +13307,23 @@
       </c>
       <c r="K188" s="43"/>
       <c r="L188" s="43"/>
-      <c r="M188" s="43"/>
-      <c r="N188" s="43"/>
+      <c r="M188" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="N188" s="43" t="s">
+        <v>267</v>
+      </c>
       <c r="O188" s="43"/>
-      <c r="P188" s="43"/>
+      <c r="P188" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="Q188" s="43"/>
-      <c r="R188" s="43"/>
-      <c r="S188" s="43"/>
+      <c r="R188" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="S188" s="43" t="s">
+        <v>456</v>
+      </c>
       <c r="T188" s="43" t="s">
         <v>265</v>
       </c>
@@ -13184,13 +13366,23 @@
       </c>
       <c r="K189" s="43"/>
       <c r="L189" s="43"/>
-      <c r="M189" s="43"/>
-      <c r="N189" s="43"/>
+      <c r="M189" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="N189" s="43" t="s">
+        <v>267</v>
+      </c>
       <c r="O189" s="43"/>
-      <c r="P189" s="43"/>
+      <c r="P189" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="Q189" s="43"/>
-      <c r="R189" s="43"/>
-      <c r="S189" s="43"/>
+      <c r="R189" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="S189" s="43" t="s">
+        <v>456</v>
+      </c>
       <c r="T189" s="43" t="s">
         <v>265</v>
       </c>
@@ -13233,13 +13425,23 @@
       </c>
       <c r="K190" s="43"/>
       <c r="L190" s="43"/>
-      <c r="M190" s="43"/>
-      <c r="N190" s="43"/>
+      <c r="M190" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="N190" s="43" t="s">
+        <v>267</v>
+      </c>
       <c r="O190" s="43"/>
-      <c r="P190" s="43"/>
+      <c r="P190" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="Q190" s="43"/>
-      <c r="R190" s="43"/>
-      <c r="S190" s="43"/>
+      <c r="R190" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="S190" s="43" t="s">
+        <v>456</v>
+      </c>
       <c r="T190" s="43" t="s">
         <v>265</v>
       </c>
@@ -13284,13 +13486,23 @@
       </c>
       <c r="K191" s="43"/>
       <c r="L191" s="43"/>
-      <c r="M191" s="43"/>
-      <c r="N191" s="43"/>
+      <c r="M191" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="N191" s="43" t="s">
+        <v>267</v>
+      </c>
       <c r="O191" s="43"/>
-      <c r="P191" s="43"/>
+      <c r="P191" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="Q191" s="43"/>
-      <c r="R191" s="43"/>
-      <c r="S191" s="43"/>
+      <c r="R191" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="S191" s="43" t="s">
+        <v>456</v>
+      </c>
       <c r="T191" s="43" t="s">
         <v>265</v>
       </c>
@@ -13333,8 +13545,12 @@
       </c>
       <c r="K192" s="43"/>
       <c r="L192" s="43"/>
-      <c r="M192" s="43"/>
-      <c r="N192" s="43"/>
+      <c r="M192" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="N192" s="43" t="s">
+        <v>267</v>
+      </c>
       <c r="O192" s="43"/>
       <c r="P192" s="43" t="s">
         <v>66</v>
@@ -13642,7 +13858,9 @@
         <v>715</v>
       </c>
       <c r="I200" s="42"/>
-      <c r="J200" s="43"/>
+      <c r="J200" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="K200" s="43"/>
       <c r="L200" s="43"/>
       <c r="M200" s="43" t="s">
@@ -18006,7 +18224,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J14 M14:N15 J16:J20 P10:R12 J22 J24:J28 M22:N28 M20:N20 P30:R198 M10:N12 J10:J12 M30:N198 J30:J198 M16:M20 N16:N19 P22:R28 P200:R200 M200:N200 P14:R20</xm:sqref>
+          <xm:sqref>J14 M14:N15 J16:J20 P10:R12 J22 J24:J28 M22:N28 M20:N20 M10:N12 J10:J12 P14:R20 J30:J198 M16:M20 N16:N19 P22:R28 P200:R200 M200:N200 M30:N198 P30:R198</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
@@ -20265,6 +20483,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F560B38A5B3C4B41B1895754B1F1A56A" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="69dc0f489d46816a4b9bb4a327e14425">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca719f03-9e45-4ef4-9920-d156f53157f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7de9a44ff87fdcabda187bbd662e75de" ns2:_="">
     <xsd:import namespace="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
@@ -20436,26 +20673,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20473,32 +20717,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
fix test ove non c'è applicabilità
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5C6F5B-92E0-4965-BDB8-17C6C1EFB9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA22CCB9-3B53-4DB9-BCDE-4C5A9A972FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="701">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1796,24 +1796,12 @@
     <t>{"Error calling Validate: {\"traceID\":\"ff8586b7e90570d2\",\"spanID\":\"ff8586b7e90570d2\",\"type\":\"/msg/jwt-validation\",\"title\":\"Campo token JWT non valido.\",\"detail\":\"Il campo action_id non è corretto\",\"status\":403,\"instance\":\"/jwt-mandatory-field-malformed\",\"workflowInstanceId\":\"UNKNOWN_WORKFLOW_ID\"}"}</t>
   </si>
   <si>
-    <t>2025-02-26T09:26:31</t>
-  </si>
-  <si>
     <t>Il campo action_id non è corretto - Campo token JWT non valido.</t>
   </si>
   <si>
-    <t>ff8586b7e90570d2</t>
-  </si>
-  <si>
-    <t>d21b619dc217cf9f</t>
-  </si>
-  <si>
     <t>Campo token JWT non valido. - Il campo person_id non è valorizzato</t>
   </si>
   <si>
-    <t>2025-02-26T09:34:37</t>
-  </si>
-  <si>
     <t>2025-02-25T19:56:51</t>
   </si>
   <si>
@@ -1976,21 +1964,9 @@
     <t>2025-02-26T18:23:05</t>
   </si>
   <si>
-    <t>a13128e1aa3b2cec</t>
-  </si>
-  <si>
-    <t>2025-02-27T09:53:29</t>
-  </si>
-  <si>
     <t>2025-02-27'</t>
   </si>
   <si>
-    <t>bfb49bcc16dd2996</t>
-  </si>
-  <si>
-    <t>2025-02-27T09:57:28</t>
-  </si>
-  <si>
     <t>Campo token JWT non valido. - Il campo action_id non è corretto</t>
   </si>
   <si>
@@ -2123,18 +2099,6 @@
     <t>Il campo purpose_of_use non è corretto - Campo token JWT non valido.</t>
   </si>
   <si>
-    <t>6c712e25d43c5900</t>
-  </si>
-  <si>
-    <t>2025-03-03T11:11:03</t>
-  </si>
-  <si>
-    <t>45eff58ad0c7892d</t>
-  </si>
-  <si>
-    <t>2025-03-03T11:20:16</t>
-  </si>
-  <si>
     <t>2025-03-03T11:31:09</t>
   </si>
   <si>
@@ -2157,9 +2121,6 @@
   </si>
   <si>
     <t>2025-03-03T13:45:23</t>
-  </si>
-  <si>
-    <t>deve essere maggione o uguale di quello di effectiveTime/low : '20250227100000+0100'.]</t>
   </si>
   <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.112 v2.1.0, Codes: ZXZZXX]</t>
@@ -2342,18 +2303,6 @@
   </si>
   <si>
     <t>2025-03-05T10:37:04</t>
-  </si>
-  <si>
-    <t>524ef061057ed37f</t>
-  </si>
-  <si>
-    <t>2025-03-05T11:21:09</t>
-  </si>
-  <si>
-    <t>4a5a704223f60d5a</t>
-  </si>
-  <si>
-    <t>2025-03-05T11:28:50</t>
   </si>
   <si>
     <t>2025-03-05T11:37:30</t>
@@ -4652,13 +4601,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W770"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N19" sqref="N19"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4941,7 +4891,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="48">
         <v>4</v>
       </c>
@@ -4958,16 +4908,16 @@
         <v>424</v>
       </c>
       <c r="F10" s="50" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="G10" s="50" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="H10" s="50" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="I10" s="41" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="J10" s="43" t="s">
         <v>66</v>
@@ -4996,7 +4946,7 @@
       </c>
       <c r="U10" s="44"/>
       <c r="V10" s="50" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="W10" s="43" t="s">
         <v>36</v>
@@ -5018,15 +4968,9 @@
       <c r="E11" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="50">
-        <v>45714</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>467</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>465</v>
-      </c>
+      <c r="F11" s="50"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
       <c r="I11" s="42"/>
       <c r="J11" s="43" t="s">
         <v>267</v>
@@ -5042,7 +4986,7 @@
         <v>267</v>
       </c>
       <c r="O11" s="43" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="P11" s="43" t="s">
         <v>66</v>
@@ -5050,8 +4994,12 @@
       <c r="Q11" s="43" t="s">
         <v>459</v>
       </c>
-      <c r="R11" s="43"/>
-      <c r="S11" s="43"/>
+      <c r="R11" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="S11" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="T11" s="43"/>
       <c r="U11" s="44"/>
       <c r="V11" s="45" t="s">
@@ -5077,15 +5025,9 @@
       <c r="E12" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="51" t="s">
-        <v>524</v>
-      </c>
-      <c r="G12" s="41" t="s">
-        <v>523</v>
-      </c>
-      <c r="H12" s="41" t="s">
-        <v>522</v>
-      </c>
+      <c r="F12" s="51"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
       <c r="I12" s="42"/>
       <c r="J12" s="43" t="s">
         <v>267</v>
@@ -5101,7 +5043,7 @@
         <v>267</v>
       </c>
       <c r="O12" s="43" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="P12" s="43" t="s">
         <v>66</v>
@@ -5113,7 +5055,7 @@
         <v>66</v>
       </c>
       <c r="S12" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T12" s="43"/>
       <c r="U12" s="44"/>
@@ -5175,15 +5117,9 @@
       <c r="E14" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="51" t="s">
-        <v>559</v>
-      </c>
-      <c r="G14" s="41" t="s">
-        <v>572</v>
-      </c>
-      <c r="H14" s="41" t="s">
-        <v>571</v>
-      </c>
+      <c r="F14" s="51"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
       <c r="I14" s="42"/>
       <c r="J14" s="43" t="s">
         <v>267</v>
@@ -5199,7 +5135,7 @@
         <v>267</v>
       </c>
       <c r="O14" s="43" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="P14" s="43" t="s">
         <v>66</v>
@@ -5211,7 +5147,7 @@
         <v>66</v>
       </c>
       <c r="S14" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T14" s="43"/>
       <c r="U14" s="44"/>
@@ -5236,15 +5172,9 @@
       <c r="E15" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="41" t="s">
-        <v>633</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>645</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>644</v>
-      </c>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="42"/>
       <c r="J15" s="43" t="s">
         <v>267</v>
@@ -5260,7 +5190,7 @@
         <v>267</v>
       </c>
       <c r="O15" s="43" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="P15" s="43" t="s">
         <v>66</v>
@@ -5272,7 +5202,7 @@
         <v>66</v>
       </c>
       <c r="S15" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T15" s="43"/>
       <c r="U15" s="44"/>
@@ -5408,15 +5338,9 @@
       <c r="E19" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="41">
-        <v>45714</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>462</v>
-      </c>
-      <c r="H19" s="41" t="s">
-        <v>464</v>
-      </c>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
       <c r="I19" s="42"/>
       <c r="J19" s="43" t="s">
         <v>267</v>
@@ -5440,12 +5364,16 @@
       <c r="Q19" s="43" t="s">
         <v>459</v>
       </c>
-      <c r="R19" s="43"/>
-      <c r="S19" s="43"/>
+      <c r="R19" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="S19" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="T19" s="43"/>
       <c r="U19" s="44"/>
       <c r="V19" s="45" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="W19" s="43" t="s">
         <v>46</v>
@@ -5467,15 +5395,9 @@
       <c r="E20" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="51" t="s">
-        <v>524</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>526</v>
-      </c>
-      <c r="H20" s="41" t="s">
-        <v>525</v>
-      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="42"/>
       <c r="J20" s="43" t="s">
         <v>267</v>
@@ -5491,7 +5413,7 @@
         <v>267</v>
       </c>
       <c r="O20" s="43" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="P20" s="43" t="s">
         <v>66</v>
@@ -5503,7 +5425,7 @@
         <v>66</v>
       </c>
       <c r="S20" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T20" s="43"/>
       <c r="V20" s="45"/>
@@ -5564,15 +5486,9 @@
       <c r="E22" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="51" t="s">
-        <v>559</v>
-      </c>
-      <c r="G22" s="41" t="s">
-        <v>574</v>
-      </c>
-      <c r="H22" s="41" t="s">
-        <v>573</v>
-      </c>
+      <c r="F22" s="51"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
       <c r="I22" s="42"/>
       <c r="J22" s="43" t="s">
         <v>267</v>
@@ -5588,7 +5504,7 @@
         <v>267</v>
       </c>
       <c r="O22" s="43" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="P22" s="43" t="s">
         <v>66</v>
@@ -5600,7 +5516,7 @@
         <v>66</v>
       </c>
       <c r="S22" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T22" s="43"/>
       <c r="U22" s="44"/>
@@ -5625,15 +5541,9 @@
       <c r="E23" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="41" t="s">
-        <v>633</v>
-      </c>
-      <c r="G23" s="41" t="s">
-        <v>647</v>
-      </c>
-      <c r="H23" s="41" t="s">
-        <v>646</v>
-      </c>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
       <c r="I23" s="42"/>
       <c r="J23" s="43" t="s">
         <v>267</v>
@@ -5649,7 +5559,7 @@
         <v>267</v>
       </c>
       <c r="O23" s="43" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="P23" s="43" t="s">
         <v>66</v>
@@ -5661,7 +5571,7 @@
         <v>66</v>
       </c>
       <c r="S23" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T23" s="43"/>
       <c r="U23" s="44"/>
@@ -5801,7 +5711,7 @@
         <v>45713</v>
       </c>
       <c r="G27" s="41" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="H27" s="41"/>
       <c r="I27" s="42"/>
@@ -5857,10 +5767,10 @@
         <v>279</v>
       </c>
       <c r="F28" s="51" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="G28" s="41" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="H28" s="41"/>
       <c r="I28" s="42"/>
@@ -5955,10 +5865,10 @@
         <v>279</v>
       </c>
       <c r="F30" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G30" s="41" t="s">
-        <v>575</v>
+        <v>563</v>
       </c>
       <c r="H30" s="41"/>
       <c r="I30" s="42"/>
@@ -6014,10 +5924,10 @@
         <v>279</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="G31" s="41" t="s">
-        <v>648</v>
+        <v>631</v>
       </c>
       <c r="H31" s="41"/>
       <c r="I31" s="42"/>
@@ -6193,7 +6103,7 @@
         <v>45713</v>
       </c>
       <c r="G35" s="41" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="H35" s="41" t="s">
         <v>454</v>
@@ -6223,7 +6133,7 @@
         <v>66</v>
       </c>
       <c r="S35" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T35" s="43"/>
       <c r="U35" s="44"/>
@@ -6254,10 +6164,10 @@
         <v>45714</v>
       </c>
       <c r="G36" s="41" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H36" s="41" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="I36" s="42"/>
       <c r="J36" s="43" t="s">
@@ -6272,7 +6182,7 @@
         <v>267</v>
       </c>
       <c r="O36" s="43" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="P36" s="43" t="s">
         <v>66</v>
@@ -6284,7 +6194,7 @@
         <v>66</v>
       </c>
       <c r="S36" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T36" s="43"/>
       <c r="U36" s="44"/>
@@ -6313,10 +6223,10 @@
         <v>45714</v>
       </c>
       <c r="G37" s="41" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="H37" s="41" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="I37" s="42"/>
       <c r="J37" s="43" t="s">
@@ -6331,7 +6241,7 @@
         <v>267</v>
       </c>
       <c r="O37" s="43" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="P37" s="43" t="s">
         <v>66</v>
@@ -6343,12 +6253,12 @@
         <v>66</v>
       </c>
       <c r="S37" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T37" s="43"/>
       <c r="U37" s="44"/>
       <c r="V37" s="45" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="W37" s="43" t="s">
         <v>46</v>
@@ -6374,10 +6284,10 @@
         <v>45714</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="H38" s="41" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="I38" s="42"/>
       <c r="J38" s="43" t="s">
@@ -6392,7 +6302,7 @@
         <v>267</v>
       </c>
       <c r="O38" s="43" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="P38" s="43" t="s">
         <v>66</v>
@@ -6404,7 +6314,7 @@
         <v>66</v>
       </c>
       <c r="S38" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T38" s="43"/>
       <c r="U38" s="44"/>
@@ -6433,10 +6343,10 @@
         <v>45714</v>
       </c>
       <c r="G39" s="41" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="H39" s="41" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="I39" s="42"/>
       <c r="J39" s="43" t="s">
@@ -6451,7 +6361,7 @@
         <v>267</v>
       </c>
       <c r="O39" s="43" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="P39" s="43" t="s">
         <v>66</v>
@@ -6463,7 +6373,7 @@
         <v>66</v>
       </c>
       <c r="S39" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T39" s="43"/>
       <c r="U39" s="44"/>
@@ -6492,10 +6402,10 @@
         <v>45714</v>
       </c>
       <c r="G40" s="41" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="H40" s="41" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="I40" s="42"/>
       <c r="J40" s="43" t="s">
@@ -6510,7 +6420,7 @@
         <v>267</v>
       </c>
       <c r="O40" s="43" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="P40" s="43" t="s">
         <v>66</v>
@@ -6522,7 +6432,7 @@
         <v>66</v>
       </c>
       <c r="S40" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T40" s="43"/>
       <c r="U40" s="44"/>
@@ -6551,10 +6461,10 @@
         <v>45714</v>
       </c>
       <c r="G41" s="41" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="H41" s="41" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="I41" s="42"/>
       <c r="J41" s="43" t="s">
@@ -6569,7 +6479,7 @@
         <v>267</v>
       </c>
       <c r="O41" s="43" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="P41" s="43" t="s">
         <v>66</v>
@@ -6581,7 +6491,7 @@
         <v>66</v>
       </c>
       <c r="S41" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T41" s="43"/>
       <c r="U41" s="44"/>
@@ -6610,10 +6520,10 @@
         <v>45714</v>
       </c>
       <c r="G42" s="41" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="H42" s="41" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="I42" s="42"/>
       <c r="J42" s="43" t="s">
@@ -6628,7 +6538,7 @@
         <v>267</v>
       </c>
       <c r="O42" s="43" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="P42" s="43" t="s">
         <v>66</v>
@@ -6640,7 +6550,7 @@
         <v>66</v>
       </c>
       <c r="S42" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T42" s="43"/>
       <c r="U42" s="44"/>
@@ -6669,10 +6579,10 @@
         <v>45714</v>
       </c>
       <c r="G43" s="41" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="H43" s="41" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="I43" s="42"/>
       <c r="J43" s="43" t="s">
@@ -6687,7 +6597,7 @@
         <v>267</v>
       </c>
       <c r="O43" s="43" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="P43" s="43" t="s">
         <v>66</v>
@@ -6699,7 +6609,7 @@
         <v>66</v>
       </c>
       <c r="S43" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T43" s="43"/>
       <c r="U43" s="44"/>
@@ -6728,10 +6638,10 @@
         <v>45714</v>
       </c>
       <c r="G44" s="41" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="H44" s="41" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="I44" s="42"/>
       <c r="J44" s="43" t="s">
@@ -6746,7 +6656,7 @@
         <v>267</v>
       </c>
       <c r="O44" s="43" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="P44" s="43" t="s">
         <v>66</v>
@@ -6758,11 +6668,11 @@
         <v>66</v>
       </c>
       <c r="S44" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T44" s="43"/>
       <c r="U44" s="44" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="V44" s="45"/>
       <c r="W44" s="43" t="s">
@@ -6786,13 +6696,13 @@
         <v>95</v>
       </c>
       <c r="F45" s="41" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="G45" s="41" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="H45" s="41" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="I45" s="42"/>
       <c r="J45" s="43" t="s">
@@ -6819,11 +6729,11 @@
         <v>66</v>
       </c>
       <c r="S45" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T45" s="43"/>
       <c r="U45" s="44" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="V45" s="45"/>
       <c r="W45" s="43" t="s">
@@ -6847,13 +6757,13 @@
         <v>338</v>
       </c>
       <c r="F46" s="51" t="s">
+        <v>518</v>
+      </c>
+      <c r="G46" s="41" t="s">
         <v>524</v>
       </c>
-      <c r="G46" s="41" t="s">
-        <v>532</v>
-      </c>
       <c r="H46" s="41" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="I46" s="42"/>
       <c r="J46" s="43" t="s">
@@ -6868,7 +6778,7 @@
         <v>267</v>
       </c>
       <c r="O46" s="43" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="P46" s="43" t="s">
         <v>66</v>
@@ -6880,11 +6790,11 @@
         <v>66</v>
       </c>
       <c r="S46" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T46" s="43"/>
       <c r="U46" s="44" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="V46" s="45"/>
       <c r="W46" s="43" t="s">
@@ -6908,13 +6818,13 @@
         <v>340</v>
       </c>
       <c r="F47" s="51" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="G47" s="41" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="H47" s="41" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="I47" s="42"/>
       <c r="J47" s="43" t="s">
@@ -6929,7 +6839,7 @@
         <v>267</v>
       </c>
       <c r="O47" s="43" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="P47" s="43" t="s">
         <v>66</v>
@@ -6941,14 +6851,14 @@
         <v>66</v>
       </c>
       <c r="S47" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T47" s="43"/>
       <c r="U47" s="44" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="V47" s="45" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="W47" s="43" t="s">
         <v>46</v>
@@ -6971,13 +6881,13 @@
         <v>339</v>
       </c>
       <c r="F48" s="51" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="G48" s="41" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="H48" s="41" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="I48" s="42"/>
       <c r="J48" s="43" t="s">
@@ -6992,7 +6902,7 @@
         <v>267</v>
       </c>
       <c r="O48" s="43" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="P48" s="43" t="s">
         <v>66</v>
@@ -7004,11 +6914,11 @@
         <v>66</v>
       </c>
       <c r="S48" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T48" s="43"/>
       <c r="U48" s="44" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="V48" s="45"/>
       <c r="W48" s="43" t="s">
@@ -7032,13 +6942,13 @@
         <v>341</v>
       </c>
       <c r="F49" s="51" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="G49" s="41" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="H49" s="41" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="I49" s="42"/>
       <c r="J49" s="43" t="s">
@@ -7053,7 +6963,7 @@
         <v>267</v>
       </c>
       <c r="O49" s="43" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="P49" s="43" t="s">
         <v>66</v>
@@ -7065,11 +6975,11 @@
         <v>66</v>
       </c>
       <c r="S49" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T49" s="43"/>
       <c r="U49" s="44" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="V49" s="45"/>
       <c r="W49" s="43" t="s">
@@ -7093,13 +7003,13 @@
         <v>342</v>
       </c>
       <c r="F50" s="51" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="G50" s="41" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="H50" s="41" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="I50" s="42"/>
       <c r="J50" s="43" t="s">
@@ -7114,7 +7024,7 @@
         <v>267</v>
       </c>
       <c r="O50" s="43" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="P50" s="43" t="s">
         <v>66</v>
@@ -7126,11 +7036,11 @@
         <v>66</v>
       </c>
       <c r="S50" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T50" s="43"/>
       <c r="U50" s="44" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="V50" s="45"/>
       <c r="W50" s="43" t="s">
@@ -7154,13 +7064,13 @@
         <v>343</v>
       </c>
       <c r="F51" s="51" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="G51" s="41" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="H51" s="41" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="I51" s="42"/>
       <c r="J51" s="43" t="s">
@@ -7175,7 +7085,7 @@
         <v>267</v>
       </c>
       <c r="O51" s="43" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="P51" s="43" t="s">
         <v>66</v>
@@ -7187,11 +7097,11 @@
         <v>66</v>
       </c>
       <c r="S51" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T51" s="43"/>
       <c r="U51" s="44" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="V51" s="45"/>
       <c r="W51" s="43" t="s">
@@ -7215,13 +7125,13 @@
         <v>344</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="G52" s="41" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="H52" s="41" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="I52" s="42"/>
       <c r="J52" s="43" t="s">
@@ -7236,7 +7146,7 @@
         <v>267</v>
       </c>
       <c r="O52" s="43" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="P52" s="43" t="s">
         <v>66</v>
@@ -7248,11 +7158,11 @@
         <v>66</v>
       </c>
       <c r="S52" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T52" s="43"/>
       <c r="U52" s="44" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="V52" s="45"/>
       <c r="W52" s="43" t="s">
@@ -7276,13 +7186,13 @@
         <v>345</v>
       </c>
       <c r="F53" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G53" s="41" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="H53" s="41" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="I53" s="42"/>
       <c r="J53" s="43" t="s">
@@ -7297,7 +7207,7 @@
         <v>267</v>
       </c>
       <c r="O53" s="43" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="P53" s="43" t="s">
         <v>66</v>
@@ -7309,11 +7219,11 @@
         <v>66</v>
       </c>
       <c r="S53" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T53" s="43"/>
       <c r="U53" s="44" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="V53" s="45"/>
       <c r="W53" s="43" t="s">
@@ -7337,13 +7247,13 @@
         <v>346</v>
       </c>
       <c r="F54" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G54" s="41" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="H54" s="41" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
       <c r="I54" s="42"/>
       <c r="J54" s="43" t="s">
@@ -7358,7 +7268,7 @@
         <v>267</v>
       </c>
       <c r="O54" s="43" t="s">
-        <v>587</v>
+        <v>574</v>
       </c>
       <c r="P54" s="43" t="s">
         <v>66</v>
@@ -7370,11 +7280,11 @@
         <v>66</v>
       </c>
       <c r="S54" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T54" s="43"/>
       <c r="U54" s="44" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="V54" s="45"/>
       <c r="W54" s="43" t="s">
@@ -7398,13 +7308,13 @@
         <v>347</v>
       </c>
       <c r="F55" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G55" s="41" t="s">
-        <v>592</v>
+        <v>579</v>
       </c>
       <c r="H55" s="41" t="s">
-        <v>591</v>
+        <v>578</v>
       </c>
       <c r="I55" s="42"/>
       <c r="J55" s="43" t="s">
@@ -7419,7 +7329,7 @@
         <v>267</v>
       </c>
       <c r="O55" s="43" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="P55" s="43" t="s">
         <v>66</v>
@@ -7431,11 +7341,11 @@
         <v>66</v>
       </c>
       <c r="S55" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T55" s="43"/>
       <c r="U55" s="44" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="V55" s="45"/>
       <c r="W55" s="43" t="s">
@@ -7459,13 +7369,13 @@
         <v>348</v>
       </c>
       <c r="F56" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G56" s="41" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="H56" s="41" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="I56" s="42"/>
       <c r="J56" s="43" t="s">
@@ -7480,7 +7390,7 @@
         <v>267</v>
       </c>
       <c r="O56" s="43" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="P56" s="43" t="s">
         <v>66</v>
@@ -7492,11 +7402,11 @@
         <v>66</v>
       </c>
       <c r="S56" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T56" s="43"/>
       <c r="U56" s="44" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="V56" s="45"/>
       <c r="W56" s="43" t="s">
@@ -7520,13 +7430,13 @@
         <v>349</v>
       </c>
       <c r="F57" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G57" s="41" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="H57" s="41" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
       <c r="I57" s="42"/>
       <c r="J57" s="43" t="s">
@@ -7541,7 +7451,7 @@
         <v>267</v>
       </c>
       <c r="O57" s="43" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="P57" s="43" t="s">
         <v>66</v>
@@ -7553,11 +7463,11 @@
         <v>66</v>
       </c>
       <c r="S57" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T57" s="43"/>
       <c r="U57" s="44" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="V57" s="45"/>
       <c r="W57" s="43" t="s">
@@ -7581,13 +7491,13 @@
         <v>350</v>
       </c>
       <c r="F58" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G58" s="41" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="H58" s="41" t="s">
-        <v>576</v>
+        <v>564</v>
       </c>
       <c r="I58" s="42"/>
       <c r="J58" s="43" t="s">
@@ -7602,7 +7512,7 @@
         <v>267</v>
       </c>
       <c r="O58" s="43" t="s">
-        <v>717</v>
+        <v>700</v>
       </c>
       <c r="P58" s="43" t="s">
         <v>66</v>
@@ -7614,11 +7524,11 @@
         <v>66</v>
       </c>
       <c r="S58" s="43" t="s">
-        <v>583</v>
+        <v>66</v>
       </c>
       <c r="T58" s="43"/>
       <c r="U58" s="44" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="V58" s="45"/>
       <c r="W58" s="43" t="s">
@@ -7642,13 +7552,13 @@
         <v>351</v>
       </c>
       <c r="F59" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G59" s="41" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="H59" s="41" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="I59" s="42"/>
       <c r="J59" s="43" t="s">
@@ -7663,7 +7573,7 @@
         <v>267</v>
       </c>
       <c r="O59" s="43" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="P59" s="43" t="s">
         <v>66</v>
@@ -7675,11 +7585,11 @@
         <v>66</v>
       </c>
       <c r="S59" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T59" s="43"/>
       <c r="U59" s="44" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="V59" s="45"/>
       <c r="W59" s="43" t="s">
@@ -7703,13 +7613,13 @@
         <v>111</v>
       </c>
       <c r="F60" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G60" s="41" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="H60" s="41" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="I60" s="42"/>
       <c r="J60" s="43" t="s">
@@ -7724,7 +7634,7 @@
         <v>267</v>
       </c>
       <c r="O60" s="43" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="P60" s="43" t="s">
         <v>66</v>
@@ -7736,11 +7646,11 @@
         <v>66</v>
       </c>
       <c r="S60" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T60" s="43"/>
       <c r="U60" s="44" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="V60" s="45"/>
       <c r="W60" s="43" t="s">
@@ -7764,13 +7674,13 @@
         <v>113</v>
       </c>
       <c r="F61" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G61" s="41" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="H61" s="41" t="s">
-        <v>597</v>
+        <v>584</v>
       </c>
       <c r="I61" s="42"/>
       <c r="J61" s="43" t="s">
@@ -7785,7 +7695,7 @@
         <v>267</v>
       </c>
       <c r="O61" s="43" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
       <c r="P61" s="43" t="s">
         <v>66</v>
@@ -7797,11 +7707,11 @@
         <v>66</v>
       </c>
       <c r="S61" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T61" s="43"/>
       <c r="U61" s="44" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="V61" s="45"/>
       <c r="W61" s="43" t="s">
@@ -7825,13 +7735,13 @@
         <v>352</v>
       </c>
       <c r="F62" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G62" s="41" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="H62" s="41" t="s">
-        <v>600</v>
+        <v>587</v>
       </c>
       <c r="I62" s="42"/>
       <c r="J62" s="43" t="s">
@@ -7846,7 +7756,7 @@
         <v>267</v>
       </c>
       <c r="O62" s="43" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="P62" s="43" t="s">
         <v>66</v>
@@ -7858,11 +7768,11 @@
         <v>66</v>
       </c>
       <c r="S62" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T62" s="43"/>
       <c r="U62" s="44" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="V62" s="45"/>
       <c r="W62" s="43" t="s">
@@ -7886,13 +7796,13 @@
         <v>353</v>
       </c>
       <c r="F63" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G63" s="41" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="H63" s="41" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="I63" s="42"/>
       <c r="J63" s="43" t="s">
@@ -7907,7 +7817,7 @@
         <v>267</v>
       </c>
       <c r="O63" s="43" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="P63" s="43" t="s">
         <v>66</v>
@@ -7919,11 +7829,11 @@
         <v>66</v>
       </c>
       <c r="S63" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T63" s="43"/>
       <c r="U63" s="44" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="V63" s="45"/>
       <c r="W63" s="43" t="s">
@@ -7947,13 +7857,13 @@
         <v>354</v>
       </c>
       <c r="F64" s="41" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="G64" s="41" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="H64" s="41" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="I64" s="42"/>
       <c r="J64" s="43" t="s">
@@ -7968,7 +7878,7 @@
         <v>267</v>
       </c>
       <c r="O64" s="43" t="s">
-        <v>616</v>
+        <v>603</v>
       </c>
       <c r="P64" s="43" t="s">
         <v>66</v>
@@ -7980,11 +7890,11 @@
         <v>66</v>
       </c>
       <c r="S64" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T64" s="43"/>
       <c r="U64" s="44" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="V64" s="45"/>
       <c r="W64" s="43" t="s">
@@ -8008,13 +7918,13 @@
         <v>355</v>
       </c>
       <c r="F65" s="41" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="G65" s="41" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="H65" s="41" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="I65" s="42"/>
       <c r="J65" s="43" t="s">
@@ -8029,7 +7939,7 @@
         <v>267</v>
       </c>
       <c r="O65" s="43" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="P65" s="43" t="s">
         <v>66</v>
@@ -8041,7 +7951,7 @@
         <v>66</v>
       </c>
       <c r="S65" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T65" s="43"/>
       <c r="U65" s="44"/>
@@ -8067,13 +7977,13 @@
         <v>119</v>
       </c>
       <c r="F66" s="41" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="G66" s="41" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
       <c r="H66" s="41" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
       <c r="I66" s="42"/>
       <c r="J66" s="43" t="s">
@@ -8088,7 +7998,7 @@
         <v>267</v>
       </c>
       <c r="O66" s="43" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
       <c r="P66" s="43" t="s">
         <v>66</v>
@@ -8100,7 +8010,7 @@
         <v>66</v>
       </c>
       <c r="S66" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T66" s="43"/>
       <c r="U66" s="44"/>
@@ -8126,13 +8036,13 @@
         <v>121</v>
       </c>
       <c r="F67" s="41" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="G67" s="41" t="s">
-        <v>620</v>
+        <v>607</v>
       </c>
       <c r="H67" s="41" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="I67" s="42"/>
       <c r="J67" s="43" t="s">
@@ -8147,7 +8057,7 @@
         <v>267</v>
       </c>
       <c r="O67" s="43" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="P67" s="43" t="s">
         <v>66</v>
@@ -8159,7 +8069,7 @@
         <v>66</v>
       </c>
       <c r="S67" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T67" s="43"/>
       <c r="U67" s="44"/>
@@ -8185,13 +8095,13 @@
         <v>356</v>
       </c>
       <c r="F68" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G68" s="41" t="s">
-        <v>666</v>
+        <v>649</v>
       </c>
       <c r="H68" s="41" t="s">
-        <v>665</v>
+        <v>648</v>
       </c>
       <c r="I68" s="42"/>
       <c r="J68" s="43" t="s">
@@ -8206,7 +8116,7 @@
         <v>267</v>
       </c>
       <c r="O68" s="43" t="s">
-        <v>664</v>
+        <v>647</v>
       </c>
       <c r="P68" s="43" t="s">
         <v>66</v>
@@ -8218,7 +8128,7 @@
         <v>66</v>
       </c>
       <c r="S68" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T68" s="43"/>
       <c r="U68" s="44"/>
@@ -8244,13 +8154,13 @@
         <v>357</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="G69" s="41" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="H69" s="41" t="s">
-        <v>623</v>
+        <v>610</v>
       </c>
       <c r="I69" s="42"/>
       <c r="J69" s="43" t="s">
@@ -8265,7 +8175,7 @@
         <v>267</v>
       </c>
       <c r="O69" s="43" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="P69" s="43" t="s">
         <v>66</v>
@@ -8277,7 +8187,7 @@
         <v>66</v>
       </c>
       <c r="S69" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T69" s="43"/>
       <c r="U69" s="44"/>
@@ -8303,13 +8213,13 @@
         <v>358</v>
       </c>
       <c r="F70" s="41" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="G70" s="41" t="s">
-        <v>627</v>
+        <v>614</v>
       </c>
       <c r="H70" s="41" t="s">
-        <v>626</v>
+        <v>613</v>
       </c>
       <c r="I70" s="42"/>
       <c r="J70" s="43" t="s">
@@ -8324,7 +8234,7 @@
         <v>267</v>
       </c>
       <c r="O70" s="43" t="s">
-        <v>625</v>
+        <v>612</v>
       </c>
       <c r="P70" s="43" t="s">
         <v>66</v>
@@ -8336,7 +8246,7 @@
         <v>66</v>
       </c>
       <c r="S70" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T70" s="43"/>
       <c r="U70" s="44"/>
@@ -8362,13 +8272,13 @@
         <v>359</v>
       </c>
       <c r="F71" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G71" s="41" t="s">
-        <v>663</v>
+        <v>646</v>
       </c>
       <c r="H71" s="41" t="s">
-        <v>662</v>
+        <v>645</v>
       </c>
       <c r="I71" s="42"/>
       <c r="J71" s="43" t="s">
@@ -8383,7 +8293,7 @@
         <v>267</v>
       </c>
       <c r="O71" s="43" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
       <c r="P71" s="43" t="s">
         <v>66</v>
@@ -8395,7 +8305,7 @@
         <v>66</v>
       </c>
       <c r="S71" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T71" s="43"/>
       <c r="U71" s="44"/>
@@ -8421,13 +8331,13 @@
         <v>127</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="G72" s="41" t="s">
-        <v>630</v>
+        <v>617</v>
       </c>
       <c r="H72" s="41" t="s">
-        <v>629</v>
+        <v>616</v>
       </c>
       <c r="I72" s="42"/>
       <c r="J72" s="43" t="s">
@@ -8442,7 +8352,7 @@
         <v>267</v>
       </c>
       <c r="O72" s="43" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
       <c r="P72" s="43" t="s">
         <v>66</v>
@@ -8454,7 +8364,7 @@
         <v>66</v>
       </c>
       <c r="S72" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T72" s="43"/>
       <c r="U72" s="44"/>
@@ -8480,13 +8390,13 @@
         <v>129</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="G73" s="41" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="H73" s="41" t="s">
-        <v>632</v>
+        <v>619</v>
       </c>
       <c r="I73" s="42"/>
       <c r="J73" s="43" t="s">
@@ -8501,7 +8411,7 @@
         <v>267</v>
       </c>
       <c r="O73" s="43" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
       <c r="P73" s="43" t="s">
         <v>66</v>
@@ -8513,7 +8423,7 @@
         <v>66</v>
       </c>
       <c r="S73" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T73" s="43"/>
       <c r="U73" s="44"/>
@@ -8539,13 +8449,13 @@
         <v>360</v>
       </c>
       <c r="F74" s="41" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="G74" s="41" t="s">
-        <v>640</v>
+        <v>627</v>
       </c>
       <c r="H74" s="41" t="s">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="I74" s="42"/>
       <c r="J74" s="43" t="s">
@@ -8560,7 +8470,7 @@
         <v>267</v>
       </c>
       <c r="O74" s="43" t="s">
-        <v>635</v>
+        <v>622</v>
       </c>
       <c r="P74" s="43" t="s">
         <v>66</v>
@@ -8572,7 +8482,7 @@
         <v>66</v>
       </c>
       <c r="S74" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T74" s="43"/>
       <c r="U74" s="44"/>
@@ -8598,13 +8508,13 @@
         <v>415</v>
       </c>
       <c r="F75" s="41" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="G75" s="41" t="s">
-        <v>643</v>
+        <v>630</v>
       </c>
       <c r="H75" s="41" t="s">
-        <v>642</v>
+        <v>629</v>
       </c>
       <c r="I75" s="42"/>
       <c r="J75" s="43" t="s">
@@ -8619,7 +8529,7 @@
         <v>267</v>
       </c>
       <c r="O75" s="43" t="s">
-        <v>641</v>
+        <v>628</v>
       </c>
       <c r="P75" s="43" t="s">
         <v>66</v>
@@ -8631,7 +8541,7 @@
         <v>66</v>
       </c>
       <c r="S75" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T75" s="43"/>
       <c r="U75" s="44"/>
@@ -8657,13 +8567,13 @@
         <v>361</v>
       </c>
       <c r="F76" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G76" s="41" t="s">
-        <v>669</v>
+        <v>652</v>
       </c>
       <c r="H76" s="41" t="s">
-        <v>668</v>
+        <v>651</v>
       </c>
       <c r="I76" s="42"/>
       <c r="J76" s="43" t="s">
@@ -8678,7 +8588,7 @@
         <v>267</v>
       </c>
       <c r="O76" s="43" t="s">
-        <v>667</v>
+        <v>650</v>
       </c>
       <c r="P76" s="43" t="s">
         <v>66</v>
@@ -8690,7 +8600,7 @@
         <v>66</v>
       </c>
       <c r="S76" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T76" s="43"/>
       <c r="U76" s="44"/>
@@ -8729,7 +8639,7 @@
       <c r="Q77" s="29"/>
       <c r="R77" s="29"/>
       <c r="S77" s="29" t="s">
-        <v>636</v>
+        <v>623</v>
       </c>
       <c r="T77" s="29"/>
       <c r="U77" s="34"/>
@@ -8768,7 +8678,7 @@
       <c r="Q78" s="29"/>
       <c r="R78" s="29"/>
       <c r="S78" s="29" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="T78" s="29"/>
       <c r="U78" s="34"/>
@@ -8806,7 +8716,7 @@
       <c r="P79" s="29"/>
       <c r="Q79" s="29"/>
       <c r="R79" s="29" t="s">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="S79" s="29"/>
       <c r="T79" s="29"/>
@@ -10683,13 +10593,13 @@
         <v>209</v>
       </c>
       <c r="F130" s="41" t="s">
+        <v>620</v>
+      </c>
+      <c r="G130" s="41" t="s">
+        <v>634</v>
+      </c>
+      <c r="H130" s="41" t="s">
         <v>633</v>
-      </c>
-      <c r="G130" s="41" t="s">
-        <v>651</v>
-      </c>
-      <c r="H130" s="41" t="s">
-        <v>650</v>
       </c>
       <c r="I130" s="42"/>
       <c r="J130" s="43" t="s">
@@ -10704,7 +10614,7 @@
         <v>267</v>
       </c>
       <c r="O130" s="43" t="s">
-        <v>649</v>
+        <v>632</v>
       </c>
       <c r="P130" s="43" t="s">
         <v>66</v>
@@ -10742,13 +10652,13 @@
         <v>390</v>
       </c>
       <c r="F131" s="41" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="G131" s="41" t="s">
-        <v>653</v>
+        <v>636</v>
       </c>
       <c r="H131" s="41" t="s">
-        <v>652</v>
+        <v>635</v>
       </c>
       <c r="I131" s="42"/>
       <c r="J131" s="43" t="s">
@@ -10763,7 +10673,7 @@
         <v>267</v>
       </c>
       <c r="O131" s="43" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="P131" s="43" t="s">
         <v>66</v>
@@ -10801,13 +10711,13 @@
         <v>391</v>
       </c>
       <c r="F132" s="41" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="G132" s="41" t="s">
-        <v>656</v>
+        <v>639</v>
       </c>
       <c r="H132" s="41" t="s">
-        <v>655</v>
+        <v>638</v>
       </c>
       <c r="I132" s="42"/>
       <c r="J132" s="43" t="s">
@@ -10822,7 +10732,7 @@
         <v>267</v>
       </c>
       <c r="O132" s="43" t="s">
-        <v>654</v>
+        <v>637</v>
       </c>
       <c r="P132" s="43" t="s">
         <v>66</v>
@@ -10860,13 +10770,13 @@
         <v>392</v>
       </c>
       <c r="F133" s="41" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="G133" s="41" t="s">
-        <v>659</v>
+        <v>642</v>
       </c>
       <c r="H133" s="41" t="s">
-        <v>658</v>
+        <v>641</v>
       </c>
       <c r="I133" s="42"/>
       <c r="J133" s="43" t="s">
@@ -10881,7 +10791,7 @@
         <v>267</v>
       </c>
       <c r="O133" s="43" t="s">
-        <v>657</v>
+        <v>640</v>
       </c>
       <c r="P133" s="43" t="s">
         <v>66</v>
@@ -10919,13 +10829,13 @@
         <v>393</v>
       </c>
       <c r="F134" s="41" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="G134" s="41" t="s">
-        <v>659</v>
+        <v>642</v>
       </c>
       <c r="H134" s="41" t="s">
-        <v>660</v>
+        <v>643</v>
       </c>
       <c r="I134" s="42"/>
       <c r="J134" s="43" t="s">
@@ -10940,7 +10850,7 @@
         <v>267</v>
       </c>
       <c r="O134" s="43" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="P134" s="43" t="s">
         <v>66</v>
@@ -10978,13 +10888,13 @@
         <v>394</v>
       </c>
       <c r="F135" s="41" t="s">
+        <v>644</v>
+      </c>
+      <c r="G135" s="41" t="s">
+        <v>662</v>
+      </c>
+      <c r="H135" s="41" t="s">
         <v>661</v>
-      </c>
-      <c r="G135" s="41" t="s">
-        <v>679</v>
-      </c>
-      <c r="H135" s="41" t="s">
-        <v>678</v>
       </c>
       <c r="I135" s="42"/>
       <c r="J135" s="43" t="s">
@@ -10999,7 +10909,7 @@
         <v>267</v>
       </c>
       <c r="O135" s="43" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="P135" s="43" t="s">
         <v>66</v>
@@ -11037,13 +10947,13 @@
         <v>395</v>
       </c>
       <c r="F136" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G136" s="41" t="s">
-        <v>682</v>
+        <v>665</v>
       </c>
       <c r="H136" s="41" t="s">
-        <v>681</v>
+        <v>664</v>
       </c>
       <c r="I136" s="42"/>
       <c r="J136" s="43" t="s">
@@ -11058,7 +10968,7 @@
         <v>267</v>
       </c>
       <c r="O136" s="43" t="s">
-        <v>680</v>
+        <v>663</v>
       </c>
       <c r="P136" s="43" t="s">
         <v>66</v>
@@ -11096,13 +11006,13 @@
         <v>217</v>
       </c>
       <c r="F137" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G137" s="41" t="s">
-        <v>684</v>
+        <v>667</v>
       </c>
       <c r="H137" s="41" t="s">
-        <v>683</v>
+        <v>666</v>
       </c>
       <c r="I137" s="42"/>
       <c r="J137" s="43" t="s">
@@ -11117,7 +11027,7 @@
         <v>267</v>
       </c>
       <c r="O137" s="43" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
       <c r="P137" s="43" t="s">
         <v>66</v>
@@ -11155,13 +11065,13 @@
         <v>219</v>
       </c>
       <c r="F138" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G138" s="41" t="s">
-        <v>687</v>
+        <v>670</v>
       </c>
       <c r="H138" s="41" t="s">
-        <v>686</v>
+        <v>669</v>
       </c>
       <c r="I138" s="42"/>
       <c r="J138" s="43" t="s">
@@ -11176,7 +11086,7 @@
         <v>267</v>
       </c>
       <c r="O138" s="43" t="s">
-        <v>685</v>
+        <v>668</v>
       </c>
       <c r="P138" s="43" t="s">
         <v>66</v>
@@ -11214,13 +11124,13 @@
         <v>324</v>
       </c>
       <c r="F139" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G139" s="41" t="s">
-        <v>691</v>
+        <v>674</v>
       </c>
       <c r="H139" s="41" t="s">
-        <v>690</v>
+        <v>673</v>
       </c>
       <c r="I139" s="42"/>
       <c r="J139" s="43" t="s">
@@ -11235,7 +11145,7 @@
         <v>267</v>
       </c>
       <c r="O139" s="43" t="s">
-        <v>688</v>
+        <v>671</v>
       </c>
       <c r="P139" s="43" t="s">
         <v>66</v>
@@ -11273,13 +11183,13 @@
         <v>325</v>
       </c>
       <c r="F140" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G140" s="41" t="s">
-        <v>694</v>
+        <v>677</v>
       </c>
       <c r="H140" s="41" t="s">
-        <v>693</v>
+        <v>676</v>
       </c>
       <c r="I140" s="42"/>
       <c r="J140" s="43" t="s">
@@ -11294,7 +11204,7 @@
         <v>267</v>
       </c>
       <c r="O140" s="43" t="s">
-        <v>692</v>
+        <v>675</v>
       </c>
       <c r="P140" s="43" t="s">
         <v>66</v>
@@ -11332,13 +11242,13 @@
         <v>326</v>
       </c>
       <c r="F141" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G141" s="41" t="s">
-        <v>694</v>
+        <v>677</v>
       </c>
       <c r="H141" s="41" t="s">
-        <v>695</v>
+        <v>678</v>
       </c>
       <c r="I141" s="42"/>
       <c r="J141" s="43" t="s">
@@ -11353,7 +11263,7 @@
         <v>267</v>
       </c>
       <c r="O141" s="43" t="s">
-        <v>685</v>
+        <v>668</v>
       </c>
       <c r="P141" s="43" t="s">
         <v>66</v>
@@ -11391,13 +11301,13 @@
         <v>327</v>
       </c>
       <c r="F142" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G142" s="41" t="s">
-        <v>698</v>
+        <v>681</v>
       </c>
       <c r="H142" s="41" t="s">
-        <v>697</v>
+        <v>680</v>
       </c>
       <c r="I142" s="42"/>
       <c r="J142" s="43" t="s">
@@ -11412,7 +11322,7 @@
         <v>267</v>
       </c>
       <c r="O142" s="43" t="s">
-        <v>696</v>
+        <v>679</v>
       </c>
       <c r="P142" s="43" t="s">
         <v>66</v>
@@ -11450,13 +11360,13 @@
         <v>328</v>
       </c>
       <c r="F143" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G143" s="41" t="s">
-        <v>701</v>
+        <v>684</v>
       </c>
       <c r="H143" s="41" t="s">
-        <v>700</v>
+        <v>683</v>
       </c>
       <c r="I143" s="42"/>
       <c r="J143" s="43" t="s">
@@ -11471,7 +11381,7 @@
         <v>267</v>
       </c>
       <c r="O143" s="43" t="s">
-        <v>699</v>
+        <v>682</v>
       </c>
       <c r="P143" s="43" t="s">
         <v>66</v>
@@ -11509,13 +11419,13 @@
         <v>329</v>
       </c>
       <c r="F144" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G144" s="41" t="s">
-        <v>704</v>
+        <v>687</v>
       </c>
       <c r="H144" s="41" t="s">
-        <v>703</v>
+        <v>686</v>
       </c>
       <c r="I144" s="42"/>
       <c r="J144" s="43" t="s">
@@ -11530,7 +11440,7 @@
         <v>267</v>
       </c>
       <c r="O144" s="43" t="s">
-        <v>702</v>
+        <v>685</v>
       </c>
       <c r="P144" s="43" t="s">
         <v>66</v>
@@ -11568,13 +11478,13 @@
         <v>330</v>
       </c>
       <c r="F145" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G145" s="41" t="s">
-        <v>707</v>
+        <v>690</v>
       </c>
       <c r="H145" s="41" t="s">
-        <v>706</v>
+        <v>689</v>
       </c>
       <c r="I145" s="42"/>
       <c r="J145" s="43" t="s">
@@ -11589,7 +11499,7 @@
         <v>267</v>
       </c>
       <c r="O145" s="43" t="s">
-        <v>705</v>
+        <v>688</v>
       </c>
       <c r="P145" s="43" t="s">
         <v>66</v>
@@ -11627,13 +11537,13 @@
         <v>331</v>
       </c>
       <c r="F146" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G146" s="41" t="s">
-        <v>710</v>
+        <v>693</v>
       </c>
       <c r="H146" s="41" t="s">
-        <v>709</v>
+        <v>692</v>
       </c>
       <c r="I146" s="42"/>
       <c r="J146" s="43" t="s">
@@ -11648,7 +11558,7 @@
         <v>267</v>
       </c>
       <c r="O146" s="43" t="s">
-        <v>708</v>
+        <v>691</v>
       </c>
       <c r="P146" s="43" t="s">
         <v>66</v>
@@ -11686,13 +11596,13 @@
         <v>333</v>
       </c>
       <c r="F147" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G147" s="41" t="s">
-        <v>713</v>
+        <v>696</v>
       </c>
       <c r="H147" s="41" t="s">
-        <v>712</v>
+        <v>695</v>
       </c>
       <c r="I147" s="42"/>
       <c r="J147" s="43" t="s">
@@ -11707,7 +11617,7 @@
         <v>267</v>
       </c>
       <c r="O147" s="43" t="s">
-        <v>711</v>
+        <v>694</v>
       </c>
       <c r="P147" s="43" t="s">
         <v>66</v>
@@ -11758,7 +11668,7 @@
       <c r="Q148" s="29"/>
       <c r="R148" s="29"/>
       <c r="S148" s="29" t="s">
-        <v>636</v>
+        <v>623</v>
       </c>
       <c r="T148" s="29"/>
       <c r="U148" s="34"/>
@@ -11797,7 +11707,7 @@
       <c r="Q149" s="29"/>
       <c r="R149" s="29"/>
       <c r="S149" s="29" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="T149" s="29"/>
       <c r="U149" s="34"/>
@@ -11835,7 +11745,7 @@
       <c r="P150" s="29"/>
       <c r="Q150" s="29"/>
       <c r="R150" s="29" t="s">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="S150" s="29"/>
       <c r="T150" s="29"/>
@@ -11874,7 +11784,7 @@
       <c r="P151" s="29"/>
       <c r="Q151" s="29"/>
       <c r="R151" s="29" t="s">
-        <v>689</v>
+        <v>672</v>
       </c>
       <c r="S151" s="29"/>
       <c r="T151" s="29"/>
@@ -11913,7 +11823,7 @@
       <c r="P152" s="29"/>
       <c r="Q152" s="29"/>
       <c r="R152" s="29" t="s">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="S152" s="29"/>
       <c r="T152" s="29"/>
@@ -12367,7 +12277,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="165" spans="1:23" s="46" customFormat="1" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:23" s="46" customFormat="1" ht="110.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="38">
         <v>191</v>
       </c>
@@ -12410,7 +12320,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="166" spans="1:23" s="46" customFormat="1" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23" s="46" customFormat="1" ht="46.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="38">
         <v>376</v>
       </c>
@@ -12453,7 +12363,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="31">
         <v>417</v>
       </c>
@@ -12490,7 +12400,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="31">
         <v>418</v>
       </c>
@@ -12527,7 +12437,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="31">
         <v>419</v>
       </c>
@@ -13082,7 +12992,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="31">
         <v>444</v>
       </c>
@@ -13119,7 +13029,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="31">
         <v>445</v>
       </c>
@@ -13156,7 +13066,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="186" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="38">
         <v>446</v>
       </c>
@@ -13173,16 +13083,16 @@
         <v>321</v>
       </c>
       <c r="F186" s="41" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="G186" s="41" t="s">
-        <v>609</v>
+        <v>596</v>
       </c>
       <c r="H186" s="41" t="s">
-        <v>608</v>
+        <v>595</v>
       </c>
       <c r="I186" s="42" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="J186" s="43" t="s">
         <v>66</v>
@@ -13215,7 +13125,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="187" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="38">
         <v>447</v>
       </c>
@@ -13232,16 +13142,16 @@
         <v>322</v>
       </c>
       <c r="F187" s="41" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="G187" s="41" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="H187" s="41" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="I187" s="42" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="J187" s="43" t="s">
         <v>66</v>
@@ -13274,7 +13184,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="38">
         <v>448</v>
       </c>
@@ -13285,22 +13195,22 @@
         <v>51</v>
       </c>
       <c r="D188" s="38" t="s">
-        <v>670</v>
+        <v>653</v>
       </c>
       <c r="E188" s="47" t="s">
         <v>441</v>
       </c>
       <c r="F188" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G188" s="41" t="s">
-        <v>674</v>
+        <v>657</v>
       </c>
       <c r="H188" s="41" t="s">
-        <v>673</v>
+        <v>656</v>
       </c>
       <c r="I188" s="42" t="s">
-        <v>672</v>
+        <v>655</v>
       </c>
       <c r="J188" s="43" t="s">
         <v>66</v>
@@ -13333,7 +13243,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="189" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="38">
         <v>449</v>
       </c>
@@ -13344,22 +13254,22 @@
         <v>51</v>
       </c>
       <c r="D189" s="38" t="s">
-        <v>671</v>
+        <v>654</v>
       </c>
       <c r="E189" s="47" t="s">
         <v>442</v>
       </c>
       <c r="F189" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G189" s="41" t="s">
-        <v>677</v>
+        <v>660</v>
       </c>
       <c r="H189" s="41" t="s">
-        <v>676</v>
+        <v>659</v>
       </c>
       <c r="I189" s="42" t="s">
-        <v>675</v>
+        <v>658</v>
       </c>
       <c r="J189" s="43" t="s">
         <v>66</v>
@@ -13392,7 +13302,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="190" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="38">
         <v>450</v>
       </c>
@@ -13409,16 +13319,16 @@
         <v>427</v>
       </c>
       <c r="F190" s="51" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G190" s="41" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="H190" s="41" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="I190" s="42" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="J190" s="43" t="s">
         <v>66</v>
@@ -13447,13 +13357,13 @@
       </c>
       <c r="U190" s="44"/>
       <c r="V190" s="45" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="W190" s="43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="191" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="38">
         <v>451</v>
       </c>
@@ -13470,16 +13380,16 @@
         <v>428</v>
       </c>
       <c r="F191" s="41" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="G191" s="41" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H191" s="41" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="I191" s="42" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="J191" s="43" t="s">
         <v>66</v>
@@ -13512,7 +13422,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="192" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="38">
         <v>452</v>
       </c>
@@ -13529,16 +13439,16 @@
         <v>422</v>
       </c>
       <c r="F192" s="41" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="G192" s="41" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="H192" s="41" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="I192" s="42" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="J192" s="43" t="s">
         <v>66</v>
@@ -13567,13 +13477,13 @@
       </c>
       <c r="U192" s="44"/>
       <c r="V192" s="45" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="W192" s="43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="193" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="31">
         <v>454</v>
       </c>
@@ -13610,7 +13520,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="194" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="31">
         <v>455</v>
       </c>
@@ -13647,7 +13557,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="195" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="31">
         <v>456</v>
       </c>
@@ -13684,7 +13594,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="196" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="31">
         <v>457</v>
       </c>
@@ -13721,7 +13631,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="197" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="31">
         <v>458</v>
       </c>
@@ -13758,7 +13668,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="31">
         <v>459</v>
       </c>
@@ -13795,7 +13705,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="199" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="31">
         <v>460</v>
       </c>
@@ -13849,13 +13759,13 @@
         <v>443</v>
       </c>
       <c r="F200" s="41" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
       <c r="G200" s="41" t="s">
-        <v>716</v>
+        <v>699</v>
       </c>
       <c r="H200" s="41" t="s">
-        <v>715</v>
+        <v>698</v>
       </c>
       <c r="I200" s="42"/>
       <c r="J200" s="43" t="s">
@@ -13870,7 +13780,7 @@
         <v>267</v>
       </c>
       <c r="O200" s="43" t="s">
-        <v>714</v>
+        <v>697</v>
       </c>
       <c r="P200" s="43" t="s">
         <v>66</v>
@@ -18203,7 +18113,13 @@
       <c r="W770" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:W200" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A9:W200" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="22">
+      <filters>
+        <filter val="KO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -18224,7 +18140,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J14 M14:N15 J16:J20 P10:R12 J22 J24:J28 M22:N28 M20:N20 M10:N12 J10:J12 P14:R20 J30:J198 M16:M20 N16:N19 P22:R28 P200:R200 M200:N200 M30:N198 P30:R198</xm:sqref>
+          <xm:sqref>J14 M14:N15 J16:J20 S14:S15 J22 J24:J28 M22:N28 M20:N20 M10:N12 J10:J12 S19:S20 J30:J198 M16:M20 N16:N19 P22:R28 P200:R200 M200:N200 M30:N198 P30:R198 S35:S76 S22:S23 P14:R20 S11:S12 P10:R12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
@@ -20483,25 +20399,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F560B38A5B3C4B41B1895754B1F1A56A" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="69dc0f489d46816a4b9bb4a327e14425">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca719f03-9e45-4ef4-9920-d156f53157f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7de9a44ff87fdcabda187bbd662e75de" ns2:_="">
     <xsd:import namespace="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
@@ -20673,7 +20570,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -20691,32 +20633,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
completamento dei workflowInstanceId mancanti
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA22CCB9-3B53-4DB9-BCDE-4C5A9A972FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBAD2DF-0E9E-47D3-83E1-8712E97952FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2036" uniqueCount="760">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1826,9 +1826,6 @@
     <t>/msg/semantic</t>
   </si>
   <si>
-    <t>2025-02-25T20:31:59</t>
-  </si>
-  <si>
     <t>[ERRORE-12| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ],[W002 | Si consiglia di valorizzare l'elemento organizer[CLUSTER]/code]</t>
   </si>
   <si>
@@ -1973,9 +1970,6 @@
     <t>Campo token JWT non valido. - Il campo purpose_of_use non è corretto</t>
   </si>
   <si>
-    <t>2025-02-27T10:01:53</t>
-  </si>
-  <si>
     <t>ERROR: -1,-1 cvc-datatype-valid.1.2.3: '18719-5' is not a valid value of union type 'uid'.,ERROR: -1,-1 cvc-attribute.3: The value '18719-5' of attribute 'codeSystem' on element 'confidentialityCode' is not valid with respect to its type, 'uid'.</t>
   </si>
   <si>
@@ -2097,9 +2091,6 @@
   </si>
   <si>
     <t>Il campo purpose_of_use non è corretto - Campo token JWT non valido.</t>
-  </si>
-  <si>
-    <t>2025-03-03T11:31:09</t>
   </si>
   <si>
     <t>988fa3c278ed8f24</t>
@@ -2305,9 +2296,6 @@
     <t>2025-03-05T10:37:04</t>
   </si>
   <si>
-    <t>2025-03-05T11:37:30</t>
-  </si>
-  <si>
     <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{"urn:hl7-org:v3":confidentialityCode}' is expected.</t>
   </si>
   <si>
@@ -2513,6 +2501,195 @@
   </si>
   <si>
     <t>ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'confidentialityCode' is not valid with respect to its type, 'cs'.</t>
+  </si>
+  <si>
+    <t>il timeout viene simulato spegnendo la connessione di rete</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.5127d7a2d6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.ab58cd30a1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.73f64e56cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.d9ac2965e3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.6a45f93a1d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.b1f6398ccc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.433aa990aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.87b81320b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.3891644d71^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.d3c08ef5cc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>il test del timeout viene simulato spegnendo la connessione di rete</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.c59851b07a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.d4f62a9e8e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.ee4062e4d5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.5f96aaec9b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.fa10496a9b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.3683f9f6de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.55cd1e991e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.7dec7892a8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.5e70a8a928^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.f86ae29432^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.f71510684b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.10fafebc95^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.cde77a9a8d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.c4b07e1160^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.44bde8e784^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.ae1b349a6a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.18f225bf7e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.c1cafe4389^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.524670ca13^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.30004e373d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.38b0f792b4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.7d6d5024bd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.1b4ce4d6d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.bf2796a22e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.0f4ba70929^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.edc7d504e0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.06a772f797^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.feda319422^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.be430f2fa0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.c2d04d085b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.ab8543e365^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.6366ed19b6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.32258d91ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.68e1a6272a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.3fff304f76^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.bd31eed57e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.780272e66d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.484a5cb0fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.5876b130c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.312391feec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.856543c04f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.5ad2e97069^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.c02f214f02^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.7844d9ab98^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.d2c3c34a50^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.791c7b157b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.9c1621538d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.fbec971273^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.44322b8400^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.23498d1136^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.4e00b77522^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4601,14 +4778,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W770"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A35" sqref="A35:XFD35"/>
+      <selection pane="bottomRight" activeCell="I200" sqref="I200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4891,7 +5067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="48">
         <v>4</v>
       </c>
@@ -4908,16 +5084,16 @@
         <v>424</v>
       </c>
       <c r="F10" s="50" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G10" s="50" t="s">
+        <v>523</v>
+      </c>
+      <c r="H10" s="50" t="s">
+        <v>524</v>
+      </c>
+      <c r="I10" s="41" t="s">
         <v>525</v>
-      </c>
-      <c r="H10" s="50" t="s">
-        <v>526</v>
-      </c>
-      <c r="I10" s="41" t="s">
-        <v>527</v>
       </c>
       <c r="J10" s="43" t="s">
         <v>66</v>
@@ -4946,7 +5122,7 @@
       </c>
       <c r="U10" s="44"/>
       <c r="V10" s="50" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="W10" s="43" t="s">
         <v>36</v>
@@ -5043,7 +5219,7 @@
         <v>267</v>
       </c>
       <c r="O12" s="43" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="P12" s="43" t="s">
         <v>66</v>
@@ -5135,7 +5311,7 @@
         <v>267</v>
       </c>
       <c r="O14" s="43" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="P14" s="43" t="s">
         <v>66</v>
@@ -5190,7 +5366,7 @@
         <v>267</v>
       </c>
       <c r="O15" s="43" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="P15" s="43" t="s">
         <v>66</v>
@@ -5413,7 +5589,7 @@
         <v>267</v>
       </c>
       <c r="O20" s="43" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="P20" s="43" t="s">
         <v>66</v>
@@ -5559,7 +5735,7 @@
         <v>267</v>
       </c>
       <c r="O23" s="43" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="P23" s="43" t="s">
         <v>66</v>
@@ -5707,19 +5883,19 @@
       <c r="E27" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="F27" s="41">
-        <v>45713</v>
-      </c>
-      <c r="G27" s="41" t="s">
-        <v>472</v>
-      </c>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
       <c r="H27" s="41"/>
       <c r="I27" s="42"/>
       <c r="J27" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
+        <v>267</v>
+      </c>
+      <c r="K27" s="43" t="s">
+        <v>278</v>
+      </c>
+      <c r="L27" s="43" t="s">
+        <v>697</v>
+      </c>
       <c r="M27" s="43" t="s">
         <v>66</v>
       </c>
@@ -5739,7 +5915,7 @@
         <v>66</v>
       </c>
       <c r="S27" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T27" s="43"/>
       <c r="U27" s="44" t="s">
@@ -5766,19 +5942,19 @@
       <c r="E28" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="F28" s="51" t="s">
-        <v>518</v>
-      </c>
-      <c r="G28" s="41" t="s">
-        <v>521</v>
-      </c>
+      <c r="F28" s="51"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="41"/>
       <c r="I28" s="42"/>
       <c r="J28" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
+        <v>267</v>
+      </c>
+      <c r="K28" s="43" t="s">
+        <v>278</v>
+      </c>
+      <c r="L28" s="43" t="s">
+        <v>708</v>
+      </c>
       <c r="M28" s="43" t="s">
         <v>66</v>
       </c>
@@ -5864,19 +6040,19 @@
       <c r="E30" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="F30" s="51" t="s">
-        <v>551</v>
-      </c>
-      <c r="G30" s="41" t="s">
-        <v>563</v>
-      </c>
+      <c r="F30" s="51"/>
+      <c r="G30" s="41"/>
       <c r="H30" s="41"/>
       <c r="I30" s="42"/>
       <c r="J30" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
+        <v>267</v>
+      </c>
+      <c r="K30" s="43" t="s">
+        <v>278</v>
+      </c>
+      <c r="L30" s="43" t="s">
+        <v>708</v>
+      </c>
       <c r="M30" s="43" t="s">
         <v>66</v>
       </c>
@@ -5896,7 +6072,7 @@
         <v>66</v>
       </c>
       <c r="S30" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T30" s="43"/>
       <c r="U30" s="44" t="s">
@@ -5923,19 +6099,19 @@
       <c r="E31" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="F31" s="41" t="s">
-        <v>620</v>
-      </c>
-      <c r="G31" s="41" t="s">
-        <v>631</v>
-      </c>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
       <c r="H31" s="41"/>
       <c r="I31" s="42"/>
       <c r="J31" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
+        <v>267</v>
+      </c>
+      <c r="K31" s="43" t="s">
+        <v>278</v>
+      </c>
+      <c r="L31" s="43" t="s">
+        <v>708</v>
+      </c>
       <c r="M31" s="43" t="s">
         <v>66</v>
       </c>
@@ -5955,7 +6131,7 @@
         <v>66</v>
       </c>
       <c r="S31" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T31" s="43"/>
       <c r="U31" s="44" t="s">
@@ -6108,7 +6284,9 @@
       <c r="H35" s="41" t="s">
         <v>454</v>
       </c>
-      <c r="I35" s="42"/>
+      <c r="I35" s="42" t="s">
+        <v>759</v>
+      </c>
       <c r="J35" s="43" t="s">
         <v>66</v>
       </c>
@@ -6169,7 +6347,9 @@
       <c r="H36" s="41" t="s">
         <v>466</v>
       </c>
-      <c r="I36" s="42"/>
+      <c r="I36" s="42" t="s">
+        <v>698</v>
+      </c>
       <c r="J36" s="43" t="s">
         <v>66</v>
       </c>
@@ -6228,7 +6408,9 @@
       <c r="H37" s="41" t="s">
         <v>470</v>
       </c>
-      <c r="I37" s="42"/>
+      <c r="I37" s="42" t="s">
+        <v>699</v>
+      </c>
       <c r="J37" s="43" t="s">
         <v>66</v>
       </c>
@@ -6284,12 +6466,14 @@
         <v>45714</v>
       </c>
       <c r="G38" s="41" t="s">
+        <v>473</v>
+      </c>
+      <c r="H38" s="41" t="s">
         <v>474</v>
       </c>
-      <c r="H38" s="41" t="s">
-        <v>475</v>
-      </c>
-      <c r="I38" s="42"/>
+      <c r="I38" s="42" t="s">
+        <v>700</v>
+      </c>
       <c r="J38" s="43" t="s">
         <v>66</v>
       </c>
@@ -6302,7 +6486,7 @@
         <v>267</v>
       </c>
       <c r="O38" s="43" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="P38" s="43" t="s">
         <v>66</v>
@@ -6343,12 +6527,14 @@
         <v>45714</v>
       </c>
       <c r="G39" s="41" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H39" s="41" t="s">
-        <v>477</v>
-      </c>
-      <c r="I39" s="42"/>
+        <v>476</v>
+      </c>
+      <c r="I39" s="42" t="s">
+        <v>701</v>
+      </c>
       <c r="J39" s="43" t="s">
         <v>66</v>
       </c>
@@ -6361,7 +6547,7 @@
         <v>267</v>
       </c>
       <c r="O39" s="43" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="P39" s="43" t="s">
         <v>66</v>
@@ -6402,12 +6588,14 @@
         <v>45714</v>
       </c>
       <c r="G40" s="41" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="H40" s="41" t="s">
-        <v>480</v>
-      </c>
-      <c r="I40" s="42"/>
+        <v>479</v>
+      </c>
+      <c r="I40" s="42" t="s">
+        <v>702</v>
+      </c>
       <c r="J40" s="43" t="s">
         <v>66</v>
       </c>
@@ -6420,7 +6608,7 @@
         <v>267</v>
       </c>
       <c r="O40" s="43" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="P40" s="43" t="s">
         <v>66</v>
@@ -6461,12 +6649,14 @@
         <v>45714</v>
       </c>
       <c r="G41" s="41" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H41" s="41" t="s">
-        <v>483</v>
-      </c>
-      <c r="I41" s="42"/>
+        <v>482</v>
+      </c>
+      <c r="I41" s="42" t="s">
+        <v>703</v>
+      </c>
       <c r="J41" s="43" t="s">
         <v>66</v>
       </c>
@@ -6479,7 +6669,7 @@
         <v>267</v>
       </c>
       <c r="O41" s="43" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P41" s="43" t="s">
         <v>66</v>
@@ -6520,12 +6710,14 @@
         <v>45714</v>
       </c>
       <c r="G42" s="41" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H42" s="41" t="s">
-        <v>486</v>
-      </c>
-      <c r="I42" s="42"/>
+        <v>485</v>
+      </c>
+      <c r="I42" s="42" t="s">
+        <v>704</v>
+      </c>
       <c r="J42" s="43" t="s">
         <v>66</v>
       </c>
@@ -6538,7 +6730,7 @@
         <v>267</v>
       </c>
       <c r="O42" s="43" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P42" s="43" t="s">
         <v>66</v>
@@ -6579,12 +6771,14 @@
         <v>45714</v>
       </c>
       <c r="G43" s="41" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H43" s="41" t="s">
-        <v>511</v>
-      </c>
-      <c r="I43" s="42"/>
+        <v>510</v>
+      </c>
+      <c r="I43" s="42" t="s">
+        <v>705</v>
+      </c>
       <c r="J43" s="43" t="s">
         <v>66</v>
       </c>
@@ -6597,7 +6791,7 @@
         <v>267</v>
       </c>
       <c r="O43" s="43" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P43" s="43" t="s">
         <v>66</v>
@@ -6638,12 +6832,14 @@
         <v>45714</v>
       </c>
       <c r="G44" s="41" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H44" s="41" t="s">
-        <v>514</v>
-      </c>
-      <c r="I44" s="42"/>
+        <v>513</v>
+      </c>
+      <c r="I44" s="42" t="s">
+        <v>706</v>
+      </c>
       <c r="J44" s="43" t="s">
         <v>66</v>
       </c>
@@ -6656,7 +6852,7 @@
         <v>267</v>
       </c>
       <c r="O44" s="43" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="P44" s="43" t="s">
         <v>66</v>
@@ -6672,7 +6868,7 @@
       </c>
       <c r="T44" s="43"/>
       <c r="U44" s="44" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="V44" s="45"/>
       <c r="W44" s="43" t="s">
@@ -6696,15 +6892,17 @@
         <v>95</v>
       </c>
       <c r="F45" s="41" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="G45" s="41" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H45" s="41" t="s">
-        <v>516</v>
-      </c>
-      <c r="I45" s="42"/>
+        <v>515</v>
+      </c>
+      <c r="I45" s="42" t="s">
+        <v>707</v>
+      </c>
       <c r="J45" s="43" t="s">
         <v>66</v>
       </c>
@@ -6733,7 +6931,7 @@
       </c>
       <c r="T45" s="43"/>
       <c r="U45" s="44" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="V45" s="45"/>
       <c r="W45" s="43" t="s">
@@ -6757,15 +6955,17 @@
         <v>338</v>
       </c>
       <c r="F46" s="51" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G46" s="41" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H46" s="41" t="s">
-        <v>523</v>
-      </c>
-      <c r="I46" s="42"/>
+        <v>521</v>
+      </c>
+      <c r="I46" s="42" t="s">
+        <v>709</v>
+      </c>
       <c r="J46" s="43" t="s">
         <v>66</v>
       </c>
@@ -6778,7 +6978,7 @@
         <v>267</v>
       </c>
       <c r="O46" s="43" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="P46" s="43" t="s">
         <v>66</v>
@@ -6794,7 +6994,7 @@
       </c>
       <c r="T46" s="43"/>
       <c r="U46" s="44" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="V46" s="45"/>
       <c r="W46" s="43" t="s">
@@ -6818,15 +7018,17 @@
         <v>340</v>
       </c>
       <c r="F47" s="51" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G47" s="41" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="H47" s="41" t="s">
-        <v>534</v>
-      </c>
-      <c r="I47" s="42"/>
+        <v>532</v>
+      </c>
+      <c r="I47" s="42" t="s">
+        <v>710</v>
+      </c>
       <c r="J47" s="43" t="s">
         <v>66</v>
       </c>
@@ -6839,7 +7041,7 @@
         <v>267</v>
       </c>
       <c r="O47" s="43" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="P47" s="43" t="s">
         <v>66</v>
@@ -6855,10 +7057,10 @@
       </c>
       <c r="T47" s="43"/>
       <c r="U47" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="V47" s="45" t="s">
         <v>492</v>
-      </c>
-      <c r="V47" s="45" t="s">
-        <v>493</v>
       </c>
       <c r="W47" s="43" t="s">
         <v>46</v>
@@ -6881,15 +7083,17 @@
         <v>339</v>
       </c>
       <c r="F48" s="51" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G48" s="41" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H48" s="41" t="s">
-        <v>537</v>
-      </c>
-      <c r="I48" s="42"/>
+        <v>535</v>
+      </c>
+      <c r="I48" s="42" t="s">
+        <v>711</v>
+      </c>
       <c r="J48" s="43" t="s">
         <v>66</v>
       </c>
@@ -6902,7 +7106,7 @@
         <v>267</v>
       </c>
       <c r="O48" s="43" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="P48" s="43" t="s">
         <v>66</v>
@@ -6918,7 +7122,7 @@
       </c>
       <c r="T48" s="43"/>
       <c r="U48" s="44" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="V48" s="45"/>
       <c r="W48" s="43" t="s">
@@ -6942,15 +7146,17 @@
         <v>341</v>
       </c>
       <c r="F49" s="51" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G49" s="41" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H49" s="41" t="s">
-        <v>540</v>
-      </c>
-      <c r="I49" s="42"/>
+        <v>538</v>
+      </c>
+      <c r="I49" s="42" t="s">
+        <v>712</v>
+      </c>
       <c r="J49" s="43" t="s">
         <v>66</v>
       </c>
@@ -6963,7 +7169,7 @@
         <v>267</v>
       </c>
       <c r="O49" s="43" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="P49" s="43" t="s">
         <v>66</v>
@@ -6979,7 +7185,7 @@
       </c>
       <c r="T49" s="43"/>
       <c r="U49" s="44" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="V49" s="45"/>
       <c r="W49" s="43" t="s">
@@ -7003,15 +7209,17 @@
         <v>342</v>
       </c>
       <c r="F50" s="51" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G50" s="41" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H50" s="41" t="s">
-        <v>543</v>
-      </c>
-      <c r="I50" s="42"/>
+        <v>541</v>
+      </c>
+      <c r="I50" s="42" t="s">
+        <v>713</v>
+      </c>
       <c r="J50" s="43" t="s">
         <v>66</v>
       </c>
@@ -7024,7 +7232,7 @@
         <v>267</v>
       </c>
       <c r="O50" s="43" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="P50" s="43" t="s">
         <v>66</v>
@@ -7040,7 +7248,7 @@
       </c>
       <c r="T50" s="43"/>
       <c r="U50" s="44" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="V50" s="45"/>
       <c r="W50" s="43" t="s">
@@ -7064,15 +7272,17 @@
         <v>343</v>
       </c>
       <c r="F51" s="51" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G51" s="41" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="H51" s="41" t="s">
-        <v>545</v>
-      </c>
-      <c r="I51" s="42"/>
+        <v>543</v>
+      </c>
+      <c r="I51" s="42" t="s">
+        <v>714</v>
+      </c>
       <c r="J51" s="43" t="s">
         <v>66</v>
       </c>
@@ -7085,7 +7295,7 @@
         <v>267</v>
       </c>
       <c r="O51" s="43" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="P51" s="43" t="s">
         <v>66</v>
@@ -7101,7 +7311,7 @@
       </c>
       <c r="T51" s="43"/>
       <c r="U51" s="44" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V51" s="45"/>
       <c r="W51" s="43" t="s">
@@ -7125,15 +7335,17 @@
         <v>344</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G52" s="41" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="H52" s="41" t="s">
-        <v>548</v>
-      </c>
-      <c r="I52" s="42"/>
+        <v>546</v>
+      </c>
+      <c r="I52" s="42" t="s">
+        <v>715</v>
+      </c>
       <c r="J52" s="43" t="s">
         <v>66</v>
       </c>
@@ -7146,7 +7358,7 @@
         <v>267</v>
       </c>
       <c r="O52" s="43" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="P52" s="43" t="s">
         <v>66</v>
@@ -7162,7 +7374,7 @@
       </c>
       <c r="T52" s="43"/>
       <c r="U52" s="44" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="V52" s="45"/>
       <c r="W52" s="43" t="s">
@@ -7186,15 +7398,17 @@
         <v>345</v>
       </c>
       <c r="F53" s="51" t="s">
+        <v>549</v>
+      </c>
+      <c r="G53" s="41" t="s">
         <v>551</v>
       </c>
-      <c r="G53" s="41" t="s">
-        <v>553</v>
-      </c>
       <c r="H53" s="41" t="s">
-        <v>552</v>
-      </c>
-      <c r="I53" s="42"/>
+        <v>550</v>
+      </c>
+      <c r="I53" s="42" t="s">
+        <v>716</v>
+      </c>
       <c r="J53" s="43" t="s">
         <v>66</v>
       </c>
@@ -7207,7 +7421,7 @@
         <v>267</v>
       </c>
       <c r="O53" s="43" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="P53" s="43" t="s">
         <v>66</v>
@@ -7223,7 +7437,7 @@
       </c>
       <c r="T53" s="43"/>
       <c r="U53" s="44" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="V53" s="45"/>
       <c r="W53" s="43" t="s">
@@ -7247,15 +7461,17 @@
         <v>346</v>
       </c>
       <c r="F54" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G54" s="41" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="H54" s="41" t="s">
-        <v>575</v>
-      </c>
-      <c r="I54" s="42"/>
+        <v>572</v>
+      </c>
+      <c r="I54" s="42" t="s">
+        <v>717</v>
+      </c>
       <c r="J54" s="43" t="s">
         <v>66</v>
       </c>
@@ -7268,7 +7484,7 @@
         <v>267</v>
       </c>
       <c r="O54" s="43" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="P54" s="43" t="s">
         <v>66</v>
@@ -7284,7 +7500,7 @@
       </c>
       <c r="T54" s="43"/>
       <c r="U54" s="44" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="V54" s="45"/>
       <c r="W54" s="43" t="s">
@@ -7308,15 +7524,17 @@
         <v>347</v>
       </c>
       <c r="F55" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G55" s="41" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="H55" s="41" t="s">
-        <v>578</v>
-      </c>
-      <c r="I55" s="42"/>
+        <v>575</v>
+      </c>
+      <c r="I55" s="42" t="s">
+        <v>718</v>
+      </c>
       <c r="J55" s="43" t="s">
         <v>66</v>
       </c>
@@ -7329,7 +7547,7 @@
         <v>267</v>
       </c>
       <c r="O55" s="43" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="P55" s="43" t="s">
         <v>66</v>
@@ -7345,7 +7563,7 @@
       </c>
       <c r="T55" s="43"/>
       <c r="U55" s="44" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="V55" s="45"/>
       <c r="W55" s="43" t="s">
@@ -7369,15 +7587,17 @@
         <v>348</v>
       </c>
       <c r="F56" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G56" s="41" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="H56" s="41" t="s">
-        <v>581</v>
-      </c>
-      <c r="I56" s="42"/>
+        <v>578</v>
+      </c>
+      <c r="I56" s="42" t="s">
+        <v>719</v>
+      </c>
       <c r="J56" s="43" t="s">
         <v>66</v>
       </c>
@@ -7390,7 +7610,7 @@
         <v>267</v>
       </c>
       <c r="O56" s="43" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="P56" s="43" t="s">
         <v>66</v>
@@ -7406,7 +7626,7 @@
       </c>
       <c r="T56" s="43"/>
       <c r="U56" s="44" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="V56" s="45"/>
       <c r="W56" s="43" t="s">
@@ -7430,15 +7650,17 @@
         <v>349</v>
       </c>
       <c r="F57" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G57" s="41" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="H57" s="41" t="s">
-        <v>572</v>
-      </c>
-      <c r="I57" s="42"/>
+        <v>569</v>
+      </c>
+      <c r="I57" s="42" t="s">
+        <v>720</v>
+      </c>
       <c r="J57" s="43" t="s">
         <v>66</v>
       </c>
@@ -7451,7 +7673,7 @@
         <v>267</v>
       </c>
       <c r="O57" s="43" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="P57" s="43" t="s">
         <v>66</v>
@@ -7467,7 +7689,7 @@
       </c>
       <c r="T57" s="43"/>
       <c r="U57" s="44" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="V57" s="45"/>
       <c r="W57" s="43" t="s">
@@ -7491,15 +7713,17 @@
         <v>350</v>
       </c>
       <c r="F58" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G58" s="41" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H58" s="41" t="s">
-        <v>564</v>
-      </c>
-      <c r="I58" s="42"/>
+        <v>561</v>
+      </c>
+      <c r="I58" s="42" t="s">
+        <v>721</v>
+      </c>
       <c r="J58" s="43" t="s">
         <v>66</v>
       </c>
@@ -7512,7 +7736,7 @@
         <v>267</v>
       </c>
       <c r="O58" s="43" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="P58" s="43" t="s">
         <v>66</v>
@@ -7528,7 +7752,7 @@
       </c>
       <c r="T58" s="43"/>
       <c r="U58" s="44" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="V58" s="45"/>
       <c r="W58" s="43" t="s">
@@ -7552,15 +7776,17 @@
         <v>351</v>
       </c>
       <c r="F59" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G59" s="41" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="H59" s="41" t="s">
-        <v>566</v>
-      </c>
-      <c r="I59" s="42"/>
+        <v>563</v>
+      </c>
+      <c r="I59" s="42" t="s">
+        <v>722</v>
+      </c>
       <c r="J59" s="43" t="s">
         <v>66</v>
       </c>
@@ -7573,7 +7799,7 @@
         <v>267</v>
       </c>
       <c r="O59" s="43" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="P59" s="43" t="s">
         <v>66</v>
@@ -7589,7 +7815,7 @@
       </c>
       <c r="T59" s="43"/>
       <c r="U59" s="44" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="V59" s="45"/>
       <c r="W59" s="43" t="s">
@@ -7613,15 +7839,17 @@
         <v>111</v>
       </c>
       <c r="F60" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G60" s="41" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="H60" s="41" t="s">
-        <v>569</v>
-      </c>
-      <c r="I60" s="42"/>
+        <v>566</v>
+      </c>
+      <c r="I60" s="42" t="s">
+        <v>723</v>
+      </c>
       <c r="J60" s="43" t="s">
         <v>66</v>
       </c>
@@ -7634,7 +7862,7 @@
         <v>267</v>
       </c>
       <c r="O60" s="43" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="P60" s="43" t="s">
         <v>66</v>
@@ -7650,7 +7878,7 @@
       </c>
       <c r="T60" s="43"/>
       <c r="U60" s="44" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="V60" s="45"/>
       <c r="W60" s="43" t="s">
@@ -7674,15 +7902,17 @@
         <v>113</v>
       </c>
       <c r="F61" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G61" s="41" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="H61" s="41" t="s">
-        <v>584</v>
-      </c>
-      <c r="I61" s="42"/>
+        <v>581</v>
+      </c>
+      <c r="I61" s="42" t="s">
+        <v>724</v>
+      </c>
       <c r="J61" s="43" t="s">
         <v>66</v>
       </c>
@@ -7695,7 +7925,7 @@
         <v>267</v>
       </c>
       <c r="O61" s="43" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="P61" s="43" t="s">
         <v>66</v>
@@ -7711,7 +7941,7 @@
       </c>
       <c r="T61" s="43"/>
       <c r="U61" s="44" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V61" s="45"/>
       <c r="W61" s="43" t="s">
@@ -7735,15 +7965,17 @@
         <v>352</v>
       </c>
       <c r="F62" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G62" s="41" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H62" s="41" t="s">
-        <v>587</v>
-      </c>
-      <c r="I62" s="42"/>
+        <v>584</v>
+      </c>
+      <c r="I62" s="42" t="s">
+        <v>725</v>
+      </c>
       <c r="J62" s="43" t="s">
         <v>66</v>
       </c>
@@ -7756,7 +7988,7 @@
         <v>267</v>
       </c>
       <c r="O62" s="43" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="P62" s="43" t="s">
         <v>66</v>
@@ -7772,7 +8004,7 @@
       </c>
       <c r="T62" s="43"/>
       <c r="U62" s="44" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="V62" s="45"/>
       <c r="W62" s="43" t="s">
@@ -7796,15 +8028,17 @@
         <v>353</v>
       </c>
       <c r="F63" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G63" s="41" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="H63" s="41" t="s">
-        <v>589</v>
-      </c>
-      <c r="I63" s="42"/>
+        <v>586</v>
+      </c>
+      <c r="I63" s="42" t="s">
+        <v>726</v>
+      </c>
       <c r="J63" s="43" t="s">
         <v>66</v>
       </c>
@@ -7817,7 +8051,7 @@
         <v>267</v>
       </c>
       <c r="O63" s="43" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="P63" s="43" t="s">
         <v>66</v>
@@ -7833,7 +8067,7 @@
       </c>
       <c r="T63" s="43"/>
       <c r="U63" s="44" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="V63" s="45"/>
       <c r="W63" s="43" t="s">
@@ -7857,15 +8091,17 @@
         <v>354</v>
       </c>
       <c r="F64" s="41" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="G64" s="41" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="H64" s="41" t="s">
-        <v>604</v>
-      </c>
-      <c r="I64" s="42"/>
+        <v>601</v>
+      </c>
+      <c r="I64" s="42" t="s">
+        <v>727</v>
+      </c>
       <c r="J64" s="43" t="s">
         <v>66</v>
       </c>
@@ -7878,7 +8114,7 @@
         <v>267</v>
       </c>
       <c r="O64" s="43" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="P64" s="43" t="s">
         <v>66</v>
@@ -7894,7 +8130,7 @@
       </c>
       <c r="T64" s="43"/>
       <c r="U64" s="44" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="V64" s="45"/>
       <c r="W64" s="43" t="s">
@@ -7918,15 +8154,17 @@
         <v>355</v>
       </c>
       <c r="F65" s="41" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="G65" s="41" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="H65" s="41" t="s">
-        <v>591</v>
-      </c>
-      <c r="I65" s="42"/>
+        <v>588</v>
+      </c>
+      <c r="I65" s="42" t="s">
+        <v>728</v>
+      </c>
       <c r="J65" s="43" t="s">
         <v>66</v>
       </c>
@@ -7939,7 +8177,7 @@
         <v>267</v>
       </c>
       <c r="O65" s="43" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="P65" s="43" t="s">
         <v>66</v>
@@ -7977,15 +8215,17 @@
         <v>119</v>
       </c>
       <c r="F66" s="41" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="G66" s="41" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H66" s="41" t="s">
-        <v>601</v>
-      </c>
-      <c r="I66" s="42"/>
+        <v>598</v>
+      </c>
+      <c r="I66" s="42" t="s">
+        <v>729</v>
+      </c>
       <c r="J66" s="43" t="s">
         <v>66</v>
       </c>
@@ -7998,7 +8238,7 @@
         <v>267</v>
       </c>
       <c r="O66" s="43" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="P66" s="43" t="s">
         <v>66</v>
@@ -8036,15 +8276,17 @@
         <v>121</v>
       </c>
       <c r="F67" s="41" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="G67" s="41" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="H67" s="41" t="s">
-        <v>608</v>
-      </c>
-      <c r="I67" s="42"/>
+        <v>605</v>
+      </c>
+      <c r="I67" s="42" t="s">
+        <v>730</v>
+      </c>
       <c r="J67" s="43" t="s">
         <v>66</v>
       </c>
@@ -8057,7 +8299,7 @@
         <v>267</v>
       </c>
       <c r="O67" s="43" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="P67" s="43" t="s">
         <v>66</v>
@@ -8095,15 +8337,17 @@
         <v>356</v>
       </c>
       <c r="F68" s="41" t="s">
+        <v>640</v>
+      </c>
+      <c r="G68" s="41" t="s">
+        <v>645</v>
+      </c>
+      <c r="H68" s="41" t="s">
         <v>644</v>
       </c>
-      <c r="G68" s="41" t="s">
-        <v>649</v>
-      </c>
-      <c r="H68" s="41" t="s">
-        <v>648</v>
-      </c>
-      <c r="I68" s="42"/>
+      <c r="I68" s="42" t="s">
+        <v>731</v>
+      </c>
       <c r="J68" s="43" t="s">
         <v>66</v>
       </c>
@@ -8116,7 +8360,7 @@
         <v>267</v>
       </c>
       <c r="O68" s="43" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="P68" s="43" t="s">
         <v>66</v>
@@ -8154,15 +8398,17 @@
         <v>357</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="G69" s="41" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="H69" s="41" t="s">
-        <v>610</v>
-      </c>
-      <c r="I69" s="42"/>
+        <v>607</v>
+      </c>
+      <c r="I69" s="42" t="s">
+        <v>732</v>
+      </c>
       <c r="J69" s="43" t="s">
         <v>66</v>
       </c>
@@ -8175,7 +8421,7 @@
         <v>267</v>
       </c>
       <c r="O69" s="43" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="P69" s="43" t="s">
         <v>66</v>
@@ -8213,15 +8459,17 @@
         <v>358</v>
       </c>
       <c r="F70" s="41" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="G70" s="41" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="H70" s="41" t="s">
-        <v>613</v>
-      </c>
-      <c r="I70" s="42"/>
+        <v>610</v>
+      </c>
+      <c r="I70" s="42" t="s">
+        <v>733</v>
+      </c>
       <c r="J70" s="43" t="s">
         <v>66</v>
       </c>
@@ -8234,7 +8482,7 @@
         <v>267</v>
       </c>
       <c r="O70" s="43" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="P70" s="43" t="s">
         <v>66</v>
@@ -8272,15 +8520,17 @@
         <v>359</v>
       </c>
       <c r="F71" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G71" s="41" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="H71" s="41" t="s">
-        <v>645</v>
-      </c>
-      <c r="I71" s="42"/>
+        <v>641</v>
+      </c>
+      <c r="I71" s="42" t="s">
+        <v>734</v>
+      </c>
       <c r="J71" s="43" t="s">
         <v>66</v>
       </c>
@@ -8293,7 +8543,7 @@
         <v>267</v>
       </c>
       <c r="O71" s="43" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="P71" s="43" t="s">
         <v>66</v>
@@ -8331,15 +8581,17 @@
         <v>127</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="G72" s="41" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="H72" s="41" t="s">
-        <v>616</v>
-      </c>
-      <c r="I72" s="42"/>
+        <v>613</v>
+      </c>
+      <c r="I72" s="42" t="s">
+        <v>735</v>
+      </c>
       <c r="J72" s="43" t="s">
         <v>66</v>
       </c>
@@ -8352,7 +8604,7 @@
         <v>267</v>
       </c>
       <c r="O72" s="43" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="P72" s="43" t="s">
         <v>66</v>
@@ -8390,15 +8642,17 @@
         <v>129</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="G73" s="41" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="H73" s="41" t="s">
-        <v>619</v>
-      </c>
-      <c r="I73" s="42"/>
+        <v>616</v>
+      </c>
+      <c r="I73" s="42" t="s">
+        <v>736</v>
+      </c>
       <c r="J73" s="43" t="s">
         <v>66</v>
       </c>
@@ -8411,7 +8665,7 @@
         <v>267</v>
       </c>
       <c r="O73" s="43" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="P73" s="43" t="s">
         <v>66</v>
@@ -8449,15 +8703,17 @@
         <v>360</v>
       </c>
       <c r="F74" s="41" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="G74" s="41" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="H74" s="41" t="s">
-        <v>626</v>
-      </c>
-      <c r="I74" s="42"/>
+        <v>623</v>
+      </c>
+      <c r="I74" s="42" t="s">
+        <v>737</v>
+      </c>
       <c r="J74" s="43" t="s">
         <v>66</v>
       </c>
@@ -8470,7 +8726,7 @@
         <v>267</v>
       </c>
       <c r="O74" s="43" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="P74" s="43" t="s">
         <v>66</v>
@@ -8508,15 +8764,17 @@
         <v>415</v>
       </c>
       <c r="F75" s="41" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="G75" s="41" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="H75" s="41" t="s">
-        <v>629</v>
-      </c>
-      <c r="I75" s="42"/>
+        <v>626</v>
+      </c>
+      <c r="I75" s="42" t="s">
+        <v>738</v>
+      </c>
       <c r="J75" s="43" t="s">
         <v>66</v>
       </c>
@@ -8529,7 +8787,7 @@
         <v>267</v>
       </c>
       <c r="O75" s="43" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="P75" s="43" t="s">
         <v>66</v>
@@ -8567,15 +8825,17 @@
         <v>361</v>
       </c>
       <c r="F76" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G76" s="41" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="H76" s="41" t="s">
-        <v>651</v>
-      </c>
-      <c r="I76" s="42"/>
+        <v>647</v>
+      </c>
+      <c r="I76" s="42" t="s">
+        <v>739</v>
+      </c>
       <c r="J76" s="43" t="s">
         <v>66</v>
       </c>
@@ -8588,7 +8848,7 @@
         <v>267</v>
       </c>
       <c r="O76" s="43" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="P76" s="43" t="s">
         <v>66</v>
@@ -8639,7 +8899,7 @@
       <c r="Q77" s="29"/>
       <c r="R77" s="29"/>
       <c r="S77" s="29" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="T77" s="29"/>
       <c r="U77" s="34"/>
@@ -8678,7 +8938,7 @@
       <c r="Q78" s="29"/>
       <c r="R78" s="29"/>
       <c r="S78" s="29" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="T78" s="29"/>
       <c r="U78" s="34"/>
@@ -8716,7 +8976,7 @@
       <c r="P79" s="29"/>
       <c r="Q79" s="29"/>
       <c r="R79" s="29" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="S79" s="29"/>
       <c r="T79" s="29"/>
@@ -10593,15 +10853,17 @@
         <v>209</v>
       </c>
       <c r="F130" s="41" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="G130" s="41" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="H130" s="41" t="s">
-        <v>633</v>
-      </c>
-      <c r="I130" s="42"/>
+        <v>629</v>
+      </c>
+      <c r="I130" s="42" t="s">
+        <v>740</v>
+      </c>
       <c r="J130" s="43" t="s">
         <v>66</v>
       </c>
@@ -10614,7 +10876,7 @@
         <v>267</v>
       </c>
       <c r="O130" s="43" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="P130" s="43" t="s">
         <v>66</v>
@@ -10626,7 +10888,7 @@
         <v>66</v>
       </c>
       <c r="S130" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T130" s="43"/>
       <c r="U130" s="44"/>
@@ -10652,15 +10914,17 @@
         <v>390</v>
       </c>
       <c r="F131" s="41" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="G131" s="41" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="H131" s="41" t="s">
-        <v>635</v>
-      </c>
-      <c r="I131" s="42"/>
+        <v>631</v>
+      </c>
+      <c r="I131" s="42" t="s">
+        <v>741</v>
+      </c>
       <c r="J131" s="43" t="s">
         <v>66</v>
       </c>
@@ -10673,7 +10937,7 @@
         <v>267</v>
       </c>
       <c r="O131" s="43" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="P131" s="43" t="s">
         <v>66</v>
@@ -10685,7 +10949,7 @@
         <v>66</v>
       </c>
       <c r="S131" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T131" s="43"/>
       <c r="U131" s="44"/>
@@ -10711,15 +10975,17 @@
         <v>391</v>
       </c>
       <c r="F132" s="41" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="G132" s="41" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="H132" s="41" t="s">
-        <v>638</v>
-      </c>
-      <c r="I132" s="42"/>
+        <v>634</v>
+      </c>
+      <c r="I132" s="42" t="s">
+        <v>742</v>
+      </c>
       <c r="J132" s="43" t="s">
         <v>66</v>
       </c>
@@ -10732,7 +10998,7 @@
         <v>267</v>
       </c>
       <c r="O132" s="43" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="P132" s="43" t="s">
         <v>66</v>
@@ -10744,7 +11010,7 @@
         <v>66</v>
       </c>
       <c r="S132" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T132" s="43"/>
       <c r="U132" s="44"/>
@@ -10770,15 +11036,17 @@
         <v>392</v>
       </c>
       <c r="F133" s="41" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="G133" s="41" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="H133" s="41" t="s">
-        <v>641</v>
-      </c>
-      <c r="I133" s="42"/>
+        <v>637</v>
+      </c>
+      <c r="I133" s="42" t="s">
+        <v>743</v>
+      </c>
       <c r="J133" s="43" t="s">
         <v>66</v>
       </c>
@@ -10791,7 +11059,7 @@
         <v>267</v>
       </c>
       <c r="O133" s="43" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="P133" s="43" t="s">
         <v>66</v>
@@ -10803,7 +11071,7 @@
         <v>66</v>
       </c>
       <c r="S133" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T133" s="43"/>
       <c r="U133" s="44"/>
@@ -10829,15 +11097,17 @@
         <v>393</v>
       </c>
       <c r="F134" s="41" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="G134" s="41" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="H134" s="41" t="s">
-        <v>643</v>
-      </c>
-      <c r="I134" s="42"/>
+        <v>639</v>
+      </c>
+      <c r="I134" s="42" t="s">
+        <v>744</v>
+      </c>
       <c r="J134" s="43" t="s">
         <v>66</v>
       </c>
@@ -10850,7 +11120,7 @@
         <v>267</v>
       </c>
       <c r="O134" s="43" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="P134" s="43" t="s">
         <v>66</v>
@@ -10862,7 +11132,7 @@
         <v>66</v>
       </c>
       <c r="S134" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T134" s="43"/>
       <c r="U134" s="44"/>
@@ -10888,15 +11158,17 @@
         <v>394</v>
       </c>
       <c r="F135" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G135" s="41" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="H135" s="41" t="s">
-        <v>661</v>
-      </c>
-      <c r="I135" s="42"/>
+        <v>657</v>
+      </c>
+      <c r="I135" s="42" t="s">
+        <v>745</v>
+      </c>
       <c r="J135" s="43" t="s">
         <v>66</v>
       </c>
@@ -10909,7 +11181,7 @@
         <v>267</v>
       </c>
       <c r="O135" s="43" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="P135" s="43" t="s">
         <v>66</v>
@@ -10921,7 +11193,7 @@
         <v>66</v>
       </c>
       <c r="S135" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T135" s="43"/>
       <c r="U135" s="44"/>
@@ -10947,15 +11219,17 @@
         <v>395</v>
       </c>
       <c r="F136" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G136" s="41" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="H136" s="41" t="s">
-        <v>664</v>
-      </c>
-      <c r="I136" s="42"/>
+        <v>660</v>
+      </c>
+      <c r="I136" s="42" t="s">
+        <v>746</v>
+      </c>
       <c r="J136" s="43" t="s">
         <v>66</v>
       </c>
@@ -10968,7 +11242,7 @@
         <v>267</v>
       </c>
       <c r="O136" s="43" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="P136" s="43" t="s">
         <v>66</v>
@@ -10980,7 +11254,7 @@
         <v>66</v>
       </c>
       <c r="S136" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T136" s="43"/>
       <c r="U136" s="44"/>
@@ -11006,15 +11280,17 @@
         <v>217</v>
       </c>
       <c r="F137" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G137" s="41" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="H137" s="41" t="s">
-        <v>666</v>
-      </c>
-      <c r="I137" s="42"/>
+        <v>662</v>
+      </c>
+      <c r="I137" s="42" t="s">
+        <v>747</v>
+      </c>
       <c r="J137" s="43" t="s">
         <v>66</v>
       </c>
@@ -11027,7 +11303,7 @@
         <v>267</v>
       </c>
       <c r="O137" s="43" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="P137" s="43" t="s">
         <v>66</v>
@@ -11039,7 +11315,7 @@
         <v>66</v>
       </c>
       <c r="S137" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T137" s="43"/>
       <c r="U137" s="44"/>
@@ -11065,15 +11341,17 @@
         <v>219</v>
       </c>
       <c r="F138" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G138" s="41" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="H138" s="41" t="s">
-        <v>669</v>
-      </c>
-      <c r="I138" s="42"/>
+        <v>665</v>
+      </c>
+      <c r="I138" s="42" t="s">
+        <v>748</v>
+      </c>
       <c r="J138" s="43" t="s">
         <v>66</v>
       </c>
@@ -11086,7 +11364,7 @@
         <v>267</v>
       </c>
       <c r="O138" s="43" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="P138" s="43" t="s">
         <v>66</v>
@@ -11098,7 +11376,7 @@
         <v>66</v>
       </c>
       <c r="S138" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T138" s="43"/>
       <c r="U138" s="44"/>
@@ -11124,15 +11402,17 @@
         <v>324</v>
       </c>
       <c r="F139" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G139" s="41" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="H139" s="41" t="s">
-        <v>673</v>
-      </c>
-      <c r="I139" s="42"/>
+        <v>669</v>
+      </c>
+      <c r="I139" s="42" t="s">
+        <v>749</v>
+      </c>
       <c r="J139" s="43" t="s">
         <v>66</v>
       </c>
@@ -11145,7 +11425,7 @@
         <v>267</v>
       </c>
       <c r="O139" s="43" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="P139" s="43" t="s">
         <v>66</v>
@@ -11157,7 +11437,7 @@
         <v>66</v>
       </c>
       <c r="S139" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T139" s="43"/>
       <c r="U139" s="44"/>
@@ -11183,15 +11463,17 @@
         <v>325</v>
       </c>
       <c r="F140" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G140" s="41" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="H140" s="41" t="s">
-        <v>676</v>
-      </c>
-      <c r="I140" s="42"/>
+        <v>672</v>
+      </c>
+      <c r="I140" s="42" t="s">
+        <v>750</v>
+      </c>
       <c r="J140" s="43" t="s">
         <v>66</v>
       </c>
@@ -11204,7 +11486,7 @@
         <v>267</v>
       </c>
       <c r="O140" s="43" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="P140" s="43" t="s">
         <v>66</v>
@@ -11216,7 +11498,7 @@
         <v>66</v>
       </c>
       <c r="S140" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T140" s="43"/>
       <c r="U140" s="44"/>
@@ -11242,15 +11524,17 @@
         <v>326</v>
       </c>
       <c r="F141" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G141" s="41" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="H141" s="41" t="s">
-        <v>678</v>
-      </c>
-      <c r="I141" s="42"/>
+        <v>674</v>
+      </c>
+      <c r="I141" s="42" t="s">
+        <v>751</v>
+      </c>
       <c r="J141" s="43" t="s">
         <v>66</v>
       </c>
@@ -11263,7 +11547,7 @@
         <v>267</v>
       </c>
       <c r="O141" s="43" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="P141" s="43" t="s">
         <v>66</v>
@@ -11275,7 +11559,7 @@
         <v>66</v>
       </c>
       <c r="S141" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T141" s="43"/>
       <c r="U141" s="44"/>
@@ -11301,15 +11585,17 @@
         <v>327</v>
       </c>
       <c r="F142" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G142" s="41" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="H142" s="41" t="s">
-        <v>680</v>
-      </c>
-      <c r="I142" s="42"/>
+        <v>676</v>
+      </c>
+      <c r="I142" s="42" t="s">
+        <v>752</v>
+      </c>
       <c r="J142" s="43" t="s">
         <v>66</v>
       </c>
@@ -11322,7 +11608,7 @@
         <v>267</v>
       </c>
       <c r="O142" s="43" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="P142" s="43" t="s">
         <v>66</v>
@@ -11334,7 +11620,7 @@
         <v>66</v>
       </c>
       <c r="S142" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T142" s="43"/>
       <c r="U142" s="44"/>
@@ -11360,15 +11646,17 @@
         <v>328</v>
       </c>
       <c r="F143" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G143" s="41" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="H143" s="41" t="s">
-        <v>683</v>
-      </c>
-      <c r="I143" s="42"/>
+        <v>679</v>
+      </c>
+      <c r="I143" s="42" t="s">
+        <v>753</v>
+      </c>
       <c r="J143" s="43" t="s">
         <v>66</v>
       </c>
@@ -11381,7 +11669,7 @@
         <v>267</v>
       </c>
       <c r="O143" s="43" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="P143" s="43" t="s">
         <v>66</v>
@@ -11393,7 +11681,7 @@
         <v>66</v>
       </c>
       <c r="S143" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T143" s="43"/>
       <c r="U143" s="44"/>
@@ -11419,15 +11707,17 @@
         <v>329</v>
       </c>
       <c r="F144" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G144" s="41" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="H144" s="41" t="s">
-        <v>686</v>
-      </c>
-      <c r="I144" s="42"/>
+        <v>682</v>
+      </c>
+      <c r="I144" s="42" t="s">
+        <v>754</v>
+      </c>
       <c r="J144" s="43" t="s">
         <v>66</v>
       </c>
@@ -11440,7 +11730,7 @@
         <v>267</v>
       </c>
       <c r="O144" s="43" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="P144" s="43" t="s">
         <v>66</v>
@@ -11452,7 +11742,7 @@
         <v>66</v>
       </c>
       <c r="S144" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T144" s="43"/>
       <c r="U144" s="44"/>
@@ -11478,15 +11768,17 @@
         <v>330</v>
       </c>
       <c r="F145" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G145" s="41" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="H145" s="41" t="s">
-        <v>689</v>
-      </c>
-      <c r="I145" s="42"/>
+        <v>685</v>
+      </c>
+      <c r="I145" s="42" t="s">
+        <v>755</v>
+      </c>
       <c r="J145" s="43" t="s">
         <v>66</v>
       </c>
@@ -11499,7 +11791,7 @@
         <v>267</v>
       </c>
       <c r="O145" s="43" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="P145" s="43" t="s">
         <v>66</v>
@@ -11511,7 +11803,7 @@
         <v>66</v>
       </c>
       <c r="S145" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T145" s="43"/>
       <c r="U145" s="44"/>
@@ -11537,15 +11829,17 @@
         <v>331</v>
       </c>
       <c r="F146" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G146" s="41" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="H146" s="41" t="s">
-        <v>692</v>
-      </c>
-      <c r="I146" s="42"/>
+        <v>688</v>
+      </c>
+      <c r="I146" s="42" t="s">
+        <v>756</v>
+      </c>
       <c r="J146" s="43" t="s">
         <v>66</v>
       </c>
@@ -11558,7 +11852,7 @@
         <v>267</v>
       </c>
       <c r="O146" s="43" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="P146" s="43" t="s">
         <v>66</v>
@@ -11570,7 +11864,7 @@
         <v>66</v>
       </c>
       <c r="S146" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T146" s="43"/>
       <c r="U146" s="44"/>
@@ -11596,15 +11890,17 @@
         <v>333</v>
       </c>
       <c r="F147" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G147" s="41" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="H147" s="41" t="s">
-        <v>695</v>
-      </c>
-      <c r="I147" s="42"/>
+        <v>691</v>
+      </c>
+      <c r="I147" s="42" t="s">
+        <v>757</v>
+      </c>
       <c r="J147" s="43" t="s">
         <v>66</v>
       </c>
@@ -11617,7 +11913,7 @@
         <v>267</v>
       </c>
       <c r="O147" s="43" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="P147" s="43" t="s">
         <v>66</v>
@@ -11629,7 +11925,7 @@
         <v>66</v>
       </c>
       <c r="S147" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T147" s="43"/>
       <c r="U147" s="44"/>
@@ -11668,7 +11964,7 @@
       <c r="Q148" s="29"/>
       <c r="R148" s="29"/>
       <c r="S148" s="29" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="T148" s="29"/>
       <c r="U148" s="34"/>
@@ -11707,7 +12003,7 @@
       <c r="Q149" s="29"/>
       <c r="R149" s="29"/>
       <c r="S149" s="29" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="T149" s="29"/>
       <c r="U149" s="34"/>
@@ -11745,7 +12041,7 @@
       <c r="P150" s="29"/>
       <c r="Q150" s="29"/>
       <c r="R150" s="29" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="S150" s="29"/>
       <c r="T150" s="29"/>
@@ -11784,7 +12080,7 @@
       <c r="P151" s="29"/>
       <c r="Q151" s="29"/>
       <c r="R151" s="29" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="S151" s="29"/>
       <c r="T151" s="29"/>
@@ -11823,7 +12119,7 @@
       <c r="P152" s="29"/>
       <c r="Q152" s="29"/>
       <c r="R152" s="29" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="S152" s="29"/>
       <c r="T152" s="29"/>
@@ -12277,7 +12573,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="165" spans="1:23" s="46" customFormat="1" ht="110.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:23" s="46" customFormat="1" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="38">
         <v>191</v>
       </c>
@@ -12320,7 +12616,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="166" spans="1:23" s="46" customFormat="1" ht="46.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23" s="46" customFormat="1" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="38">
         <v>376</v>
       </c>
@@ -12363,7 +12659,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="31">
         <v>417</v>
       </c>
@@ -12400,7 +12696,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="31">
         <v>418</v>
       </c>
@@ -12437,7 +12733,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="31">
         <v>419</v>
       </c>
@@ -12992,7 +13288,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="31">
         <v>444</v>
       </c>
@@ -13029,7 +13325,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="31">
         <v>445</v>
       </c>
@@ -13066,7 +13362,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="186" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="38">
         <v>446</v>
       </c>
@@ -13083,16 +13379,16 @@
         <v>321</v>
       </c>
       <c r="F186" s="41" t="s">
+        <v>590</v>
+      </c>
+      <c r="G186" s="41" t="s">
         <v>593</v>
       </c>
-      <c r="G186" s="41" t="s">
-        <v>596</v>
-      </c>
       <c r="H186" s="41" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="I186" s="42" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="J186" s="43" t="s">
         <v>66</v>
@@ -13125,7 +13421,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="187" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="38">
         <v>447</v>
       </c>
@@ -13142,16 +13438,16 @@
         <v>322</v>
       </c>
       <c r="F187" s="41" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="G187" s="41" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H187" s="41" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="I187" s="42" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="J187" s="43" t="s">
         <v>66</v>
@@ -13184,7 +13480,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="38">
         <v>448</v>
       </c>
@@ -13195,22 +13491,22 @@
         <v>51</v>
       </c>
       <c r="D188" s="38" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="E188" s="47" t="s">
         <v>441</v>
       </c>
       <c r="F188" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G188" s="41" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="H188" s="41" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="I188" s="42" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="J188" s="43" t="s">
         <v>66</v>
@@ -13227,12 +13523,14 @@
       <c r="P188" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="Q188" s="43"/>
+      <c r="Q188" s="43" t="s">
+        <v>459</v>
+      </c>
       <c r="R188" s="43" t="s">
         <v>66</v>
       </c>
       <c r="S188" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T188" s="43" t="s">
         <v>265</v>
@@ -13243,7 +13541,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="189" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="38">
         <v>449</v>
       </c>
@@ -13254,22 +13552,22 @@
         <v>51</v>
       </c>
       <c r="D189" s="38" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="E189" s="47" t="s">
         <v>442</v>
       </c>
       <c r="F189" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G189" s="41" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="H189" s="41" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="I189" s="42" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="J189" s="43" t="s">
         <v>66</v>
@@ -13286,12 +13584,14 @@
       <c r="P189" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="Q189" s="43"/>
+      <c r="Q189" s="43" t="s">
+        <v>459</v>
+      </c>
       <c r="R189" s="43" t="s">
         <v>66</v>
       </c>
       <c r="S189" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T189" s="43" t="s">
         <v>265</v>
@@ -13302,7 +13602,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="190" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="38">
         <v>450</v>
       </c>
@@ -13319,16 +13619,16 @@
         <v>427</v>
       </c>
       <c r="F190" s="51" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G190" s="41" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H190" s="41" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="I190" s="42" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="J190" s="43" t="s">
         <v>66</v>
@@ -13357,13 +13657,13 @@
       </c>
       <c r="U190" s="44"/>
       <c r="V190" s="45" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="W190" s="43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="191" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="38">
         <v>451</v>
       </c>
@@ -13380,16 +13680,16 @@
         <v>428</v>
       </c>
       <c r="F191" s="41" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="G191" s="41" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="H191" s="41" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="I191" s="42" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J191" s="43" t="s">
         <v>66</v>
@@ -13422,7 +13722,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="192" spans="1:23" s="46" customFormat="1" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" s="46" customFormat="1" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="38">
         <v>452</v>
       </c>
@@ -13439,16 +13739,16 @@
         <v>422</v>
       </c>
       <c r="F192" s="41" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G192" s="41" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="H192" s="41" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="I192" s="42" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="J192" s="43" t="s">
         <v>66</v>
@@ -13477,13 +13777,13 @@
       </c>
       <c r="U192" s="44"/>
       <c r="V192" s="45" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="W192" s="43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="193" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="31">
         <v>454</v>
       </c>
@@ -13520,7 +13820,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="194" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="31">
         <v>455</v>
       </c>
@@ -13557,7 +13857,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="195" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="31">
         <v>456</v>
       </c>
@@ -13594,7 +13894,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="196" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="31">
         <v>457</v>
       </c>
@@ -13631,7 +13931,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="197" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="31">
         <v>458</v>
       </c>
@@ -13668,7 +13968,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="198" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="31">
         <v>459</v>
       </c>
@@ -13705,7 +14005,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="199" spans="1:23" ht="182.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:23" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="31">
         <v>460</v>
       </c>
@@ -13759,15 +14059,17 @@
         <v>443</v>
       </c>
       <c r="F200" s="41" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="G200" s="41" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="H200" s="41" t="s">
-        <v>698</v>
-      </c>
-      <c r="I200" s="42"/>
+        <v>694</v>
+      </c>
+      <c r="I200" s="42" t="s">
+        <v>758</v>
+      </c>
       <c r="J200" s="43" t="s">
         <v>66</v>
       </c>
@@ -13780,7 +14082,7 @@
         <v>267</v>
       </c>
       <c r="O200" s="43" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="P200" s="43" t="s">
         <v>66</v>
@@ -13792,7 +14094,7 @@
         <v>66</v>
       </c>
       <c r="S200" s="43" t="s">
-        <v>456</v>
+        <v>66</v>
       </c>
       <c r="T200" s="43"/>
       <c r="U200" s="44"/>
@@ -18113,13 +18415,7 @@
       <c r="W770" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:W200" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="22">
-      <filters>
-        <filter val="KO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:W200" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -18140,7 +18436,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J14 M14:N15 J16:J20 S14:S15 J22 J24:J28 M22:N28 M20:N20 M10:N12 J10:J12 S19:S20 J30:J198 M16:M20 N16:N19 P22:R28 P200:R200 M200:N200 M30:N198 P30:R198 S35:S76 S22:S23 P14:R20 S11:S12 P10:R12</xm:sqref>
+          <xm:sqref>J14 M14:N15 J16:J20 S14:S15 J22 J24:J28 M22:N28 M20:N20 M10:N12 J10:J12 S19:S20 J30:J198 M16:M20 N16:N19 P22:R28 P200:S200 M200:N200 M30:N198 S188:S189 S35:S76 S22:S23 P14:R20 S11:S12 P10:R12 S27 S30:S31 S130:S147 P30:R198</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
@@ -20399,6 +20695,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F560B38A5B3C4B41B1895754B1F1A56A" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="69dc0f489d46816a4b9bb4a327e14425">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca719f03-9e45-4ef4-9920-d156f53157f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7de9a44ff87fdcabda187bbd662e75de" ns2:_="">
     <xsd:import namespace="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
@@ -20570,26 +20885,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20607,32 +20929,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
fix test 447. 450, 452
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD23209-8152-4A31-9D76-C7EBA95B9A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1E5CBD-C4CD-4F1D-97A5-851648DD8BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="767">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2638,30 +2638,6 @@
     <t>2025-04-02'</t>
   </si>
   <si>
-    <t>{"Id":"3fa85f64-5717-4562-b3fc-2c963f66afa6","Data":"2025-04-02T13:39:01.9566538Z","Status":200,"TraceID":"1fb3a04feeffdb29","SpanID":"1fb3a04feeffdb29","Warning":"[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell\u0027elemento observation/code.--\u003E ],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell\u0027elemento observation/code.--\u003E ]","WorkflowInstanceId":"2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.fc5a916ec6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId","Type":null,"Title":null,"Detail":null,"Instance":null}</t>
-  </si>
-  <si>
-    <t>1fb3a04feeffdb29</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.fc5a916ec6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-04-02T13:39:01</t>
-  </si>
-  <si>
-    <t>{"Id":"3fa85f64-5717-4562-b3fc-2c963f66afa6","Data":"2025-04-02T13:54:31.1302595Z","Status":200,"TraceID":"e97b2691ab8fe48b","SpanID":"e97b2691ab8fe48b","Warning":null,"WorkflowInstanceId":"2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.5c1599d08a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId","Type":null,"Title":null,"Detail":null,"Instance":null}</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.5c1599d08a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e97b2691ab8fe48b</t>
-  </si>
-  <si>
-    <t>2025-04-02T13:54:31</t>
-  </si>
-  <si>
     <t>{"Id":"3fa85f64-5717-4562-b3fc-2c963f66afa6","Data":"2025-04-02T14:09:16.4064092Z","Status":200,"TraceID":"9e51dd7d2a0b1074","SpanID":"9e51dd7d2a0b1074","Warning":null,"WorkflowInstanceId":"2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.6ec3678389^^^^urn:ihe:iti:xdw:2013:workflowInstanceId","Type":null,"Title":null,"Detail":null,"Instance":null}</t>
   </si>
   <si>
@@ -2674,18 +2650,6 @@
     <t>2025-04-02T14:09:16</t>
   </si>
   <si>
-    <t>{"Id":"3fa85f64-5717-4562-b3fc-2c963f66afa6","Data":"2025-04-02T14:12:37.9291191Z","Status":200,"TraceID":"1f0335f6859bf3d1","SpanID":"1f0335f6859bf3d1","Warning":null,"WorkflowInstanceId":"2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.b77d2e35a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId","Type":null,"Title":null,"Detail":null,"Instance":null}</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.b77d2e35a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>1f0335f6859bf3d1</t>
-  </si>
-  <si>
-    <t>2025-04-02T14:12:37</t>
-  </si>
-  <si>
     <t>{"Id":"3fa85f64-5717-4562-b3fc-2c963f66afa6","Data":"2025-04-02T14:24:03.2284187Z","Status":200,"TraceID":"463d087d85bfbb44","SpanID":"463d087d85bfbb44","Warning":null,"WorkflowInstanceId":"2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.485294cf57^^^^urn:ihe:iti:xdw:2013:workflowInstanceId","Type":null,"Title":null,"Detail":null,"Instance":null}</t>
   </si>
   <si>
@@ -2708,6 +2672,45 @@
   </si>
   <si>
     <t>2025-04-02T14:25:49</t>
+  </si>
+  <si>
+    <t>{"Id":"3fa85f64-5717-4562-b3fc-2c963f66afa6","Data":"2025-04-09T11:00:59.351088Z","Status":200,"TraceID":"31310e8fb964d9ff","SpanID":"31310e8fb964d9ff","Warning":null,"WorkflowInstanceId":"2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.6517c0e57c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId","Type":null,"Title":null,"Detail":null,"Instance":null}</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.9775d4755922a02be22628a922930747e212bcc8e434d70e2a8fef03d550e655.6517c0e57c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>31310e8fb964d9ff</t>
+  </si>
+  <si>
+    <t>2025-04-09T11:00:59</t>
+  </si>
+  <si>
+    <t>2025-04-09'</t>
+  </si>
+  <si>
+    <t>{"Id":"3fa85f64-5717-4562-b3fc-2c963f66afa6","Data":"2025-04-09T11:08:21.1203919Z","Status":200,"TraceID":"e63e2fa8328e6d5a","SpanID":"e63e2fa8328e6d5a","Warning":null,"WorkflowInstanceId":"2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.b3e5f84bfd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId","Type":null,"Title":null,"Detail":null,"Instance":null}</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.b3e5f84bfd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e63e2fa8328e6d5a</t>
+  </si>
+  <si>
+    <t>2025-04-09T11:08:21</t>
+  </si>
+  <si>
+    <t>{"Id":"3fa85f64-5717-4562-b3fc-2c963f66afa6","Data":"2025-04-09T12:56:01.0221432Z","Status":200,"TraceID":"942f5df6d98ac5e2480eaa9a1ed890c3","SpanID":"b1cedd08751bf45d","Warning":"[W002 | Si consiglia di valorizzare l\u0027elemento organizer[CLUSTER]/code]","WorkflowInstanceId":"2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.f47370cc54^^^^urn:ihe:iti:xdw:2013:workflowInstanceId","Type":null,"Title":null,"Detail":null,"Instance":null}</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.f47370cc54^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>942f5df6d98ac5e2480eaa9a1ed890c3</t>
+  </si>
+  <si>
+    <t>2025-04-09T12:56:01</t>
   </si>
 </sst>
 </file>
@@ -4802,7 +4805,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G189" sqref="G189:I189"/>
+      <selection pane="bottomRight" activeCell="G192" sqref="G192:I192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13400,13 +13403,13 @@
         <v>741</v>
       </c>
       <c r="G186" s="41" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="H186" s="41" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
       <c r="I186" s="42" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
       <c r="J186" s="43" t="s">
         <v>66</v>
@@ -13435,7 +13438,7 @@
       </c>
       <c r="U186" s="44"/>
       <c r="V186" s="45" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="W186" s="43" t="s">
         <v>36</v>
@@ -13458,16 +13461,16 @@
         <v>322</v>
       </c>
       <c r="F187" s="41" t="s">
-        <v>741</v>
+        <v>758</v>
       </c>
       <c r="G187" s="41" t="s">
-        <v>757</v>
+        <v>762</v>
       </c>
       <c r="H187" s="41" t="s">
-        <v>756</v>
+        <v>761</v>
       </c>
       <c r="I187" s="42" t="s">
-        <v>755</v>
+        <v>760</v>
       </c>
       <c r="J187" s="43" t="s">
         <v>66</v>
@@ -13496,7 +13499,7 @@
       </c>
       <c r="U187" s="44"/>
       <c r="V187" s="45" t="s">
-        <v>754</v>
+        <v>759</v>
       </c>
       <c r="W187" s="43" t="s">
         <v>36</v>
@@ -13522,13 +13525,13 @@
         <v>741</v>
       </c>
       <c r="G188" s="41" t="s">
-        <v>761</v>
+        <v>749</v>
       </c>
       <c r="H188" s="41" t="s">
-        <v>760</v>
+        <v>748</v>
       </c>
       <c r="I188" s="42" t="s">
-        <v>759</v>
+        <v>747</v>
       </c>
       <c r="J188" s="43" t="s">
         <v>66</v>
@@ -13559,7 +13562,7 @@
       </c>
       <c r="U188" s="44"/>
       <c r="V188" s="45" t="s">
-        <v>758</v>
+        <v>746</v>
       </c>
       <c r="W188" s="43" t="s">
         <v>36</v>
@@ -13585,13 +13588,13 @@
         <v>741</v>
       </c>
       <c r="G189" s="41" t="s">
-        <v>765</v>
+        <v>753</v>
       </c>
       <c r="H189" s="41" t="s">
-        <v>764</v>
+        <v>752</v>
       </c>
       <c r="I189" s="42" t="s">
-        <v>763</v>
+        <v>751</v>
       </c>
       <c r="J189" s="43" t="s">
         <v>66</v>
@@ -13622,7 +13625,7 @@
       </c>
       <c r="U189" s="44"/>
       <c r="V189" s="45" t="s">
-        <v>762</v>
+        <v>750</v>
       </c>
       <c r="W189" s="43" t="s">
         <v>36</v>
@@ -13645,16 +13648,16 @@
         <v>427</v>
       </c>
       <c r="F190" s="51" t="s">
-        <v>741</v>
+        <v>758</v>
       </c>
       <c r="G190" s="41" t="s">
-        <v>749</v>
+        <v>757</v>
       </c>
       <c r="H190" s="41" t="s">
-        <v>748</v>
+        <v>756</v>
       </c>
       <c r="I190" s="42" t="s">
-        <v>747</v>
+        <v>755</v>
       </c>
       <c r="J190" s="43" t="s">
         <v>66</v>
@@ -13683,7 +13686,7 @@
       </c>
       <c r="U190" s="44"/>
       <c r="V190" s="45" t="s">
-        <v>746</v>
+        <v>754</v>
       </c>
       <c r="W190" s="43" t="s">
         <v>36</v>
@@ -13765,16 +13768,16 @@
         <v>422</v>
       </c>
       <c r="F192" s="41" t="s">
-        <v>741</v>
+        <v>758</v>
       </c>
       <c r="G192" s="41" t="s">
-        <v>745</v>
+        <v>766</v>
       </c>
       <c r="H192" s="41" t="s">
-        <v>743</v>
+        <v>765</v>
       </c>
       <c r="I192" s="42" t="s">
-        <v>744</v>
+        <v>764</v>
       </c>
       <c r="J192" s="43" t="s">
         <v>66</v>
@@ -13803,7 +13806,7 @@
       </c>
       <c r="U192" s="44"/>
       <c r="V192" s="45" t="s">
-        <v>742</v>
+        <v>763</v>
       </c>
       <c r="W192" s="43" t="s">
         <v>36</v>
@@ -20721,6 +20724,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F560B38A5B3C4B41B1895754B1F1A56A" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="69dc0f489d46816a4b9bb4a327e14425">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca719f03-9e45-4ef4-9920-d156f53157f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7de9a44ff87fdcabda187bbd662e75de" ns2:_="">
     <xsd:import namespace="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
@@ -20892,26 +20914,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20929,32 +20958,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
fix test 452 LAB -> 452_VALIDAZIONE_CDA2_LAB_CT17
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1E5CBD-C4CD-4F1D-97A5-851648DD8BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6516D87C-8782-4826-811E-92F2B45E5B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="768">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2701,16 +2701,19 @@
     <t>2025-04-09T11:08:21</t>
   </si>
   <si>
-    <t>{"Id":"3fa85f64-5717-4562-b3fc-2c963f66afa6","Data":"2025-04-09T12:56:01.0221432Z","Status":200,"TraceID":"942f5df6d98ac5e2480eaa9a1ed890c3","SpanID":"b1cedd08751bf45d","Warning":"[W002 | Si consiglia di valorizzare l\u0027elemento organizer[CLUSTER]/code]","WorkflowInstanceId":"2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.f47370cc54^^^^urn:ihe:iti:xdw:2013:workflowInstanceId","Type":null,"Title":null,"Detail":null,"Instance":null}</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.f47370cc54^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>942f5df6d98ac5e2480eaa9a1ed890c3</t>
-  </si>
-  <si>
-    <t>2025-04-09T12:56:01</t>
+    <t>{"Id":"3fa85f64-5717-4562-b3fc-2c963f66afa6","Data":"2025-04-15T09:46:51.2724069Z","Status":200,"TraceID":"a0805cb94e17bf1a39622289fb29c494","SpanID":"0d0f38c34cd6f4c9","Warning":"[W002 | Si consiglia di valorizzare l\u0027elemento organizer[CLUSTER]/code]","WorkflowInstanceId":"2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.f547a6bc7c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId","Type":null,"Title":null,"Detail":null,"Instance":null}</t>
+  </si>
+  <si>
+    <t>a0805cb94e17bf1a39622289fb29c494</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.f547a6bc7c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-04-15T09:46:51</t>
+  </si>
+  <si>
+    <t>2025-04-15'</t>
   </si>
 </sst>
 </file>
@@ -4802,10 +4805,10 @@
   <dimension ref="A1:W770"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="M191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G192" sqref="G192:I192"/>
+      <selection pane="bottomRight" activeCell="U192" sqref="U192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13768,16 +13771,16 @@
         <v>422</v>
       </c>
       <c r="F192" s="41" t="s">
-        <v>758</v>
+        <v>767</v>
       </c>
       <c r="G192" s="41" t="s">
         <v>766</v>
       </c>
       <c r="H192" s="41" t="s">
+        <v>764</v>
+      </c>
+      <c r="I192" s="42" t="s">
         <v>765</v>
-      </c>
-      <c r="I192" s="42" t="s">
-        <v>764</v>
       </c>
       <c r="J192" s="43" t="s">
         <v>66</v>
@@ -20724,25 +20727,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F560B38A5B3C4B41B1895754B1F1A56A" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="69dc0f489d46816a4b9bb4a327e14425">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca719f03-9e45-4ef4-9920-d156f53157f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7de9a44ff87fdcabda187bbd662e75de" ns2:_="">
     <xsd:import namespace="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
@@ -20914,7 +20898,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -20932,32 +20961,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
rifacimento di tutti i test su richiesta di FSE
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9F8EB7-680D-4EDB-BBE3-830E27013F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FFED0F-84A3-46AC-B2B0-923027DB13A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2109" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="820">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1782,9 +1782,6 @@
   </si>
   <si>
     <t>Il referto con il rispettivo errore, saranno inseriti in una coda di verifica. Tale coda sarà  accessibile dal ced della struttura mediante un cruscotto di monitoraggio messo a disposizione  ed avrà la possibilità di verificare i diversi errori ed apportare le modifiche e correzioni necessarie. A seguito di tali correzioni indicati mediante il cambio di stato del documento stesso, sarà possibile sottoporre di nuovo il documento al processi di validazione del gateway.</t>
-  </si>
-  <si>
-    <t>AuthorizationContentDeny</t>
   </si>
   <si>
     <t>{"Error calling Validate: {\"traceID\":\"ff8586b7e90570d2\",\"spanID\":\"ff8586b7e90570d2\",\"type\":\"/msg/jwt-validation\",\"title\":\"Campo token JWT non valido.\",\"detail\":\"Il campo action_id non è corretto\",\"status\":403,\"instance\":\"/jwt-mandatory-field-malformed\",\"workflowInstanceId\":\"UNKNOWN_WORKFLOW_ID\"}"}</t>
@@ -5656,10 +5653,10 @@
   <dimension ref="A1:W770"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F200" sqref="F200"/>
+      <selection pane="bottomRight" activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5959,16 +5956,16 @@
         <v>424</v>
       </c>
       <c r="F10" s="50" t="s">
+        <v>545</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>544</v>
+      </c>
+      <c r="H10" s="50" t="s">
         <v>546</v>
       </c>
-      <c r="G10" s="50" t="s">
-        <v>545</v>
-      </c>
-      <c r="H10" s="50" t="s">
+      <c r="I10" s="50" t="s">
         <v>547</v>
-      </c>
-      <c r="I10" s="50" t="s">
-        <v>548</v>
       </c>
       <c r="J10" s="43" t="s">
         <v>66</v>
@@ -5997,7 +5994,7 @@
       </c>
       <c r="U10" s="44"/>
       <c r="V10" s="50" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="W10" s="43" t="s">
         <v>36</v>
@@ -6037,7 +6034,7 @@
         <v>267</v>
       </c>
       <c r="O11" s="43" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="P11" s="43" t="s">
         <v>66</v>
@@ -6053,9 +6050,7 @@
       </c>
       <c r="T11" s="43"/>
       <c r="U11" s="44"/>
-      <c r="V11" s="45" t="s">
-        <v>458</v>
-      </c>
+      <c r="V11" s="45"/>
       <c r="W11" s="43" t="s">
         <v>46</v>
       </c>
@@ -6094,7 +6089,7 @@
         <v>267</v>
       </c>
       <c r="O12" s="43" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="P12" s="43" t="s">
         <v>66</v>
@@ -6186,7 +6181,7 @@
         <v>267</v>
       </c>
       <c r="O14" s="43" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="P14" s="43" t="s">
         <v>66</v>
@@ -6241,7 +6236,7 @@
         <v>267</v>
       </c>
       <c r="O15" s="43" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="P15" s="43" t="s">
         <v>66</v>
@@ -6407,7 +6402,7 @@
         <v>267</v>
       </c>
       <c r="O19" s="43" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="P19" s="43" t="s">
         <v>66</v>
@@ -6424,7 +6419,7 @@
       <c r="T19" s="43"/>
       <c r="U19" s="44"/>
       <c r="V19" s="45" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="W19" s="43" t="s">
         <v>46</v>
@@ -6464,7 +6459,7 @@
         <v>267</v>
       </c>
       <c r="O20" s="43" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="P20" s="43" t="s">
         <v>66</v>
@@ -6555,7 +6550,7 @@
         <v>267</v>
       </c>
       <c r="O22" s="43" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="P22" s="43" t="s">
         <v>66</v>
@@ -6610,7 +6605,7 @@
         <v>267</v>
       </c>
       <c r="O23" s="43" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="P23" s="43" t="s">
         <v>66</v>
@@ -6769,7 +6764,7 @@
         <v>278</v>
       </c>
       <c r="L27" s="43" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="M27" s="43" t="s">
         <v>66</v>
@@ -6828,7 +6823,7 @@
         <v>278</v>
       </c>
       <c r="L28" s="43" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="M28" s="43" t="s">
         <v>66</v>
@@ -6926,7 +6921,7 @@
         <v>278</v>
       </c>
       <c r="L30" s="43" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="M30" s="43" t="s">
         <v>66</v>
@@ -6985,7 +6980,7 @@
         <v>278</v>
       </c>
       <c r="L31" s="43" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="M31" s="43" t="s">
         <v>66</v>
@@ -7151,16 +7146,16 @@
         <v>75</v>
       </c>
       <c r="F35" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G35" s="41" t="s">
+        <v>550</v>
+      </c>
+      <c r="H35" s="41" t="s">
+        <v>549</v>
+      </c>
+      <c r="I35" s="42" t="s">
         <v>551</v>
-      </c>
-      <c r="H35" s="41" t="s">
-        <v>550</v>
-      </c>
-      <c r="I35" s="42" t="s">
-        <v>552</v>
       </c>
       <c r="J35" s="43" t="s">
         <v>66</v>
@@ -7191,7 +7186,7 @@
       <c r="T35" s="43"/>
       <c r="U35" s="44"/>
       <c r="V35" s="45" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="W35" s="43" t="s">
         <v>46</v>
@@ -7214,16 +7209,16 @@
         <v>77</v>
       </c>
       <c r="F36" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G36" s="41" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H36" s="41" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I36" s="42" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J36" s="43" t="s">
         <v>66</v>
@@ -7237,7 +7232,7 @@
         <v>267</v>
       </c>
       <c r="O36" s="43" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="P36" s="43" t="s">
         <v>66</v>
@@ -7254,7 +7249,7 @@
       <c r="T36" s="43"/>
       <c r="U36" s="44"/>
       <c r="V36" s="45" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="W36" s="43" t="s">
         <v>46</v>
@@ -7277,16 +7272,16 @@
         <v>79</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G37" s="41" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H37" s="41" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I37" s="42" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J37" s="43" t="s">
         <v>66</v>
@@ -7300,7 +7295,7 @@
         <v>267</v>
       </c>
       <c r="O37" s="43" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="P37" s="43" t="s">
         <v>66</v>
@@ -7317,7 +7312,7 @@
       <c r="T37" s="43"/>
       <c r="U37" s="44"/>
       <c r="V37" s="45" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="W37" s="43" t="s">
         <v>46</v>
@@ -7340,16 +7335,16 @@
         <v>81</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G38" s="41" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H38" s="41" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I38" s="42" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="J38" s="43" t="s">
         <v>66</v>
@@ -7363,7 +7358,7 @@
         <v>267</v>
       </c>
       <c r="O38" s="43" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="P38" s="43" t="s">
         <v>66</v>
@@ -7380,7 +7375,7 @@
       <c r="T38" s="43"/>
       <c r="U38" s="44"/>
       <c r="V38" s="45" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="W38" s="43" t="s">
         <v>46</v>
@@ -7403,16 +7398,16 @@
         <v>83</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G39" s="41" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H39" s="41" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I39" s="42" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="J39" s="43" t="s">
         <v>66</v>
@@ -7426,7 +7421,7 @@
         <v>267</v>
       </c>
       <c r="O39" s="43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="P39" s="43" t="s">
         <v>66</v>
@@ -7443,7 +7438,7 @@
       <c r="T39" s="43"/>
       <c r="U39" s="44"/>
       <c r="V39" s="45" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="W39" s="43" t="s">
         <v>46</v>
@@ -7466,16 +7461,16 @@
         <v>85</v>
       </c>
       <c r="F40" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G40" s="41" t="s">
+        <v>569</v>
+      </c>
+      <c r="H40" s="41" t="s">
         <v>570</v>
       </c>
-      <c r="H40" s="41" t="s">
-        <v>571</v>
-      </c>
       <c r="I40" s="42" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="J40" s="43" t="s">
         <v>66</v>
@@ -7489,7 +7484,7 @@
         <v>267</v>
       </c>
       <c r="O40" s="43" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="P40" s="43" t="s">
         <v>66</v>
@@ -7506,7 +7501,7 @@
       <c r="T40" s="43"/>
       <c r="U40" s="44"/>
       <c r="V40" s="45" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="W40" s="43" t="s">
         <v>46</v>
@@ -7529,16 +7524,16 @@
         <v>87</v>
       </c>
       <c r="F41" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G41" s="41" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H41" s="41" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I41" s="42" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="J41" s="43" t="s">
         <v>66</v>
@@ -7552,7 +7547,7 @@
         <v>267</v>
       </c>
       <c r="O41" s="43" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P41" s="43" t="s">
         <v>66</v>
@@ -7569,7 +7564,7 @@
       <c r="T41" s="43"/>
       <c r="U41" s="44"/>
       <c r="V41" s="45" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="W41" s="43" t="s">
         <v>46</v>
@@ -7592,16 +7587,16 @@
         <v>89</v>
       </c>
       <c r="F42" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G42" s="41" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H42" s="41" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I42" s="42" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J42" s="43" t="s">
         <v>66</v>
@@ -7615,7 +7610,7 @@
         <v>267</v>
       </c>
       <c r="O42" s="43" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="P42" s="43" t="s">
         <v>66</v>
@@ -7632,7 +7627,7 @@
       <c r="T42" s="43"/>
       <c r="U42" s="44"/>
       <c r="V42" s="45" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="W42" s="43" t="s">
         <v>46</v>
@@ -7655,16 +7650,16 @@
         <v>91</v>
       </c>
       <c r="F43" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G43" s="41" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H43" s="41" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I43" s="42" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J43" s="43" t="s">
         <v>66</v>
@@ -7678,7 +7673,7 @@
         <v>267</v>
       </c>
       <c r="O43" s="43" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="P43" s="43" t="s">
         <v>66</v>
@@ -7695,7 +7690,7 @@
       <c r="T43" s="43"/>
       <c r="U43" s="44"/>
       <c r="V43" s="45" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="W43" s="43" t="s">
         <v>46</v>
@@ -7718,16 +7713,16 @@
         <v>93</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G44" s="41" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H44" s="41" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I44" s="42" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J44" s="43" t="s">
         <v>66</v>
@@ -7741,7 +7736,7 @@
         <v>267</v>
       </c>
       <c r="O44" s="43" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="P44" s="43" t="s">
         <v>66</v>
@@ -7757,10 +7752,10 @@
       </c>
       <c r="T44" s="43"/>
       <c r="U44" s="44" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="V44" s="45" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="W44" s="43" t="s">
         <v>46</v>
@@ -7783,16 +7778,16 @@
         <v>95</v>
       </c>
       <c r="F45" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G45" s="41" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="H45" s="41" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I45" s="42" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J45" s="43" t="s">
         <v>66</v>
@@ -7822,10 +7817,10 @@
       </c>
       <c r="T45" s="43"/>
       <c r="U45" s="44" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="V45" s="45" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="W45" s="43" t="s">
         <v>46</v>
@@ -7848,16 +7843,16 @@
         <v>338</v>
       </c>
       <c r="F46" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G46" s="41" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H46" s="41" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I46" s="42" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="J46" s="43" t="s">
         <v>66</v>
@@ -7871,7 +7866,7 @@
         <v>267</v>
       </c>
       <c r="O46" s="43" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="P46" s="43" t="s">
         <v>66</v>
@@ -7887,10 +7882,10 @@
       </c>
       <c r="T46" s="43"/>
       <c r="U46" s="44" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="V46" s="45" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="W46" s="43" t="s">
         <v>46</v>
@@ -7913,16 +7908,16 @@
         <v>340</v>
       </c>
       <c r="F47" s="51" t="s">
+        <v>600</v>
+      </c>
+      <c r="G47" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="H47" s="41" t="s">
+        <v>602</v>
+      </c>
+      <c r="I47" s="42" t="s">
         <v>601</v>
-      </c>
-      <c r="G47" s="41" t="s">
-        <v>604</v>
-      </c>
-      <c r="H47" s="41" t="s">
-        <v>603</v>
-      </c>
-      <c r="I47" s="42" t="s">
-        <v>602</v>
       </c>
       <c r="J47" s="43" t="s">
         <v>66</v>
@@ -7936,7 +7931,7 @@
         <v>267</v>
       </c>
       <c r="O47" s="43" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="P47" s="43" t="s">
         <v>66</v>
@@ -7952,10 +7947,10 @@
       </c>
       <c r="T47" s="43"/>
       <c r="U47" s="44" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="V47" s="45" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="W47" s="43" t="s">
         <v>46</v>
@@ -7978,16 +7973,16 @@
         <v>339</v>
       </c>
       <c r="F48" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G48" s="41" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="H48" s="41" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I48" s="42" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J48" s="43" t="s">
         <v>66</v>
@@ -8001,7 +7996,7 @@
         <v>267</v>
       </c>
       <c r="O48" s="43" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="P48" s="43" t="s">
         <v>66</v>
@@ -8017,10 +8012,10 @@
       </c>
       <c r="T48" s="43"/>
       <c r="U48" s="44" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="V48" s="45" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="W48" s="43" t="s">
         <v>46</v>
@@ -8043,16 +8038,16 @@
         <v>341</v>
       </c>
       <c r="F49" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G49" s="41" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H49" s="41" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I49" s="42" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="J49" s="43" t="s">
         <v>66</v>
@@ -8066,7 +8061,7 @@
         <v>267</v>
       </c>
       <c r="O49" s="43" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="P49" s="43" t="s">
         <v>66</v>
@@ -8082,10 +8077,10 @@
       </c>
       <c r="T49" s="43"/>
       <c r="U49" s="44" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="V49" s="45" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W49" s="43" t="s">
         <v>46</v>
@@ -8108,16 +8103,16 @@
         <v>342</v>
       </c>
       <c r="F50" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G50" s="41" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H50" s="41" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I50" s="42" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="J50" s="43" t="s">
         <v>66</v>
@@ -8131,7 +8126,7 @@
         <v>267</v>
       </c>
       <c r="O50" s="43" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P50" s="43" t="s">
         <v>66</v>
@@ -8147,10 +8142,10 @@
       </c>
       <c r="T50" s="43"/>
       <c r="U50" s="44" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="V50" s="45" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="W50" s="43" t="s">
         <v>46</v>
@@ -8173,16 +8168,16 @@
         <v>343</v>
       </c>
       <c r="F51" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G51" s="41" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="H51" s="41" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I51" s="42" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J51" s="43" t="s">
         <v>66</v>
@@ -8196,7 +8191,7 @@
         <v>267</v>
       </c>
       <c r="O51" s="43" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="P51" s="43" t="s">
         <v>66</v>
@@ -8212,10 +8207,10 @@
       </c>
       <c r="T51" s="43"/>
       <c r="U51" s="44" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="V51" s="45" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="W51" s="43" t="s">
         <v>46</v>
@@ -8238,16 +8233,16 @@
         <v>344</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G52" s="41" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H52" s="41" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I52" s="42" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="J52" s="43" t="s">
         <v>66</v>
@@ -8261,7 +8256,7 @@
         <v>267</v>
       </c>
       <c r="O52" s="43" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="P52" s="43" t="s">
         <v>66</v>
@@ -8277,10 +8272,10 @@
       </c>
       <c r="T52" s="43"/>
       <c r="U52" s="44" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="V52" s="45" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="W52" s="43" t="s">
         <v>46</v>
@@ -8303,16 +8298,16 @@
         <v>345</v>
       </c>
       <c r="F53" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G53" s="41" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H53" s="41" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I53" s="42" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="J53" s="43" t="s">
         <v>66</v>
@@ -8326,7 +8321,7 @@
         <v>267</v>
       </c>
       <c r="O53" s="43" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="P53" s="43" t="s">
         <v>66</v>
@@ -8342,10 +8337,10 @@
       </c>
       <c r="T53" s="43"/>
       <c r="U53" s="44" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="V53" s="45" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="W53" s="43" t="s">
         <v>46</v>
@@ -8368,16 +8363,16 @@
         <v>346</v>
       </c>
       <c r="F54" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G54" s="41" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="H54" s="41" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I54" s="42" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J54" s="43" t="s">
         <v>66</v>
@@ -8391,7 +8386,7 @@
         <v>267</v>
       </c>
       <c r="O54" s="43" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="P54" s="43" t="s">
         <v>66</v>
@@ -8407,10 +8402,10 @@
       </c>
       <c r="T54" s="43"/>
       <c r="U54" s="44" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="V54" s="45" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="W54" s="43" t="s">
         <v>46</v>
@@ -8433,16 +8428,16 @@
         <v>347</v>
       </c>
       <c r="F55" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G55" s="41" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="H55" s="41" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I55" s="42" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="J55" s="43" t="s">
         <v>66</v>
@@ -8456,7 +8451,7 @@
         <v>267</v>
       </c>
       <c r="O55" s="43" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="P55" s="43" t="s">
         <v>66</v>
@@ -8472,10 +8467,10 @@
       </c>
       <c r="T55" s="43"/>
       <c r="U55" s="44" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="V55" s="45" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="W55" s="43" t="s">
         <v>46</v>
@@ -8498,16 +8493,16 @@
         <v>348</v>
       </c>
       <c r="F56" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G56" s="41" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H56" s="41" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I56" s="42" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J56" s="43" t="s">
         <v>66</v>
@@ -8521,7 +8516,7 @@
         <v>267</v>
       </c>
       <c r="O56" s="43" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="P56" s="43" t="s">
         <v>66</v>
@@ -8537,10 +8532,10 @@
       </c>
       <c r="T56" s="43"/>
       <c r="U56" s="44" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="V56" s="45" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="W56" s="43" t="s">
         <v>46</v>
@@ -8563,16 +8558,16 @@
         <v>349</v>
       </c>
       <c r="F57" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G57" s="41" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="H57" s="41" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I57" s="42" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J57" s="43" t="s">
         <v>66</v>
@@ -8586,7 +8581,7 @@
         <v>267</v>
       </c>
       <c r="O57" s="43" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="P57" s="43" t="s">
         <v>66</v>
@@ -8602,10 +8597,10 @@
       </c>
       <c r="T57" s="43"/>
       <c r="U57" s="44" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="V57" s="45" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="W57" s="43" t="s">
         <v>46</v>
@@ -8628,16 +8623,16 @@
         <v>350</v>
       </c>
       <c r="F58" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G58" s="41" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="H58" s="41" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I58" s="42" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J58" s="43" t="s">
         <v>66</v>
@@ -8651,7 +8646,7 @@
         <v>267</v>
       </c>
       <c r="O58" s="43" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="P58" s="43" t="s">
         <v>66</v>
@@ -8667,10 +8662,10 @@
       </c>
       <c r="T58" s="43"/>
       <c r="U58" s="44" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="V58" s="45" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="W58" s="43" t="s">
         <v>46</v>
@@ -8693,16 +8688,16 @@
         <v>351</v>
       </c>
       <c r="F59" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G59" s="41" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="H59" s="41" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I59" s="42" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J59" s="43" t="s">
         <v>66</v>
@@ -8716,7 +8711,7 @@
         <v>267</v>
       </c>
       <c r="O59" s="43" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="P59" s="43" t="s">
         <v>66</v>
@@ -8732,10 +8727,10 @@
       </c>
       <c r="T59" s="43"/>
       <c r="U59" s="44" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="V59" s="45" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="W59" s="43" t="s">
         <v>46</v>
@@ -8758,16 +8753,16 @@
         <v>111</v>
       </c>
       <c r="F60" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G60" s="41" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="H60" s="41" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I60" s="42" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="J60" s="43" t="s">
         <v>66</v>
@@ -8781,7 +8776,7 @@
         <v>267</v>
       </c>
       <c r="O60" s="43" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="P60" s="43" t="s">
         <v>66</v>
@@ -8797,10 +8792,10 @@
       </c>
       <c r="T60" s="43"/>
       <c r="U60" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="V60" s="45" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="W60" s="43" t="s">
         <v>46</v>
@@ -8823,16 +8818,16 @@
         <v>113</v>
       </c>
       <c r="F61" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G61" s="41" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="H61" s="41" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I61" s="42" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J61" s="43" t="s">
         <v>66</v>
@@ -8846,7 +8841,7 @@
         <v>267</v>
       </c>
       <c r="O61" s="43" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="P61" s="43" t="s">
         <v>66</v>
@@ -8862,10 +8857,10 @@
       </c>
       <c r="T61" s="43"/>
       <c r="U61" s="44" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="V61" s="45" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="W61" s="43" t="s">
         <v>46</v>
@@ -8888,16 +8883,16 @@
         <v>352</v>
       </c>
       <c r="F62" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G62" s="41" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="H62" s="41" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I62" s="42" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J62" s="43" t="s">
         <v>66</v>
@@ -8911,7 +8906,7 @@
         <v>267</v>
       </c>
       <c r="O62" s="43" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="P62" s="43" t="s">
         <v>66</v>
@@ -8927,10 +8922,10 @@
       </c>
       <c r="T62" s="43"/>
       <c r="U62" s="44" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="V62" s="45" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="W62" s="43" t="s">
         <v>46</v>
@@ -8953,16 +8948,16 @@
         <v>353</v>
       </c>
       <c r="F63" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G63" s="41" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H63" s="41" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I63" s="42" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J63" s="43" t="s">
         <v>66</v>
@@ -8976,7 +8971,7 @@
         <v>267</v>
       </c>
       <c r="O63" s="43" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="P63" s="43" t="s">
         <v>66</v>
@@ -8992,10 +8987,10 @@
       </c>
       <c r="T63" s="43"/>
       <c r="U63" s="44" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="V63" s="45" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="W63" s="43" t="s">
         <v>46</v>
@@ -9018,16 +9013,16 @@
         <v>354</v>
       </c>
       <c r="F64" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G64" s="41" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="H64" s="41" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I64" s="42" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J64" s="43" t="s">
         <v>66</v>
@@ -9041,7 +9036,7 @@
         <v>267</v>
       </c>
       <c r="O64" s="43" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="P64" s="43" t="s">
         <v>66</v>
@@ -9057,10 +9052,10 @@
       </c>
       <c r="T64" s="43"/>
       <c r="U64" s="44" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="V64" s="45" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="W64" s="43" t="s">
         <v>46</v>
@@ -9083,16 +9078,16 @@
         <v>355</v>
       </c>
       <c r="F65" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G65" s="41" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H65" s="41" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I65" s="42" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="J65" s="43" t="s">
         <v>66</v>
@@ -9106,7 +9101,7 @@
         <v>267</v>
       </c>
       <c r="O65" s="43" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="P65" s="43" t="s">
         <v>66</v>
@@ -9123,7 +9118,7 @@
       <c r="T65" s="43"/>
       <c r="U65" s="44"/>
       <c r="V65" s="45" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="W65" s="43" t="s">
         <v>46</v>
@@ -9146,16 +9141,16 @@
         <v>119</v>
       </c>
       <c r="F66" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G66" s="41" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H66" s="41" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="I66" s="42" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="J66" s="43" t="s">
         <v>66</v>
@@ -9169,7 +9164,7 @@
         <v>267</v>
       </c>
       <c r="O66" s="43" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="P66" s="43" t="s">
         <v>66</v>
@@ -9186,7 +9181,7 @@
       <c r="T66" s="43"/>
       <c r="U66" s="44"/>
       <c r="V66" s="45" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="W66" s="43" t="s">
         <v>46</v>
@@ -9209,16 +9204,16 @@
         <v>121</v>
       </c>
       <c r="F67" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G67" s="41" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="H67" s="41" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="I67" s="42" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="J67" s="43" t="s">
         <v>66</v>
@@ -9232,7 +9227,7 @@
         <v>267</v>
       </c>
       <c r="O67" s="43" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="P67" s="43" t="s">
         <v>66</v>
@@ -9249,7 +9244,7 @@
       <c r="T67" s="43"/>
       <c r="U67" s="44"/>
       <c r="V67" s="45" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="W67" s="43" t="s">
         <v>46</v>
@@ -9272,16 +9267,16 @@
         <v>356</v>
       </c>
       <c r="F68" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G68" s="41" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="H68" s="41" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I68" s="42" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="J68" s="43" t="s">
         <v>66</v>
@@ -9295,7 +9290,7 @@
         <v>267</v>
       </c>
       <c r="O68" s="43" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="P68" s="43" t="s">
         <v>66</v>
@@ -9312,7 +9307,7 @@
       <c r="T68" s="43"/>
       <c r="U68" s="44"/>
       <c r="V68" s="45" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="W68" s="43" t="s">
         <v>46</v>
@@ -9335,16 +9330,16 @@
         <v>357</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G69" s="41" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H69" s="41" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I69" s="42" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="J69" s="43" t="s">
         <v>66</v>
@@ -9358,7 +9353,7 @@
         <v>267</v>
       </c>
       <c r="O69" s="43" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="P69" s="43" t="s">
         <v>66</v>
@@ -9375,7 +9370,7 @@
       <c r="T69" s="43"/>
       <c r="U69" s="44"/>
       <c r="V69" s="45" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="W69" s="43" t="s">
         <v>46</v>
@@ -9398,16 +9393,16 @@
         <v>358</v>
       </c>
       <c r="F70" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G70" s="41" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="H70" s="41" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="I70" s="42" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="J70" s="43" t="s">
         <v>66</v>
@@ -9421,7 +9416,7 @@
         <v>267</v>
       </c>
       <c r="O70" s="43" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="P70" s="43" t="s">
         <v>66</v>
@@ -9438,7 +9433,7 @@
       <c r="T70" s="43"/>
       <c r="U70" s="44"/>
       <c r="V70" s="45" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="W70" s="43" t="s">
         <v>46</v>
@@ -9461,16 +9456,16 @@
         <v>359</v>
       </c>
       <c r="F71" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G71" s="41" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H71" s="41" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="I71" s="42" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="J71" s="43" t="s">
         <v>66</v>
@@ -9484,7 +9479,7 @@
         <v>267</v>
       </c>
       <c r="O71" s="43" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P71" s="43" t="s">
         <v>66</v>
@@ -9501,7 +9496,7 @@
       <c r="T71" s="43"/>
       <c r="U71" s="44"/>
       <c r="V71" s="45" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="W71" s="43" t="s">
         <v>46</v>
@@ -9524,16 +9519,16 @@
         <v>127</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G72" s="41" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="H72" s="41" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I72" s="42" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="J72" s="43" t="s">
         <v>66</v>
@@ -9547,7 +9542,7 @@
         <v>267</v>
       </c>
       <c r="O72" s="43" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="P72" s="43" t="s">
         <v>66</v>
@@ -9564,7 +9559,7 @@
       <c r="T72" s="43"/>
       <c r="U72" s="44"/>
       <c r="V72" s="45" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="W72" s="43" t="s">
         <v>46</v>
@@ -9587,16 +9582,16 @@
         <v>129</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G73" s="41" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="H73" s="41" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="I73" s="42" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="J73" s="43" t="s">
         <v>66</v>
@@ -9610,7 +9605,7 @@
         <v>267</v>
       </c>
       <c r="O73" s="43" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P73" s="43" t="s">
         <v>66</v>
@@ -9627,7 +9622,7 @@
       <c r="T73" s="43"/>
       <c r="U73" s="44"/>
       <c r="V73" s="45" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="W73" s="43" t="s">
         <v>46</v>
@@ -9650,16 +9645,16 @@
         <v>360</v>
       </c>
       <c r="F74" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G74" s="41" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="H74" s="41" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="I74" s="42" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="J74" s="43" t="s">
         <v>66</v>
@@ -9673,7 +9668,7 @@
         <v>267</v>
       </c>
       <c r="O74" s="43" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="P74" s="43" t="s">
         <v>66</v>
@@ -9690,7 +9685,7 @@
       <c r="T74" s="43"/>
       <c r="U74" s="44"/>
       <c r="V74" s="45" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="W74" s="43" t="s">
         <v>46</v>
@@ -9713,16 +9708,16 @@
         <v>415</v>
       </c>
       <c r="F75" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G75" s="41" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="H75" s="41" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="I75" s="42" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="J75" s="43" t="s">
         <v>66</v>
@@ -9736,7 +9731,7 @@
         <v>267</v>
       </c>
       <c r="O75" s="43" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="P75" s="43" t="s">
         <v>66</v>
@@ -9753,7 +9748,7 @@
       <c r="T75" s="43"/>
       <c r="U75" s="44"/>
       <c r="V75" s="45" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="W75" s="43" t="s">
         <v>46</v>
@@ -9776,16 +9771,16 @@
         <v>361</v>
       </c>
       <c r="F76" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G76" s="41" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="H76" s="41" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="I76" s="42" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="J76" s="43" t="s">
         <v>66</v>
@@ -9799,7 +9794,7 @@
         <v>267</v>
       </c>
       <c r="O76" s="43" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="P76" s="43" t="s">
         <v>66</v>
@@ -9816,7 +9811,7 @@
       <c r="T76" s="43"/>
       <c r="U76" s="44"/>
       <c r="V76" s="45" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="W76" s="43" t="s">
         <v>46</v>
@@ -9852,7 +9847,7 @@
       <c r="Q77" s="29"/>
       <c r="R77" s="29"/>
       <c r="S77" s="29" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="T77" s="29"/>
       <c r="U77" s="34"/>
@@ -9891,7 +9886,7 @@
       <c r="Q78" s="29"/>
       <c r="R78" s="29"/>
       <c r="S78" s="29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="T78" s="29"/>
       <c r="U78" s="34"/>
@@ -9929,7 +9924,7 @@
       <c r="P79" s="29"/>
       <c r="Q79" s="29"/>
       <c r="R79" s="29" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="S79" s="29"/>
       <c r="T79" s="29"/>
@@ -11806,16 +11801,16 @@
         <v>209</v>
       </c>
       <c r="F130" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G130" s="41" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="H130" s="41" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I130" s="42" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J130" s="43" t="s">
         <v>66</v>
@@ -11829,7 +11824,7 @@
         <v>267</v>
       </c>
       <c r="O130" s="43" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P130" s="43" t="s">
         <v>66</v>
@@ -11846,7 +11841,7 @@
       <c r="T130" s="43"/>
       <c r="U130" s="44"/>
       <c r="V130" s="45" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="W130" s="43" t="s">
         <v>46</v>
@@ -11869,16 +11864,16 @@
         <v>390</v>
       </c>
       <c r="F131" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G131" s="41" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H131" s="41" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="I131" s="42" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="J131" s="43" t="s">
         <v>66</v>
@@ -11892,7 +11887,7 @@
         <v>267</v>
       </c>
       <c r="O131" s="43" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="P131" s="43" t="s">
         <v>66</v>
@@ -11909,7 +11904,7 @@
       <c r="T131" s="43"/>
       <c r="U131" s="44"/>
       <c r="V131" s="45" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="W131" s="43" t="s">
         <v>46</v>
@@ -11932,16 +11927,16 @@
         <v>391</v>
       </c>
       <c r="F132" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G132" s="41" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="H132" s="41" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="I132" s="42" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="J132" s="43" t="s">
         <v>66</v>
@@ -11955,7 +11950,7 @@
         <v>267</v>
       </c>
       <c r="O132" s="43" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="P132" s="43" t="s">
         <v>66</v>
@@ -11972,7 +11967,7 @@
       <c r="T132" s="43"/>
       <c r="U132" s="44"/>
       <c r="V132" s="45" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="W132" s="43" t="s">
         <v>46</v>
@@ -11995,16 +11990,16 @@
         <v>392</v>
       </c>
       <c r="F133" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G133" s="41" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="H133" s="41" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="I133" s="42" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="J133" s="43" t="s">
         <v>66</v>
@@ -12018,7 +12013,7 @@
         <v>267</v>
       </c>
       <c r="O133" s="43" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="P133" s="43" t="s">
         <v>66</v>
@@ -12035,7 +12030,7 @@
       <c r="T133" s="43"/>
       <c r="U133" s="44"/>
       <c r="V133" s="45" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="W133" s="43" t="s">
         <v>46</v>
@@ -12058,16 +12053,16 @@
         <v>393</v>
       </c>
       <c r="F134" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G134" s="41" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="H134" s="41" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="I134" s="42" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="J134" s="43" t="s">
         <v>66</v>
@@ -12081,7 +12076,7 @@
         <v>267</v>
       </c>
       <c r="O134" s="43" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="P134" s="43" t="s">
         <v>66</v>
@@ -12098,7 +12093,7 @@
       <c r="T134" s="43"/>
       <c r="U134" s="44"/>
       <c r="V134" s="45" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="W134" s="43" t="s">
         <v>46</v>
@@ -12121,16 +12116,16 @@
         <v>394</v>
       </c>
       <c r="F135" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G135" s="41" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="H135" s="41" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I135" s="42" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="J135" s="43" t="s">
         <v>66</v>
@@ -12144,7 +12139,7 @@
         <v>267</v>
       </c>
       <c r="O135" s="43" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="P135" s="43" t="s">
         <v>66</v>
@@ -12161,7 +12156,7 @@
       <c r="T135" s="43"/>
       <c r="U135" s="44"/>
       <c r="V135" s="45" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="W135" s="43" t="s">
         <v>46</v>
@@ -12184,16 +12179,16 @@
         <v>395</v>
       </c>
       <c r="F136" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G136" s="41" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H136" s="41" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="I136" s="42" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="J136" s="43" t="s">
         <v>66</v>
@@ -12207,7 +12202,7 @@
         <v>267</v>
       </c>
       <c r="O136" s="43" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="P136" s="43" t="s">
         <v>66</v>
@@ -12224,7 +12219,7 @@
       <c r="T136" s="43"/>
       <c r="U136" s="44"/>
       <c r="V136" s="45" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="W136" s="43" t="s">
         <v>46</v>
@@ -12247,16 +12242,16 @@
         <v>217</v>
       </c>
       <c r="F137" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G137" s="41" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H137" s="41" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="I137" s="42" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="J137" s="43" t="s">
         <v>66</v>
@@ -12270,7 +12265,7 @@
         <v>267</v>
       </c>
       <c r="O137" s="43" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="P137" s="43" t="s">
         <v>66</v>
@@ -12287,7 +12282,7 @@
       <c r="T137" s="43"/>
       <c r="U137" s="44"/>
       <c r="V137" s="45" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="W137" s="43" t="s">
         <v>46</v>
@@ -12310,16 +12305,16 @@
         <v>219</v>
       </c>
       <c r="F138" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G138" s="41" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H138" s="41" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I138" s="42" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="J138" s="43" t="s">
         <v>66</v>
@@ -12333,7 +12328,7 @@
         <v>267</v>
       </c>
       <c r="O138" s="43" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="P138" s="43" t="s">
         <v>66</v>
@@ -12350,7 +12345,7 @@
       <c r="T138" s="43"/>
       <c r="U138" s="44"/>
       <c r="V138" s="45" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="W138" s="43" t="s">
         <v>46</v>
@@ -12373,16 +12368,16 @@
         <v>324</v>
       </c>
       <c r="F139" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G139" s="41" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="H139" s="41" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="I139" s="42" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="J139" s="43" t="s">
         <v>66</v>
@@ -12396,7 +12391,7 @@
         <v>267</v>
       </c>
       <c r="O139" s="43" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="P139" s="43" t="s">
         <v>66</v>
@@ -12413,7 +12408,7 @@
       <c r="T139" s="43"/>
       <c r="U139" s="44"/>
       <c r="V139" s="45" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="W139" s="43" t="s">
         <v>46</v>
@@ -12436,16 +12431,16 @@
         <v>325</v>
       </c>
       <c r="F140" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G140" s="41" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H140" s="41" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="I140" s="42" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="J140" s="43" t="s">
         <v>66</v>
@@ -12459,7 +12454,7 @@
         <v>267</v>
       </c>
       <c r="O140" s="43" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="P140" s="43" t="s">
         <v>66</v>
@@ -12476,7 +12471,7 @@
       <c r="T140" s="43"/>
       <c r="U140" s="44"/>
       <c r="V140" s="45" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="W140" s="43" t="s">
         <v>46</v>
@@ -12499,16 +12494,16 @@
         <v>326</v>
       </c>
       <c r="F141" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G141" s="41" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H141" s="41" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I141" s="42" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="J141" s="43" t="s">
         <v>66</v>
@@ -12522,7 +12517,7 @@
         <v>267</v>
       </c>
       <c r="O141" s="43" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="P141" s="43" t="s">
         <v>66</v>
@@ -12539,7 +12534,7 @@
       <c r="T141" s="43"/>
       <c r="U141" s="44"/>
       <c r="V141" s="45" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="W141" s="43" t="s">
         <v>46</v>
@@ -12562,16 +12557,16 @@
         <v>327</v>
       </c>
       <c r="F142" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G142" s="41" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="H142" s="41" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="I142" s="42" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J142" s="43" t="s">
         <v>66</v>
@@ -12585,7 +12580,7 @@
         <v>267</v>
       </c>
       <c r="O142" s="43" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="P142" s="43" t="s">
         <v>66</v>
@@ -12602,7 +12597,7 @@
       <c r="T142" s="43"/>
       <c r="U142" s="44"/>
       <c r="V142" s="45" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="W142" s="43" t="s">
         <v>46</v>
@@ -12625,16 +12620,16 @@
         <v>328</v>
       </c>
       <c r="F143" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G143" s="41" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H143" s="41" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="I143" s="42" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="J143" s="43" t="s">
         <v>66</v>
@@ -12648,7 +12643,7 @@
         <v>267</v>
       </c>
       <c r="O143" s="43" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="P143" s="43" t="s">
         <v>66</v>
@@ -12665,7 +12660,7 @@
       <c r="T143" s="43"/>
       <c r="U143" s="44"/>
       <c r="V143" s="45" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="W143" s="43" t="s">
         <v>46</v>
@@ -12688,16 +12683,16 @@
         <v>329</v>
       </c>
       <c r="F144" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G144" s="41" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H144" s="41" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="I144" s="42" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="J144" s="43" t="s">
         <v>66</v>
@@ -12711,7 +12706,7 @@
         <v>267</v>
       </c>
       <c r="O144" s="43" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="P144" s="43" t="s">
         <v>66</v>
@@ -12728,7 +12723,7 @@
       <c r="T144" s="43"/>
       <c r="U144" s="44"/>
       <c r="V144" s="45" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="W144" s="43" t="s">
         <v>46</v>
@@ -12751,16 +12746,16 @@
         <v>330</v>
       </c>
       <c r="F145" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G145" s="41" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="H145" s="41" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="I145" s="42" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="J145" s="43" t="s">
         <v>66</v>
@@ -12774,7 +12769,7 @@
         <v>267</v>
       </c>
       <c r="O145" s="43" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="P145" s="43" t="s">
         <v>66</v>
@@ -12791,7 +12786,7 @@
       <c r="T145" s="43"/>
       <c r="U145" s="44"/>
       <c r="V145" s="45" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="W145" s="43" t="s">
         <v>46</v>
@@ -12814,16 +12809,16 @@
         <v>331</v>
       </c>
       <c r="F146" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G146" s="41" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="H146" s="41" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="I146" s="42" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="J146" s="43" t="s">
         <v>66</v>
@@ -12837,7 +12832,7 @@
         <v>267</v>
       </c>
       <c r="O146" s="43" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P146" s="43" t="s">
         <v>66</v>
@@ -12854,7 +12849,7 @@
       <c r="T146" s="43"/>
       <c r="U146" s="44"/>
       <c r="V146" s="45" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W146" s="43" t="s">
         <v>46</v>
@@ -12877,16 +12872,16 @@
         <v>333</v>
       </c>
       <c r="F147" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G147" s="41" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="H147" s="41" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I147" s="42" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="J147" s="43" t="s">
         <v>66</v>
@@ -12900,7 +12895,7 @@
         <v>267</v>
       </c>
       <c r="O147" s="43" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="P147" s="43" t="s">
         <v>66</v>
@@ -12917,7 +12912,7 @@
       <c r="T147" s="43"/>
       <c r="U147" s="44"/>
       <c r="V147" s="45" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="W147" s="43" t="s">
         <v>46</v>
@@ -12953,7 +12948,7 @@
       <c r="Q148" s="29"/>
       <c r="R148" s="29"/>
       <c r="S148" s="29" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="T148" s="29"/>
       <c r="U148" s="34"/>
@@ -12992,7 +12987,7 @@
       <c r="Q149" s="29"/>
       <c r="R149" s="29"/>
       <c r="S149" s="29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="T149" s="29"/>
       <c r="U149" s="34"/>
@@ -13030,7 +13025,7 @@
       <c r="P150" s="29"/>
       <c r="Q150" s="29"/>
       <c r="R150" s="29" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="S150" s="29"/>
       <c r="T150" s="29"/>
@@ -13069,7 +13064,7 @@
       <c r="P151" s="29"/>
       <c r="Q151" s="29"/>
       <c r="R151" s="29" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="S151" s="29"/>
       <c r="T151" s="29"/>
@@ -13108,7 +13103,7 @@
       <c r="P152" s="29"/>
       <c r="Q152" s="29"/>
       <c r="R152" s="29" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="S152" s="29"/>
       <c r="T152" s="29"/>
@@ -14368,16 +14363,16 @@
         <v>321</v>
       </c>
       <c r="F186" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G186" s="41" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="H186" s="41" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="I186" s="42" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="J186" s="43" t="s">
         <v>66</v>
@@ -14406,7 +14401,7 @@
       </c>
       <c r="U186" s="44"/>
       <c r="V186" s="45" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="W186" s="43" t="s">
         <v>36</v>
@@ -14429,16 +14424,16 @@
         <v>322</v>
       </c>
       <c r="F187" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G187" s="41" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="H187" s="41" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I187" s="42" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="J187" s="43" t="s">
         <v>66</v>
@@ -14467,7 +14462,7 @@
       </c>
       <c r="U187" s="44"/>
       <c r="V187" s="45" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="W187" s="43" t="s">
         <v>36</v>
@@ -14484,22 +14479,22 @@
         <v>51</v>
       </c>
       <c r="D188" s="38" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E188" s="47" t="s">
         <v>441</v>
       </c>
       <c r="F188" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G188" s="41" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="H188" s="41" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="I188" s="42" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="J188" s="43" t="s">
         <v>66</v>
@@ -14530,7 +14525,7 @@
       </c>
       <c r="U188" s="44"/>
       <c r="V188" s="45" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="W188" s="43" t="s">
         <v>36</v>
@@ -14547,22 +14542,22 @@
         <v>51</v>
       </c>
       <c r="D189" s="38" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E189" s="47" t="s">
         <v>442</v>
       </c>
       <c r="F189" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G189" s="41" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="H189" s="41" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="I189" s="42" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="J189" s="43" t="s">
         <v>66</v>
@@ -14593,7 +14588,7 @@
       </c>
       <c r="U189" s="44"/>
       <c r="V189" s="45" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="W189" s="43" t="s">
         <v>36</v>
@@ -14616,16 +14611,16 @@
         <v>427</v>
       </c>
       <c r="F190" s="51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G190" s="41" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H190" s="41" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I190" s="42" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J190" s="43" t="s">
         <v>66</v>
@@ -14654,7 +14649,7 @@
       </c>
       <c r="U190" s="44"/>
       <c r="V190" s="45" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="W190" s="43" t="s">
         <v>36</v>
@@ -14677,16 +14672,16 @@
         <v>428</v>
       </c>
       <c r="F191" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G191" s="41" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="H191" s="41" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I191" s="42" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J191" s="43" t="s">
         <v>66</v>
@@ -14715,7 +14710,7 @@
       </c>
       <c r="U191" s="44"/>
       <c r="V191" s="45" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="W191" s="43" t="s">
         <v>36</v>
@@ -14738,16 +14733,16 @@
         <v>422</v>
       </c>
       <c r="F192" s="41" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G192" s="41" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="H192" s="41" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I192" s="42" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J192" s="43" t="s">
         <v>66</v>
@@ -14776,7 +14771,7 @@
       </c>
       <c r="U192" s="44"/>
       <c r="V192" s="45" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="W192" s="43" t="s">
         <v>36</v>
@@ -15058,16 +15053,16 @@
         <v>443</v>
       </c>
       <c r="F200" s="41" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G200" s="41" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="H200" s="41" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="I200" s="42" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="J200" s="43" t="s">
         <v>66</v>
@@ -15081,7 +15076,7 @@
         <v>267</v>
       </c>
       <c r="O200" s="43" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="P200" s="43" t="s">
         <v>66</v>
@@ -15098,7 +15093,7 @@
       <c r="T200" s="43"/>
       <c r="U200" s="44"/>
       <c r="V200" s="45" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="W200" s="43" t="s">
         <v>46</v>
@@ -21696,25 +21691,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F560B38A5B3C4B41B1895754B1F1A56A" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="69dc0f489d46816a4b9bb4a327e14425">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca719f03-9e45-4ef4-9920-d156f53157f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7de9a44ff87fdcabda187bbd662e75de" ns2:_="">
     <xsd:import namespace="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
@@ -21886,7 +21862,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca719f03-9e45-4ef4-9920-d156f53157f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -21904,32 +21925,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61CEF28A-E0A2-4D9D-9130-F7D0F35034F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ca719f03-9e45-4ef4-9920-d156f53157f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
aggiornati esito dei test in PASS
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D291D719-B295-401F-9144-46B7D0320F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDD6409-3B23-448F-8ED5-448A353E4CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1050" windowWidth="24630" windowHeight="14385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -5367,10 +5367,10 @@
   <dimension ref="A1:W755"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="O10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="T11" sqref="T11:T192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5762,7 +5762,7 @@
         <v>64</v>
       </c>
       <c r="T11" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U11" s="39"/>
       <c r="V11" s="40"/>
@@ -5817,7 +5817,7 @@
         <v>440</v>
       </c>
       <c r="T12" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U12" s="39"/>
       <c r="V12" s="40"/>
@@ -5909,7 +5909,7 @@
         <v>440</v>
       </c>
       <c r="T14" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U14" s="39"/>
       <c r="V14" s="40"/>
@@ -5964,7 +5964,7 @@
         <v>440</v>
       </c>
       <c r="T15" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U15" s="39"/>
       <c r="V15" s="40"/>
@@ -6130,7 +6130,7 @@
         <v>64</v>
       </c>
       <c r="T19" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U19" s="39"/>
       <c r="V19" s="40"/>
@@ -6185,7 +6185,7 @@
         <v>440</v>
       </c>
       <c r="T20" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U20" s="39"/>
       <c r="V20" s="40"/>
@@ -6277,7 +6277,7 @@
         <v>440</v>
       </c>
       <c r="T22" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U22" s="39"/>
       <c r="V22" s="40"/>
@@ -6332,7 +6332,7 @@
         <v>440</v>
       </c>
       <c r="T23" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U23" s="39"/>
       <c r="V23" s="40"/>
@@ -6500,7 +6500,7 @@
         <v>64</v>
       </c>
       <c r="T27" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U27" s="39" t="s">
         <v>64</v>
@@ -6559,7 +6559,7 @@
         <v>440</v>
       </c>
       <c r="T28" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U28" s="39" t="s">
         <v>64</v>
@@ -6657,7 +6657,7 @@
         <v>440</v>
       </c>
       <c r="T30" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U30" s="39" t="s">
         <v>64</v>
@@ -6716,7 +6716,7 @@
         <v>440</v>
       </c>
       <c r="T31" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U31" s="39" t="s">
         <v>64</v>
@@ -6896,7 +6896,7 @@
         <v>64</v>
       </c>
       <c r="T35" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U35" s="39"/>
       <c r="V35" s="40" t="s">
@@ -6959,7 +6959,7 @@
         <v>64</v>
       </c>
       <c r="T36" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U36" s="39"/>
       <c r="V36" s="40" t="s">
@@ -7022,7 +7022,7 @@
         <v>64</v>
       </c>
       <c r="T37" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U37" s="39"/>
       <c r="V37" s="40" t="s">
@@ -7085,7 +7085,7 @@
         <v>64</v>
       </c>
       <c r="T38" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U38" s="39"/>
       <c r="V38" s="40" t="s">
@@ -7148,7 +7148,7 @@
         <v>64</v>
       </c>
       <c r="T39" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U39" s="39"/>
       <c r="V39" s="40" t="s">
@@ -7211,7 +7211,7 @@
         <v>64</v>
       </c>
       <c r="T40" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U40" s="39"/>
       <c r="V40" s="40" t="s">
@@ -7274,7 +7274,7 @@
         <v>64</v>
       </c>
       <c r="T41" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U41" s="39"/>
       <c r="V41" s="40" t="s">
@@ -7337,7 +7337,7 @@
         <v>64</v>
       </c>
       <c r="T42" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U42" s="39"/>
       <c r="V42" s="40" t="s">
@@ -7400,7 +7400,7 @@
         <v>64</v>
       </c>
       <c r="T43" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U43" s="39"/>
       <c r="V43" s="40" t="s">
@@ -7461,7 +7461,7 @@
         <v>440</v>
       </c>
       <c r="T44" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U44" s="39"/>
       <c r="V44" s="40" t="s">
@@ -7522,7 +7522,7 @@
         <v>440</v>
       </c>
       <c r="T45" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U45" s="39"/>
       <c r="V45" s="40" t="s">
@@ -7583,7 +7583,7 @@
         <v>440</v>
       </c>
       <c r="T46" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U46" s="39"/>
       <c r="V46" s="40" t="s">
@@ -7644,7 +7644,7 @@
         <v>440</v>
       </c>
       <c r="T47" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U47" s="39"/>
       <c r="V47" s="40" t="s">
@@ -7705,7 +7705,7 @@
         <v>440</v>
       </c>
       <c r="T48" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U48" s="39"/>
       <c r="V48" s="40" t="s">
@@ -7766,7 +7766,7 @@
         <v>440</v>
       </c>
       <c r="T49" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U49" s="39"/>
       <c r="V49" s="40" t="s">
@@ -7827,7 +7827,7 @@
         <v>440</v>
       </c>
       <c r="T50" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U50" s="39"/>
       <c r="V50" s="40" t="s">
@@ -7888,7 +7888,7 @@
         <v>440</v>
       </c>
       <c r="T51" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U51" s="39"/>
       <c r="V51" s="40" t="s">
@@ -7949,7 +7949,7 @@
         <v>440</v>
       </c>
       <c r="T52" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U52" s="39"/>
       <c r="V52" s="40" t="s">
@@ -8010,7 +8010,7 @@
         <v>440</v>
       </c>
       <c r="T53" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U53" s="39"/>
       <c r="V53" s="40" t="s">
@@ -8071,7 +8071,7 @@
         <v>440</v>
       </c>
       <c r="T54" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U54" s="39"/>
       <c r="V54" s="40" t="s">
@@ -8132,7 +8132,7 @@
         <v>440</v>
       </c>
       <c r="T55" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U55" s="39"/>
       <c r="V55" s="40" t="s">
@@ -8193,7 +8193,7 @@
         <v>440</v>
       </c>
       <c r="T56" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U56" s="39"/>
       <c r="V56" s="40" t="s">
@@ -8254,7 +8254,7 @@
         <v>440</v>
       </c>
       <c r="T57" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U57" s="39"/>
       <c r="V57" s="40" t="s">
@@ -8315,7 +8315,7 @@
         <v>440</v>
       </c>
       <c r="T58" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U58" s="39"/>
       <c r="V58" s="40" t="s">
@@ -8376,7 +8376,7 @@
         <v>440</v>
       </c>
       <c r="T59" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U59" s="39"/>
       <c r="V59" s="40" t="s">
@@ -8437,7 +8437,7 @@
         <v>440</v>
       </c>
       <c r="T60" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U60" s="39"/>
       <c r="V60" s="40" t="s">
@@ -8498,7 +8498,7 @@
         <v>440</v>
       </c>
       <c r="T61" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U61" s="39"/>
       <c r="V61" s="40" t="s">
@@ -8559,7 +8559,7 @@
         <v>440</v>
       </c>
       <c r="T62" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U62" s="39"/>
       <c r="V62" s="40" t="s">
@@ -8620,7 +8620,7 @@
         <v>440</v>
       </c>
       <c r="T63" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U63" s="39"/>
       <c r="V63" s="40" t="s">
@@ -8681,7 +8681,7 @@
         <v>440</v>
       </c>
       <c r="T64" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U64" s="39"/>
       <c r="V64" s="40" t="s">
@@ -8742,7 +8742,7 @@
         <v>440</v>
       </c>
       <c r="T65" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U65" s="39"/>
       <c r="V65" s="40" t="s">
@@ -8803,7 +8803,7 @@
         <v>440</v>
       </c>
       <c r="T66" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U66" s="39"/>
       <c r="V66" s="40" t="s">
@@ -8864,7 +8864,7 @@
         <v>440</v>
       </c>
       <c r="T67" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U67" s="39"/>
       <c r="V67" s="40" t="s">
@@ -8925,7 +8925,7 @@
         <v>440</v>
       </c>
       <c r="T68" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U68" s="39"/>
       <c r="V68" s="40" t="s">
@@ -8986,7 +8986,7 @@
         <v>440</v>
       </c>
       <c r="T69" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U69" s="39"/>
       <c r="V69" s="40" t="s">
@@ -9047,7 +9047,7 @@
         <v>440</v>
       </c>
       <c r="T70" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U70" s="39"/>
       <c r="V70" s="40" t="s">
@@ -10847,7 +10847,7 @@
         <v>440</v>
       </c>
       <c r="T118" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U118" s="39"/>
       <c r="V118" s="40" t="s">
@@ -10908,7 +10908,7 @@
         <v>440</v>
       </c>
       <c r="T119" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U119" s="39"/>
       <c r="V119" s="40" t="s">
@@ -10969,7 +10969,7 @@
         <v>440</v>
       </c>
       <c r="T120" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U120" s="39"/>
       <c r="V120" s="40" t="s">
@@ -11030,7 +11030,7 @@
         <v>440</v>
       </c>
       <c r="T121" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U121" s="39"/>
       <c r="V121" s="40" t="s">
@@ -11091,7 +11091,7 @@
         <v>440</v>
       </c>
       <c r="T122" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U122" s="39"/>
       <c r="V122" s="40" t="s">
@@ -11152,7 +11152,7 @@
         <v>440</v>
       </c>
       <c r="T123" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U123" s="39"/>
       <c r="V123" s="40" t="s">
@@ -11213,7 +11213,7 @@
         <v>440</v>
       </c>
       <c r="T124" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U124" s="39"/>
       <c r="V124" s="40" t="s">
@@ -11274,7 +11274,7 @@
         <v>440</v>
       </c>
       <c r="T125" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U125" s="39"/>
       <c r="V125" s="40" t="s">
@@ -11335,7 +11335,7 @@
         <v>440</v>
       </c>
       <c r="T126" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U126" s="39"/>
       <c r="V126" s="40" t="s">
@@ -11396,7 +11396,7 @@
         <v>440</v>
       </c>
       <c r="T127" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U127" s="39"/>
       <c r="V127" s="40" t="s">
@@ -11457,7 +11457,7 @@
         <v>440</v>
       </c>
       <c r="T128" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U128" s="39"/>
       <c r="V128" s="40" t="s">
@@ -11518,7 +11518,7 @@
         <v>440</v>
       </c>
       <c r="T129" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U129" s="39"/>
       <c r="V129" s="40" t="s">
@@ -11579,7 +11579,7 @@
         <v>440</v>
       </c>
       <c r="T130" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U130" s="39"/>
       <c r="V130" s="40" t="s">
@@ -11640,7 +11640,7 @@
         <v>440</v>
       </c>
       <c r="T131" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U131" s="39"/>
       <c r="V131" s="40" t="s">
@@ -11701,7 +11701,7 @@
         <v>440</v>
       </c>
       <c r="T132" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U132" s="39"/>
       <c r="V132" s="40" t="s">
@@ -11762,7 +11762,7 @@
         <v>440</v>
       </c>
       <c r="T133" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U133" s="39"/>
       <c r="V133" s="40" t="s">
@@ -13660,7 +13660,7 @@
         <v>440</v>
       </c>
       <c r="T181" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U181" s="35"/>
       <c r="V181" s="38" t="s">
@@ -13721,7 +13721,7 @@
         <v>440</v>
       </c>
       <c r="T182" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U182" s="35"/>
       <c r="V182" s="38" t="s">
@@ -13895,7 +13895,7 @@
         <v>64</v>
       </c>
       <c r="T186" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U186" s="35"/>
       <c r="V186" s="38" t="s">
@@ -13956,7 +13956,7 @@
         <v>440</v>
       </c>
       <c r="T187" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U187" s="35"/>
       <c r="V187" s="38" t="s">
@@ -14017,7 +14017,7 @@
         <v>440</v>
       </c>
       <c r="T188" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U188" s="35"/>
       <c r="V188" s="38" t="s">
@@ -20560,12 +20560,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20827,21 +20830,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20866,18 +20875,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
corretto test 58 LAB
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDD6409-3B23-448F-8ED5-448A353E4CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B592E0F-4D09-44B2-B22A-00512B8FAE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="708">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1856,30 +1856,6 @@
   <si>
     <t>{
   "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
-  "data": "2025-05-12T19:56:03.4590406Z",
-  "status": 200,
-  "traceID": "8cf438f0ebb0a7ac33411edc4cbf54a3",
-  "spanID": "4d3359c3abc5287d",
-  "warning": "[W002 | Si consiglia di valorizzare l\u0027elemento organizer[CLUSTER]/code]",
-  "workflowInstanceId": "2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.1140632be3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId",
-  "type": null,
-  "title": null,
-  "detail": null,
-  "instance": "58"
-}</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.1140632be3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>8cf438f0ebb0a7ac33411edc4cbf54a3</t>
-  </si>
-  <si>
-    <t>2025-05-12T19:56:03</t>
-  </si>
-  <si>
-    <t>{
-  "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
   "data": "2025-05-12T19:58:03.8961217Z",
   "status": 500,
   "traceID": "f9032970195ef8247482a3ff9db5ebea",
@@ -3301,6 +3277,33 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>{
+  "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
+  "data": "2025-05-19T06:23:50.7085296Z",
+  "status": 500,
+  "traceID": "e1cd0b068710e80ae37139a9e6bb89fc",
+  "spanID": "216a731b36dd6157",
+  "warning": null,
+  "workflowInstanceId": null,
+  "type": "/msg/vocabulary",
+  "title": "Errore vocabolario.",
+  "detail": "Almeno uno dei seguenti vocaboli non \u00E8 censito: [CodeSystem: 2.16.840.1.113883.5.7 v2.1.0, Codes: X]",
+  "instance": "58"
+}</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.e91bd65a09e359d5008fcfb05475e5cdbea191674eec491e50715318b2cbdd68.901a3e990a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e1cd0b068710e80ae37139a9e6bb89fc</t>
+  </si>
+  <si>
+    <t>2025-05-19T06:23:50</t>
+  </si>
+  <si>
+    <t>2025-05-19'</t>
   </si>
 </sst>
 </file>
@@ -5364,13 +5367,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W755"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="O10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="T11" sqref="T11:T192"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5451,7 +5455,7 @@
       </c>
       <c r="D3" s="47"/>
       <c r="E3" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -5479,7 +5483,7 @@
       </c>
       <c r="D4" s="47"/>
       <c r="E4" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -5507,7 +5511,7 @@
       </c>
       <c r="D5" s="47"/>
       <c r="E5" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -5770,7 +5774,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35">
         <v>29</v>
       </c>
@@ -5825,7 +5829,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35">
         <v>30</v>
       </c>
@@ -5862,7 +5866,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>31</v>
       </c>
@@ -5917,7 +5921,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35">
         <v>32</v>
       </c>
@@ -5972,7 +5976,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35">
         <v>33</v>
       </c>
@@ -6009,7 +6013,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35">
         <v>34</v>
       </c>
@@ -6046,7 +6050,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35">
         <v>35</v>
       </c>
@@ -6138,7 +6142,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35">
         <v>37</v>
       </c>
@@ -6193,7 +6197,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35">
         <v>38</v>
       </c>
@@ -6230,7 +6234,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35">
         <v>39</v>
       </c>
@@ -6285,7 +6289,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35">
         <v>40</v>
       </c>
@@ -6340,7 +6344,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35">
         <v>41</v>
       </c>
@@ -6377,7 +6381,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35">
         <v>42</v>
       </c>
@@ -6414,7 +6418,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="35">
         <v>43</v>
       </c>
@@ -6510,7 +6514,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35">
         <v>45</v>
       </c>
@@ -6569,7 +6573,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="35">
         <v>46</v>
       </c>
@@ -6608,7 +6612,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="35">
         <v>47</v>
       </c>
@@ -6667,7 +6671,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="35">
         <v>48</v>
       </c>
@@ -6726,7 +6730,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35">
         <v>49</v>
       </c>
@@ -6765,7 +6769,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35">
         <v>50</v>
       </c>
@@ -6804,7 +6808,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="35">
         <v>51</v>
       </c>
@@ -7112,16 +7116,16 @@
         <v>79</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>447</v>
+        <v>707</v>
       </c>
       <c r="G39" s="37" t="s">
-        <v>467</v>
+        <v>706</v>
       </c>
       <c r="H39" s="37" t="s">
-        <v>466</v>
+        <v>705</v>
       </c>
       <c r="I39" s="42" t="s">
-        <v>465</v>
+        <v>704</v>
       </c>
       <c r="J39" s="38" t="s">
         <v>64</v>
@@ -7152,7 +7156,7 @@
       </c>
       <c r="U39" s="39"/>
       <c r="V39" s="40" t="s">
-        <v>464</v>
+        <v>703</v>
       </c>
       <c r="W39" s="38" t="s">
         <v>44</v>
@@ -7178,13 +7182,13 @@
         <v>447</v>
       </c>
       <c r="G40" s="37" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H40" s="37" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="I40" s="42" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="J40" s="38" t="s">
         <v>64</v>
@@ -7215,7 +7219,7 @@
       </c>
       <c r="U40" s="39"/>
       <c r="V40" s="40" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="W40" s="38" t="s">
         <v>44</v>
@@ -7241,13 +7245,13 @@
         <v>447</v>
       </c>
       <c r="G41" s="37" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="H41" s="37" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="I41" s="42" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="J41" s="38" t="s">
         <v>64</v>
@@ -7278,7 +7282,7 @@
       </c>
       <c r="U41" s="39"/>
       <c r="V41" s="40" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="W41" s="38" t="s">
         <v>44</v>
@@ -7304,13 +7308,13 @@
         <v>447</v>
       </c>
       <c r="G42" s="37" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="H42" s="37" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="I42" s="42" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="J42" s="38" t="s">
         <v>64</v>
@@ -7341,7 +7345,7 @@
       </c>
       <c r="U42" s="39"/>
       <c r="V42" s="40" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="W42" s="38" t="s">
         <v>44</v>
@@ -7367,13 +7371,13 @@
         <v>447</v>
       </c>
       <c r="G43" s="37" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="H43" s="37" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="I43" s="42" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="J43" s="38" t="s">
         <v>64</v>
@@ -7404,13 +7408,13 @@
       </c>
       <c r="U43" s="39"/>
       <c r="V43" s="40" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="W43" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35">
         <v>64</v>
       </c>
@@ -7427,16 +7431,16 @@
         <v>298</v>
       </c>
       <c r="F44" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G44" s="37" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="H44" s="37" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="I44" s="42" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="J44" s="38"/>
       <c r="K44" s="38"/>
@@ -7465,13 +7469,13 @@
       </c>
       <c r="U44" s="39"/>
       <c r="V44" s="40" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="W44" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35">
         <v>66</v>
       </c>
@@ -7488,16 +7492,16 @@
         <v>299</v>
       </c>
       <c r="F45" s="37" t="s">
+        <v>492</v>
+      </c>
+      <c r="G45" s="37" t="s">
         <v>496</v>
       </c>
-      <c r="G45" s="37" t="s">
-        <v>500</v>
-      </c>
       <c r="H45" s="37" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="I45" s="42" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="J45" s="38"/>
       <c r="K45" s="38"/>
@@ -7526,13 +7530,13 @@
       </c>
       <c r="U45" s="39"/>
       <c r="V45" s="40" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="W45" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="35">
         <v>67</v>
       </c>
@@ -7549,16 +7553,16 @@
         <v>300</v>
       </c>
       <c r="F46" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G46" s="37" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="H46" s="37" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="I46" s="42" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="J46" s="38"/>
       <c r="K46" s="38"/>
@@ -7587,13 +7591,13 @@
       </c>
       <c r="U46" s="39"/>
       <c r="V46" s="40" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="W46" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="35">
         <v>68</v>
       </c>
@@ -7610,16 +7614,16 @@
         <v>301</v>
       </c>
       <c r="F47" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G47" s="37" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="H47" s="37" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="I47" s="42" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="J47" s="38"/>
       <c r="K47" s="38"/>
@@ -7648,13 +7652,13 @@
       </c>
       <c r="U47" s="39"/>
       <c r="V47" s="40" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="W47" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="35">
         <v>69</v>
       </c>
@@ -7671,16 +7675,16 @@
         <v>302</v>
       </c>
       <c r="F48" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G48" s="37" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="H48" s="37" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="I48" s="42" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="J48" s="38"/>
       <c r="K48" s="38"/>
@@ -7709,13 +7713,13 @@
       </c>
       <c r="U48" s="39"/>
       <c r="V48" s="40" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="W48" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="35">
         <v>70</v>
       </c>
@@ -7732,16 +7736,16 @@
         <v>303</v>
       </c>
       <c r="F49" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G49" s="37" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="H49" s="37" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="I49" s="42" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="J49" s="38"/>
       <c r="K49" s="38"/>
@@ -7770,13 +7774,13 @@
       </c>
       <c r="U49" s="39"/>
       <c r="V49" s="40" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="W49" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="35">
         <v>71</v>
       </c>
@@ -7793,16 +7797,16 @@
         <v>304</v>
       </c>
       <c r="F50" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G50" s="37" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="H50" s="37" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="I50" s="42" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="J50" s="38"/>
       <c r="K50" s="38"/>
@@ -7831,13 +7835,13 @@
       </c>
       <c r="U50" s="39"/>
       <c r="V50" s="40" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="W50" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="35">
         <v>72</v>
       </c>
@@ -7854,16 +7858,16 @@
         <v>305</v>
       </c>
       <c r="F51" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G51" s="37" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="H51" s="37" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="I51" s="42" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="J51" s="38"/>
       <c r="K51" s="38"/>
@@ -7892,13 +7896,13 @@
       </c>
       <c r="U51" s="39"/>
       <c r="V51" s="40" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="W51" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="35">
         <v>73</v>
       </c>
@@ -7915,16 +7919,16 @@
         <v>306</v>
       </c>
       <c r="F52" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G52" s="37" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="H52" s="37" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="I52" s="42" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="J52" s="38"/>
       <c r="K52" s="38"/>
@@ -7953,13 +7957,13 @@
       </c>
       <c r="U52" s="39"/>
       <c r="V52" s="40" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="W52" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="35">
         <v>74</v>
       </c>
@@ -7976,16 +7980,16 @@
         <v>307</v>
       </c>
       <c r="F53" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G53" s="37" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="H53" s="37" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="I53" s="42" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="J53" s="38"/>
       <c r="K53" s="38"/>
@@ -8014,13 +8018,13 @@
       </c>
       <c r="U53" s="39"/>
       <c r="V53" s="40" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="W53" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="35">
         <v>76</v>
       </c>
@@ -8037,16 +8041,16 @@
         <v>308</v>
       </c>
       <c r="F54" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G54" s="37" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="H54" s="37" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="I54" s="42" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="J54" s="38"/>
       <c r="K54" s="38"/>
@@ -8075,13 +8079,13 @@
       </c>
       <c r="U54" s="39"/>
       <c r="V54" s="40" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="W54" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="35">
         <v>78</v>
       </c>
@@ -8098,16 +8102,16 @@
         <v>100</v>
       </c>
       <c r="F55" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G55" s="37" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="H55" s="37" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="I55" s="42" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="J55" s="38"/>
       <c r="K55" s="38"/>
@@ -8136,13 +8140,13 @@
       </c>
       <c r="U55" s="39"/>
       <c r="V55" s="40" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="W55" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="35">
         <v>79</v>
       </c>
@@ -8159,16 +8163,16 @@
         <v>309</v>
       </c>
       <c r="F56" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G56" s="37" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="H56" s="37" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="I56" s="42" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="J56" s="38"/>
       <c r="K56" s="38"/>
@@ -8197,13 +8201,13 @@
       </c>
       <c r="U56" s="39"/>
       <c r="V56" s="40" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="W56" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="35">
         <v>80</v>
       </c>
@@ -8220,16 +8224,16 @@
         <v>310</v>
       </c>
       <c r="F57" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G57" s="37" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="H57" s="37" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="I57" s="42" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="J57" s="38"/>
       <c r="K57" s="38"/>
@@ -8258,13 +8262,13 @@
       </c>
       <c r="U57" s="39"/>
       <c r="V57" s="40" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="W57" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="35">
         <v>81</v>
       </c>
@@ -8281,16 +8285,16 @@
         <v>311</v>
       </c>
       <c r="F58" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G58" s="37" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="H58" s="37" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="I58" s="42" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="J58" s="38"/>
       <c r="K58" s="38"/>
@@ -8319,13 +8323,13 @@
       </c>
       <c r="U58" s="39"/>
       <c r="V58" s="40" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="W58" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="35">
         <v>82</v>
       </c>
@@ -8342,16 +8346,16 @@
         <v>312</v>
       </c>
       <c r="F59" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G59" s="37" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="H59" s="37" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="I59" s="42" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="J59" s="38"/>
       <c r="K59" s="38"/>
@@ -8380,13 +8384,13 @@
       </c>
       <c r="U59" s="39"/>
       <c r="V59" s="40" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="W59" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="35">
         <v>83</v>
       </c>
@@ -8403,16 +8407,16 @@
         <v>106</v>
       </c>
       <c r="F60" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G60" s="37" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="H60" s="37" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="I60" s="42" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="J60" s="38"/>
       <c r="K60" s="38"/>
@@ -8441,13 +8445,13 @@
       </c>
       <c r="U60" s="39"/>
       <c r="V60" s="40" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="W60" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="35">
         <v>84</v>
       </c>
@@ -8464,16 +8468,16 @@
         <v>108</v>
       </c>
       <c r="F61" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G61" s="37" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H61" s="37" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="I61" s="42" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="J61" s="38"/>
       <c r="K61" s="38"/>
@@ -8502,13 +8506,13 @@
       </c>
       <c r="U61" s="39"/>
       <c r="V61" s="40" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="W61" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="35">
         <v>85</v>
       </c>
@@ -8525,16 +8529,16 @@
         <v>313</v>
       </c>
       <c r="F62" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G62" s="37" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="H62" s="37" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="I62" s="42" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="J62" s="38"/>
       <c r="K62" s="38"/>
@@ -8563,13 +8567,13 @@
       </c>
       <c r="U62" s="39"/>
       <c r="V62" s="40" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="W62" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="35">
         <v>86</v>
       </c>
@@ -8586,16 +8590,16 @@
         <v>314</v>
       </c>
       <c r="F63" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G63" s="37" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="H63" s="37" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="I63" s="42" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J63" s="38"/>
       <c r="K63" s="38"/>
@@ -8624,13 +8628,13 @@
       </c>
       <c r="U63" s="39"/>
       <c r="V63" s="40" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="W63" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="35">
         <v>87</v>
       </c>
@@ -8647,16 +8651,16 @@
         <v>315</v>
       </c>
       <c r="F64" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G64" s="37" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="H64" s="37" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="I64" s="42" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="J64" s="38"/>
       <c r="K64" s="38"/>
@@ -8685,13 +8689,13 @@
       </c>
       <c r="U64" s="39"/>
       <c r="V64" s="40" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="W64" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="35">
         <v>88</v>
       </c>
@@ -8708,16 +8712,16 @@
         <v>316</v>
       </c>
       <c r="F65" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G65" s="37" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="H65" s="37" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="I65" s="42" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="J65" s="38"/>
       <c r="K65" s="38"/>
@@ -8746,13 +8750,13 @@
       </c>
       <c r="U65" s="39"/>
       <c r="V65" s="40" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="W65" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="35">
         <v>89</v>
       </c>
@@ -8769,16 +8773,16 @@
         <v>114</v>
       </c>
       <c r="F66" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G66" s="37" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="H66" s="37" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="I66" s="42" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="J66" s="38"/>
       <c r="K66" s="38"/>
@@ -8807,13 +8811,13 @@
       </c>
       <c r="U66" s="39"/>
       <c r="V66" s="40" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="W66" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="35">
         <v>90</v>
       </c>
@@ -8830,16 +8834,16 @@
         <v>116</v>
       </c>
       <c r="F67" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G67" s="37" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="H67" s="37" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="I67" s="42" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="J67" s="38"/>
       <c r="K67" s="38"/>
@@ -8868,13 +8872,13 @@
       </c>
       <c r="U67" s="39"/>
       <c r="V67" s="40" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="W67" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="35">
         <v>91</v>
       </c>
@@ -8891,16 +8895,16 @@
         <v>317</v>
       </c>
       <c r="F68" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G68" s="37" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H68" s="37" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="I68" s="42" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="J68" s="38"/>
       <c r="K68" s="38"/>
@@ -8929,13 +8933,13 @@
       </c>
       <c r="U68" s="39"/>
       <c r="V68" s="40" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="W68" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="35">
         <v>92</v>
       </c>
@@ -8952,16 +8956,16 @@
         <v>367</v>
       </c>
       <c r="F69" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G69" s="37" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="H69" s="37" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="I69" s="42" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="J69" s="38"/>
       <c r="K69" s="38"/>
@@ -8990,13 +8994,13 @@
       </c>
       <c r="U69" s="39"/>
       <c r="V69" s="40" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="W69" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="35">
         <v>93</v>
       </c>
@@ -9013,16 +9017,16 @@
         <v>318</v>
       </c>
       <c r="F70" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G70" s="37" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="H70" s="37" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="I70" s="42" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="J70" s="38"/>
       <c r="K70" s="38"/>
@@ -9051,13 +9055,13 @@
       </c>
       <c r="U70" s="39"/>
       <c r="V70" s="40" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="W70" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="35">
         <v>95</v>
       </c>
@@ -9094,7 +9098,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="35">
         <v>97</v>
       </c>
@@ -9131,7 +9135,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="35">
         <v>98</v>
       </c>
@@ -9168,7 +9172,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="35">
         <v>99</v>
       </c>
@@ -9205,7 +9209,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="35">
         <v>100</v>
       </c>
@@ -9242,7 +9246,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="35">
         <v>101</v>
       </c>
@@ -9279,7 +9283,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="35">
         <v>102</v>
       </c>
@@ -9316,7 +9320,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="35">
         <v>103</v>
       </c>
@@ -9353,7 +9357,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="35">
         <v>104</v>
       </c>
@@ -9390,7 +9394,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="35">
         <v>105</v>
       </c>
@@ -9427,7 +9431,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="35">
         <v>106</v>
       </c>
@@ -9464,7 +9468,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="35">
         <v>108</v>
       </c>
@@ -9501,7 +9505,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="35">
         <v>110</v>
       </c>
@@ -9538,7 +9542,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="35">
         <v>111</v>
       </c>
@@ -9575,7 +9579,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="35">
         <v>112</v>
       </c>
@@ -9612,7 +9616,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="35">
         <v>113</v>
       </c>
@@ -9649,7 +9653,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="35">
         <v>114</v>
       </c>
@@ -9686,7 +9690,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="35">
         <v>115</v>
       </c>
@@ -9723,7 +9727,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="35">
         <v>116</v>
       </c>
@@ -9760,7 +9764,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="35">
         <v>117</v>
       </c>
@@ -9797,7 +9801,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="35">
         <v>118</v>
       </c>
@@ -9834,7 +9838,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="35">
         <v>119</v>
       </c>
@@ -9871,7 +9875,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="35">
         <v>120</v>
       </c>
@@ -9908,7 +9912,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="35">
         <v>121</v>
       </c>
@@ -9945,7 +9949,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="35">
         <v>123</v>
       </c>
@@ -9982,7 +9986,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="35">
         <v>125</v>
       </c>
@@ -10019,7 +10023,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="35">
         <v>126</v>
       </c>
@@ -10056,7 +10060,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="35">
         <v>127</v>
       </c>
@@ -10093,7 +10097,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="35">
         <v>128</v>
       </c>
@@ -10130,7 +10134,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="35">
         <v>129</v>
       </c>
@@ -10167,7 +10171,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="35">
         <v>130</v>
       </c>
@@ -10204,7 +10208,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="35">
         <v>131</v>
       </c>
@@ -10241,7 +10245,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="35">
         <v>132</v>
       </c>
@@ -10278,7 +10282,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="35">
         <v>133</v>
       </c>
@@ -10315,7 +10319,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="35">
         <v>134</v>
       </c>
@@ -10352,7 +10356,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="35">
         <v>135</v>
       </c>
@@ -10389,7 +10393,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="35">
         <v>136</v>
       </c>
@@ -10426,7 +10430,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="35">
         <v>137</v>
       </c>
@@ -10463,7 +10467,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="35">
         <v>138</v>
       </c>
@@ -10500,7 +10504,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="35">
         <v>139</v>
       </c>
@@ -10537,7 +10541,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="35">
         <v>140</v>
       </c>
@@ -10574,7 +10578,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="35">
         <v>141</v>
       </c>
@@ -10611,7 +10615,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="35">
         <v>142</v>
       </c>
@@ -10648,7 +10652,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="35">
         <v>143</v>
       </c>
@@ -10685,7 +10689,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="35">
         <v>144</v>
       </c>
@@ -10722,7 +10726,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="35">
         <v>145</v>
       </c>
@@ -10759,7 +10763,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="35">
         <v>146</v>
       </c>
@@ -10796,7 +10800,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="35">
         <v>152</v>
       </c>
@@ -10813,16 +10817,16 @@
         <v>344</v>
       </c>
       <c r="F118" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G118" s="37" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="H118" s="37" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="I118" s="37" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="J118" s="38"/>
       <c r="K118" s="38"/>
@@ -10851,13 +10855,13 @@
       </c>
       <c r="U118" s="39"/>
       <c r="V118" s="40" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="W118" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="35">
         <v>154</v>
       </c>
@@ -10874,16 +10878,16 @@
         <v>345</v>
       </c>
       <c r="F119" s="37" t="s">
+        <v>625</v>
+      </c>
+      <c r="G119" s="37" t="s">
         <v>629</v>
       </c>
-      <c r="G119" s="37" t="s">
-        <v>633</v>
-      </c>
       <c r="H119" s="37" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="I119" s="42" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="J119" s="38"/>
       <c r="K119" s="38"/>
@@ -10912,13 +10916,13 @@
       </c>
       <c r="U119" s="39"/>
       <c r="V119" s="40" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="W119" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="35">
         <v>155</v>
       </c>
@@ -10935,16 +10939,16 @@
         <v>346</v>
       </c>
       <c r="F120" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G120" s="37" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="H120" s="37" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="I120" s="42" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="J120" s="38"/>
       <c r="K120" s="38"/>
@@ -10973,13 +10977,13 @@
       </c>
       <c r="U120" s="39"/>
       <c r="V120" s="40" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="W120" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="35">
         <v>156</v>
       </c>
@@ -10996,16 +11000,16 @@
         <v>347</v>
       </c>
       <c r="F121" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G121" s="37" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="H121" s="37" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="I121" s="42" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="J121" s="38"/>
       <c r="K121" s="38"/>
@@ -11034,13 +11038,13 @@
       </c>
       <c r="U121" s="39"/>
       <c r="V121" s="40" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="W121" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="35">
         <v>158</v>
       </c>
@@ -11057,16 +11061,16 @@
         <v>348</v>
       </c>
       <c r="F122" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G122" s="37" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="H122" s="37" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="I122" s="42" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="J122" s="38"/>
       <c r="K122" s="38"/>
@@ -11095,13 +11099,13 @@
       </c>
       <c r="U122" s="39"/>
       <c r="V122" s="40" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="W122" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="35">
         <v>159</v>
       </c>
@@ -11118,16 +11122,16 @@
         <v>192</v>
       </c>
       <c r="F123" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G123" s="37" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="H123" s="37" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="I123" s="42" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="J123" s="38"/>
       <c r="K123" s="38"/>
@@ -11156,13 +11160,13 @@
       </c>
       <c r="U123" s="39"/>
       <c r="V123" s="40" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="W123" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="35">
         <v>160</v>
       </c>
@@ -11179,16 +11183,16 @@
         <v>194</v>
       </c>
       <c r="F124" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G124" s="37" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="H124" s="37" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="I124" s="42" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="J124" s="38"/>
       <c r="K124" s="38"/>
@@ -11217,13 +11221,13 @@
       </c>
       <c r="U124" s="39"/>
       <c r="V124" s="40" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="W124" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="35">
         <v>161</v>
       </c>
@@ -11240,16 +11244,16 @@
         <v>284</v>
       </c>
       <c r="F125" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G125" s="37" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="H125" s="37" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="I125" s="42" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="J125" s="38"/>
       <c r="K125" s="38"/>
@@ -11278,13 +11282,13 @@
       </c>
       <c r="U125" s="39"/>
       <c r="V125" s="40" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="W125" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="35">
         <v>162</v>
       </c>
@@ -11301,16 +11305,16 @@
         <v>285</v>
       </c>
       <c r="F126" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G126" s="37" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="H126" s="37" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="I126" s="42" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="J126" s="38"/>
       <c r="K126" s="38"/>
@@ -11339,13 +11343,13 @@
       </c>
       <c r="U126" s="39"/>
       <c r="V126" s="40" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="W126" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="35">
         <v>163</v>
       </c>
@@ -11362,16 +11366,16 @@
         <v>286</v>
       </c>
       <c r="F127" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G127" s="37" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="H127" s="37" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="I127" s="42" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="J127" s="38"/>
       <c r="K127" s="38"/>
@@ -11400,13 +11404,13 @@
       </c>
       <c r="U127" s="39"/>
       <c r="V127" s="40" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="W127" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="35">
         <v>164</v>
       </c>
@@ -11423,16 +11427,16 @@
         <v>287</v>
       </c>
       <c r="F128" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G128" s="37" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="H128" s="37" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="I128" s="42" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="J128" s="38"/>
       <c r="K128" s="38"/>
@@ -11461,13 +11465,13 @@
       </c>
       <c r="U128" s="39"/>
       <c r="V128" s="40" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="W128" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="35">
         <v>165</v>
       </c>
@@ -11484,16 +11488,16 @@
         <v>288</v>
       </c>
       <c r="F129" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G129" s="37" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="H129" s="37" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="I129" s="42" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="J129" s="38"/>
       <c r="K129" s="38"/>
@@ -11522,13 +11526,13 @@
       </c>
       <c r="U129" s="39"/>
       <c r="V129" s="40" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="W129" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="35">
         <v>166</v>
       </c>
@@ -11545,16 +11549,16 @@
         <v>289</v>
       </c>
       <c r="F130" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G130" s="37" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="H130" s="37" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="I130" s="42" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="J130" s="38"/>
       <c r="K130" s="38"/>
@@ -11583,13 +11587,13 @@
       </c>
       <c r="U130" s="39"/>
       <c r="V130" s="40" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="W130" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="35">
         <v>167</v>
       </c>
@@ -11606,16 +11610,16 @@
         <v>290</v>
       </c>
       <c r="F131" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G131" s="37" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="H131" s="37" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="I131" s="42" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="J131" s="38"/>
       <c r="K131" s="38"/>
@@ -11644,13 +11648,13 @@
       </c>
       <c r="U131" s="39"/>
       <c r="V131" s="40" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="W131" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="35">
         <v>168</v>
       </c>
@@ -11667,16 +11671,16 @@
         <v>291</v>
       </c>
       <c r="F132" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G132" s="37" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="H132" s="37" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="I132" s="42" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="J132" s="38"/>
       <c r="K132" s="38"/>
@@ -11705,13 +11709,13 @@
       </c>
       <c r="U132" s="39"/>
       <c r="V132" s="40" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="W132" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="35">
         <v>169</v>
       </c>
@@ -11728,16 +11732,16 @@
         <v>293</v>
       </c>
       <c r="F133" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G133" s="37" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="H133" s="37" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="I133" s="42" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="J133" s="38"/>
       <c r="K133" s="38"/>
@@ -11766,13 +11770,13 @@
       </c>
       <c r="U133" s="39"/>
       <c r="V133" s="40" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="W133" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="35">
         <v>175</v>
       </c>
@@ -11809,7 +11813,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="35">
         <v>177</v>
       </c>
@@ -11846,7 +11850,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="35">
         <v>178</v>
       </c>
@@ -11883,7 +11887,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="35">
         <v>179</v>
       </c>
@@ -11920,7 +11924,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="138" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="35">
         <v>180</v>
       </c>
@@ -11957,7 +11961,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="139" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="35">
         <v>181</v>
       </c>
@@ -11994,7 +11998,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="140" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="35">
         <v>182</v>
       </c>
@@ -12031,7 +12035,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="141" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="35">
         <v>183</v>
       </c>
@@ -12068,7 +12072,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="142" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="35">
         <v>184</v>
       </c>
@@ -12105,7 +12109,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="143" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="35">
         <v>185</v>
       </c>
@@ -12142,7 +12146,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="144" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="35">
         <v>186</v>
       </c>
@@ -12179,7 +12183,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="145" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="35">
         <v>187</v>
       </c>
@@ -12216,7 +12220,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="146" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="35">
         <v>188</v>
       </c>
@@ -12253,7 +12257,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="147" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="35">
         <v>189</v>
       </c>
@@ -12290,7 +12294,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="35">
         <v>190</v>
       </c>
@@ -12413,7 +12417,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="35">
         <v>417</v>
       </c>
@@ -12450,7 +12454,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="35">
         <v>418</v>
       </c>
@@ -12487,7 +12491,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="35">
         <v>419</v>
       </c>
@@ -12524,7 +12528,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="35">
         <v>423</v>
       </c>
@@ -12561,7 +12565,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="35">
         <v>424</v>
       </c>
@@ -12598,7 +12602,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="35">
         <v>425</v>
       </c>
@@ -12635,7 +12639,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="35">
         <v>432</v>
       </c>
@@ -12672,7 +12676,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="35">
         <v>433</v>
       </c>
@@ -12709,7 +12713,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="35">
         <v>434</v>
       </c>
@@ -12746,7 +12750,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="35">
         <v>435</v>
       </c>
@@ -12783,7 +12787,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="35">
         <v>437</v>
       </c>
@@ -12820,7 +12824,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="35">
         <v>438</v>
       </c>
@@ -12857,7 +12861,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="35">
         <v>440</v>
       </c>
@@ -12894,7 +12898,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="164" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="35">
         <v>441</v>
       </c>
@@ -12931,7 +12935,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="165" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="35">
         <v>442</v>
       </c>
@@ -12968,7 +12972,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="166" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="35">
         <v>443</v>
       </c>
@@ -13005,7 +13009,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="35">
         <v>444</v>
       </c>
@@ -13042,7 +13046,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="35">
         <v>445</v>
       </c>
@@ -13079,7 +13083,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="35">
         <v>448</v>
       </c>
@@ -13096,16 +13100,16 @@
         <v>395</v>
       </c>
       <c r="F169" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G169" s="37" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="H169" s="37" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="I169" s="42" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="J169" s="38"/>
       <c r="K169" s="38"/>
@@ -13134,13 +13138,13 @@
       </c>
       <c r="U169" s="39"/>
       <c r="V169" s="40" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="W169" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="35">
         <v>449</v>
       </c>
@@ -13157,16 +13161,16 @@
         <v>396</v>
       </c>
       <c r="F170" s="37" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G170" s="37" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="H170" s="37" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="I170" s="42" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="J170" s="38"/>
       <c r="K170" s="38"/>
@@ -13195,13 +13199,13 @@
       </c>
       <c r="U170" s="39"/>
       <c r="V170" s="40" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="W170" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="35">
         <v>450</v>
       </c>
@@ -13218,16 +13222,16 @@
         <v>379</v>
       </c>
       <c r="F171" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G171" s="37" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="H171" s="37" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="I171" s="42" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="J171" s="38"/>
       <c r="K171" s="38"/>
@@ -13244,13 +13248,13 @@
       </c>
       <c r="U171" s="39"/>
       <c r="V171" s="40" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="W171" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="35">
         <v>451</v>
       </c>
@@ -13267,16 +13271,16 @@
         <v>380</v>
       </c>
       <c r="F172" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G172" s="37" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="H172" s="37" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="I172" s="42" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="J172" s="38"/>
       <c r="K172" s="38"/>
@@ -13293,7 +13297,7 @@
       </c>
       <c r="U172" s="39"/>
       <c r="V172" s="40" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="W172" s="38" t="s">
         <v>36</v>
@@ -13319,13 +13323,13 @@
         <v>447</v>
       </c>
       <c r="G173" s="37" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="H173" s="37" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="I173" s="42" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="J173" s="38" t="s">
         <v>64</v>
@@ -13344,13 +13348,13 @@
       </c>
       <c r="U173" s="39"/>
       <c r="V173" s="40" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="W173" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="35">
         <v>454</v>
       </c>
@@ -13387,7 +13391,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="175" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="35">
         <v>455</v>
       </c>
@@ -13424,7 +13428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="176" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="35">
         <v>456</v>
       </c>
@@ -13461,7 +13465,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="35">
         <v>457</v>
       </c>
@@ -13498,7 +13502,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="35">
         <v>458</v>
       </c>
@@ -13535,7 +13539,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="35">
         <v>459</v>
       </c>
@@ -13572,7 +13576,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="35">
         <v>460</v>
       </c>
@@ -13609,7 +13613,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="35">
         <v>461</v>
       </c>
@@ -13626,16 +13630,16 @@
         <v>397</v>
       </c>
       <c r="F181" s="35" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G181" s="35" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="H181" s="35" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="I181" s="35" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="J181" s="38"/>
       <c r="K181" s="38"/>
@@ -13664,13 +13668,13 @@
       </c>
       <c r="U181" s="35"/>
       <c r="V181" s="38" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="W181" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="35">
         <v>462</v>
       </c>
@@ -13687,16 +13691,16 @@
         <v>402</v>
       </c>
       <c r="F182" s="35" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G182" s="35" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="H182" s="35" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="I182" s="35" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="J182" s="38"/>
       <c r="K182" s="38"/>
@@ -13725,13 +13729,13 @@
       </c>
       <c r="U182" s="35"/>
       <c r="V182" s="38" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="W182" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="35">
         <v>463</v>
       </c>
@@ -13768,7 +13772,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="35">
         <v>464</v>
       </c>
@@ -13805,7 +13809,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="35">
         <v>465</v>
       </c>
@@ -13862,13 +13866,13 @@
         <v>447</v>
       </c>
       <c r="G186" s="35" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="H186" s="45" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="I186" s="35" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="J186" s="38" t="s">
         <v>64</v>
@@ -13899,13 +13903,13 @@
       </c>
       <c r="U186" s="35"/>
       <c r="V186" s="38" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="W186" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="35">
         <v>467</v>
       </c>
@@ -13922,16 +13926,16 @@
         <v>410</v>
       </c>
       <c r="F187" s="35" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G187" s="35" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="H187" s="35" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="I187" s="35" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="J187" s="38"/>
       <c r="K187" s="38"/>
@@ -13960,13 +13964,13 @@
       </c>
       <c r="U187" s="35"/>
       <c r="V187" s="38" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="W187" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="35">
         <v>468</v>
       </c>
@@ -13983,16 +13987,16 @@
         <v>412</v>
       </c>
       <c r="F188" s="35" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="G188" s="35" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="H188" s="35" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="I188" s="35" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="J188" s="38"/>
       <c r="K188" s="38"/>
@@ -14021,13 +14025,13 @@
       </c>
       <c r="U188" s="35"/>
       <c r="V188" s="38" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="W188" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="35">
         <v>469</v>
       </c>
@@ -14064,7 +14068,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="190" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="35">
         <v>470</v>
       </c>
@@ -14101,7 +14105,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="191" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="35">
         <v>471</v>
       </c>
@@ -14118,16 +14122,16 @@
         <v>429</v>
       </c>
       <c r="F191" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G191" s="37" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="H191" s="37" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="I191" s="42" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="J191" s="38"/>
       <c r="K191" s="38"/>
@@ -14144,13 +14148,13 @@
       </c>
       <c r="U191" s="39"/>
       <c r="V191" s="40" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="W191" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="192" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="35">
         <v>472</v>
       </c>
@@ -14167,16 +14171,16 @@
         <v>434</v>
       </c>
       <c r="F192" s="37" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G192" s="37" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="H192" s="37" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="I192" s="42" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="J192" s="38"/>
       <c r="K192" s="38"/>
@@ -14193,7 +14197,7 @@
       </c>
       <c r="U192" s="39"/>
       <c r="V192" s="40" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="W192" s="38" t="s">
         <v>36</v>
@@ -18276,7 +18280,13 @@
     <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A9:W192" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A9:W192" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="LAB"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -20560,15 +20570,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20830,27 +20837,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20875,9 +20876,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiunti messaggi di errore e messaggi per i time out
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B592E0F-4D09-44B2-B22A-00512B8FAE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FC6878-BC30-490A-AD3F-37859E4CBD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1971" uniqueCount="761">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2435,30 +2435,6 @@
   <si>
     <t>{
   "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
-  "data": "2025-05-13T13:19:45.4958625Z",
-  "status": 200,
-  "traceID": "7e7041e363d131b481ae5c80e3937a7e",
-  "spanID": "64f1c2b4a1384609",
-  "warning": null,
-  "workflowInstanceId": "2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.084574209f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId",
-  "type": null,
-  "title": null,
-  "detail": null,
-  "instance": null
-}</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.084574209f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>7e7041e363d131b481ae5c80e3937a7e</t>
-  </si>
-  <si>
-    <t>2025-05-13T13:19:45</t>
-  </si>
-  <si>
-    <t>{
-  "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
   "data": "2025-05-13T13:22:56.2701131Z",
   "status": 500,
   "traceID": "c3900fe3589029a76f7c7ab444d0d58d",
@@ -2894,30 +2870,6 @@
   <si>
     <t>{
   "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
-  "data": "2025-05-14T12:03:48.8434568Z",
-  "status": 200,
-  "traceID": "691448ea8e3bd6246d04087762b5ec20",
-  "spanID": "9a5ba023302ce847",
-  "warning": null,
-  "workflowInstanceId": "2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.ca754df069^^^^urn:ihe:iti:xdw:2013:workflowInstanceId",
-  "type": null,
-  "title": null,
-  "detail": null,
-  "instance": null
-}</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.ca754df069^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>691448ea8e3bd6246d04087762b5ec20</t>
-  </si>
-  <si>
-    <t>2025-05-14T12:03:48</t>
-  </si>
-  <si>
-    <t>{
-  "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
   "data": "2025-05-14T12:42:50.8335619Z",
   "status": 500,
   "traceID": "febb806718a0e132095f732c14a84877",
@@ -3304,6 +3256,287 @@
   </si>
   <si>
     <t>2025-05-19'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Campo token JWT non valido.",
+  "detail": "JWT payload: Person id presente nel JWT differente dal codice fiscale del paziente previsto sul CDA",</t>
+  </si>
+  <si>
+    <t>"title": "Errore semantico.",
+"detail": "[ERRORE-12| L\u0027elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi \u0027country\u0027, \u0027city\u0027 e \u0027streetAddressLine\u0027 ],[W002 | Si consiglia di valorizzare l\u0027elemento organizer[CLUSTER]/code]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-15| L\u0027elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi \u0027given\u0027 e \u0027family\u0027],[W002 | Si consiglia di valorizzare l\u0027elemento organizer[CLUSTER]/code]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore vocabolario.",
+  "detail": "Almeno uno dei seguenti vocaboli non \u00E8 censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: T]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore vocabolario.",
+  "detail": "Almeno uno dei seguenti vocaboli non \u00E8 censito: [CodeSystem: 2.16.840.1.113883.5.7 v2.1.0, Codes: X]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore di sintassi.",
+  "detail": "ERROR: -1,-1 cvc-datatype-valid.1.2.3: \u0027\u0027 is not a valid value of union type \u0027uid\u0027.,ERROR: -1,-1 cvc-attribute.3: The value \u0027\u0027 of attribute \u0027root\u0027 on element \u0027id\u0027 is not valid with respect to its type, \u0027uid\u0027.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b1| L\u0027elemento code della section DEVE essere valorizzato con uno dei seguenti codici LOINC individuati:\n\t\t\t\t\t\t18717-9 BANCA DEL SANGUE\n\t\t\t\t\t\t18718-7 MARCATORI CELLULARI \n\t\t\t\t\t\t18719-5 CHIMICA\n\t\t\t\t\t\t18720-3\tCOAGULAZIONE\n\t\t\t\t\t\t18721-1 MONITORAGGIO TERAPEUTICO DEI FARMACI\n\t\t\t\t\t\t18722-9 FERTILIT\u00C0\n\t\t\t\t\t\t18723-7 EMATOLOGIA\n\t\t\t\t\t\t18724-5 HLA\n\t\t\t\t\t\t18725-2 MICROBIOLOGIA\n\t\t\t\t\t\t18727-8 SEROLOGIA\n\t\t\t\t\t\t18728-6 TOSSICOLOGIA\n\t\t\t\t\t\t18729-4 ESAMI DELLE URINE\n\t\t\t\t\t\t18767-4 EMOGASANALISI\n\t\t\t\t\t\t18768-2 CONTE CELLULARE\u002BDIFFERENZIALE\n\t\t\t\t\t\t18769-0 SUSCETTIBILIT\u00C0 ANTIMICROBICA\n\t\t\t\t\t\t26435-8 PATOLOGIA MOLECOLARE\n\t\t\t\t\t\t26436-6 ESAMI DI LABORATORIO\n\t\t\t\t\t\t26437-4 TEST DI SENSIBILIT\u00C0 A SOSTANZE CHIMICHE\n\t\t\t\t\t\t26438-2 CITOLOGIA\n\t\t\t\t\t\t18716-1 ALLERGOLOGIA\n\t\t\t\t\t\t26439-0 PATOLOGIA CHIRURGICA],[W002 | Si consiglia di valorizzare l\u0027elemento organizer[CLUSTER]/code]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore vocabolario.",
+  "detail": "Almeno uno dei seguenti vocaboli non \u00E8 censito: [CodeSystem: 2.16.840.1.113883.5.129, Codes: 18717-9]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore di sintassi.",
+  "detail": "ERROR: -1,-1 cvc-pattern-valid: Value \u0027\u0027 is not facet-valid with respect to pattern \u0027[^\\s]\u002B\u0027 for type \u0027cs\u0027.,ERROR: -1,-1 cvc-attribute.3: The value \u0027\u0027 of attribute \u0027code\u0027 on element \u0027code\u0027 is not valid with respect to its type, \u0027cs\u0027.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-11| L\u0027elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi \u0027country\u0027, \u0027city\u0027 e \u0027streetAddressLine\u0027 ],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO\u0027 contenere l\u0027elemento \u0027entry\u0027 ]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "title": "Errore semantico.",
+  "detail": "[ERRORE-14| L\u0027elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi \u0027given\u0027 e \u0027family\u0027],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO\u0027 contenere l\u0027elemento \u0027entry\u0027 ]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l\u0027elemento \u0027text\u0027],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO\u0027 contenere l\u0027elemento \u0027entry\u0027 ]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b3| Sezione Decorso Ospedaliero: la sezione DEVE essere presente],[ERRORE-b4| Sezione Decorso Ospedaliero: La sezione deve contenere l\u0027elemento \u0027text\u0027],[ERRORE-b17| Il codice \u0027\u0027 non \u00E8 corretto. La sezione deve essere valorizzata con uno dei seguenti codici:\n\t\t\t46241-6\tSezione Motivo del ricovero\n\t\t\t47039-3\tSezione Inquadramento clinico iniziale\n\t\t\t8648-8  Sezione Decorso Ospedaliero\n\t\t\t55109-3 Sezione Complicanze\n\t\t\t11493-4 Sezione Riscontri ed accertamenti significativi\n\t\t\t34104-0 Sezione Consulenza\n\t\t\t30954-2 Sezione Esami eseguiti durante il ricovero\n\t\t\t47519-4 Sezione Procedure eseguite durante il ricovero\n\t\t\t48765-2 Sezione Allergie\n\t\t\t10160-0 Sezione Terapia farmacologica effettuata durante il ricovero\n\t\t\t11535-2 Sezione Condizioni del paziente alla dimissione e diagnosi alla dimissione\n\t\t\t10183-2 Sezione Terapia farmacologica alla dimissione\n\t\t\t18776-5 Sezione Istruzioni di follow-up\n\t\t\t],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO\u0027 contenere l\u0027elemento \u0027entry\u0027 ]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b26| Sotto-sezione Anamnesi: l\u0027elemento entry/observation/effectiveTime deve essere presente e deve avere l\u0027elemento \u0027low\u0027 valorizzato]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b94|Sezione Terapia farmacologica alla dimissione: section/entry/substanceAdministration/effectiveTime deve avere l\u0027elemento \u0027low\u0027 valorizzato ]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore vocabolario.",
+  "detail": "Almeno uno dei seguenti vocaboli non \u00E8 censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 3001XXA.01]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore vocabolario.",
+  "detail": "Almeno uno dei seguenti vocaboli non \u00E8 censito: [CodeSystem: 2.16.840.1.113883.5.112 v2.1.0, Codes: ZXZZXX]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-11| L\u0027elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i suoi sotto-elementi \u0027country\u0027, \u0027city\u0027 e \u0027streetAddressLine\u0027.   ]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-14| L\u0027elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi \u0027given\u0027 e \u0027family\u0027]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-34| L\u0027elemento participant/associatedEntity deve contenere l\u0027elemento \u0027id\u0027.],[ERRORE-45a| L\u0027elemento telecom di un\u0027organizzazione non pu\u00F2 essere di tipo Home, ovvero l\u0027attributo @use deve essere diverso da: H | HP | HV.\n\t\t\t],[ERRORE-54| L\u0027indirizzo di un\u0027organizzazione non pu\u00F2 essere di tipo Home, ovvero l\u0027attributo @use deve essere diverso da: H | HP | HV.\n\t\t\t]",</t>
+  </si>
+  <si>
+    <t>{
+  "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
+  "data": "2025-05-21T13:22:25.8072531Z",
+  "status": 500,
+  "traceID": "2703b53a707ebb7447bb84908964d229",
+  "spanID": "3eaced2e70bb4cc0",
+  "warning": null,
+  "workflowInstanceId": null,
+  "type": "/msg/vocabulary",
+  "title": "Errore vocabolario.",
+  "detail": "Almeno uno dei seguenti vocaboli non \u00E8 censito: [CodeSystem: 2.16.840.1.113883.5.7 v2.1.0, Codes: X]",
+  "instance": "/validation/error"
+}</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.3df664b5ebf2cb9f80459ec4402743d0166f96898aa71d631d88190060a07c55.f9b7b4284b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2703b53a707ebb7447bb84908964d229</t>
+  </si>
+  <si>
+    <t>2025-05-21T13:22:25</t>
+  </si>
+  <si>
+    <t>2025-05-21'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore di sintassi.",
+  "detail": "ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element \u0027{\u0022urn:hl7-org:v3\u0022:priorityCode}\u0027. One of \u0027{\u0022urn:hl7-org:v3\u0022:realmCode, \u0022urn:hl7-org:v3\u0022:typeId, \u0022urn:hl7-org:v3\u0022:templateId, \u0022urn:hl7-org:v3\u0022:id}\u0027 is expected.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore di sintassi.",
+  "detail": "ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element \u0027{\u0022urn:hl7-org:v3\u0022:text}\u0027. One of \u0027{\u0022urn:hl7-org:v3\u0022:realmCode, \u0022urn:hl7-org:v3\u0022:typeId, \u0022urn:hl7-org:v3\u0022:templateId, \u0022urn:hl7-org:v3\u0022:id, \u0022urn:hl7-org:v3\u0022:code}\u0027 is expected.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b4| Sezione Referto: DEVE essere presente la sezione \u0022Referto\u0022.],[ERRORE-b5| Sezione Referto: La sezione deve contenere l\u0027elemento \u0027text\u0027.]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b13| Sezione Precedenti Esami Eseguiti: La section deve contenere l\u0027elemento \u0027text\u0027.]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore di sintassi.",
+  "detail": "ERROR: -1,-1 cvc-complex-type.2.4.b: The content of element \u0027observation\u0027 is not complete. One of \u0027{\u0022urn:hl7-org:v3\u0022:id, \u0022urn:hl7-org:v3\u0022:code}\u0027 is expected.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b22| Sezione Storia Clinica: L\u0027elemento entry/observation/effectiveTime deve essere presente e deve avere l\u0027elemento \u0027low\u0027 valorizzato.]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b26| Sezione Storia Clinica: La entry/organizer deve avere un elemento subject/relatedSubject il quale deve contenere l\u0027elemento \u0027code\u0027. ]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b58| Sotto sezione Allergie: L\u0027elemento participant/participantRole/playingEntity deve avere l\u0027attributo code valorizzato con @nullFlavor=\u0027UNK\u0027 nel caso in cui non \u00E8 noto l\u0027agente della reazione allergica altrimenti\n\t\t\t\tcode/@codeSystem valorizzato come segue:\n\t\t\t\t- \u00272.16.840.1.113883.6.73\u0027 per la codifica \u0022WHO ATC\u0022\n\t\t\t\t- \u00272.16.840.1.113883.2.9.6.1.5\u0027 per la codifica \u0022AIC\u0022\n\t\t\t\t- \u00272.16.840.1.113883.2.9.77.22.11.2\u0027 per il value set \u0022AllergenNoDrugs\u0022 (- per le allergie non a farmaci \u2013)\n\t\t\t]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore di sintassi.",
+  "detail": "ERROR: -1,-1 cvc-datatype-valid.1.2.3: \u0027XX\u0027 is not a valid value of union type \u0027real\u0027.,ERROR: -1,-1 cvc-attribute.3: The value \u0027XX\u0027 of attribute \u0027value\u0027 on element \u0027value\u0027 is not valid with respect to its type, \u0027real\u0027.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-40| L\u0027elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l\u0027elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: \u0027PROG\u0027|\u0027DIR\u0027|\u0027RAD_PROG|\u0027RAD_DIR\u0027 ]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-11| L\u0027elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi \u0027country\u0027, \u0027city\u0027 e \u0027streetAddressLine\u0027 ]",</t>
+  </si>
+  <si>
+    <t>{
+  "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
+  "data": "2025-05-21T15:06:35.7523132Z",
+  "status": 500,
+  "traceID": "dd88ef23aee6b152f10a3b1e041b6728",
+  "spanID": "439812e35bd177e7",
+  "warning": null,
+  "workflowInstanceId": null,
+  "type": "/msg/vocabulary",
+  "title": "Errore vocabolario.",
+  "detail": "Almeno uno dei seguenti vocaboli non \u00E8 censito: [CodeSystem: 2.16.840.1.113883.5.7 v2.1.0, Codes: X]",
+  "instance": "/validation/error"
+}</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190925.4.4.83a4c05d663926983e00aca4f670b4183133f2ddd40cf04481868fb2007f2237.0acb3ea64d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>dd88ef23aee6b152f10a3b1e041b6728</t>
+  </si>
+  <si>
+    <t>2025-05-21T15:06:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore di sintassi.",
+  "detail": "ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element \u0027{\u0022urn:hl7-org:v3\u0022:effectiveTime}\u0027. One of \u0027{\u0022urn:hl7-org:v3\u0022:realmCode, \u0022urn:hl7-org:v3\u0022:typeId, \u0022urn:hl7-org:v3\u0022:templateId, \u0022urn:hl7-org:v3\u0022:id, \u0022urn:hl7-org:v3\u0022:code}\u0027 is expected.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b4| Sezione Referto: la sezione DEVE essere presente],[ERRORE-b5| Sezione Referto: la sezione DEVE contenere un elemento \u0027text\u0027],[ERRORE-b20| Il codice \u0027\u0027 non \u00E8 corretto. La sezione deve essere valorizzata con uno dei seguenti codici:\n\t\t\t29299-5\tSezione Quesito Diagnostico\n\t\t\t11329-0\tSezione Storia Clinica\n\t\t\t30954-2\tSezione Precedenti Esami Eseguiti\n\t\t\t29545-1\tSezione Esame Obiettivo\n\t\t\t62387-6\tSezione Prestazioni\n\t\t\t93126-1\tSezione Confronto Con Precedenti Esami Eseguiti\n\t\t\t47045-0\tSezione Referto\n\t\t\t29548-5 Sezione Diagnosi\n\t\t\t55110-1\tSezione Conclusioni\n\t\t\t62385-0\tSezione Suggerimenti Per Il Medico Prescrittore \n\t\t\t80615-8 Sezione Accertamenti e Controlli Consigliati \n\t\t\t93341-6 Sezione Terapia Farmacologica Consigliata\n\t\t\t]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b6| Sezione Quesito Diagnostico: la sezione DEVE contenere un elemento \u0027text\u0027]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b26| Sezione Storia Clinica: l\u0027elemento entry/observation/effectiveTime deve essere presente e deve avere l\u0027elemento \u0027low\u0027 valorizzato],[ERRORE-b27| Sezione Storia Clinica: l\u0027elemento entry/observation/effectiveTime deve essere presente e deve avere l\u0027elemento \u0027high\u0027 valorizzato nel caso in cui il problema risulta non essere pi\u00F9 presente]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b36| Sezione Storia Clinica: l\u0027elemento entry/organizer/subject/relatedSubject deve avere l\u0027attributo @classCode=\u0027PRS\u0027 e deve contenere l\u0027elemento \u0027code\u0027]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b53| Sotto-sezione Allergie: l\u0027elemento entry/act/entryRelationship/observation/effectiveTime deve essere presente e deve avere l\u0027elemento \u0027low\u0027 valorizzato ]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-b61| Sotto sezione Allergie: L\u0027elemento participant/participantRole/playingEntity deve avere l\u0027attributo code valorizzato con @nullFlavor=\u0027UNK\u0027 nel caso in cui non \u00E8 noto l\u0027agente della reazione allergica altrimenti\n\t\t\t\tcode/@codeSystem valorizzato come segue:\n\t\t\t\t- \u00272.16.840.1.113883.6.73\u0027 per la codifica \u0022WHO ATC\u0022\n\t\t\t\t- \u00272.16.840.1.113883.2.9.6.1.5\u0027 per la codifica \u0022AIC\u0022\n\t\t\t\t- \u00272.16.840.1.113883.2.9.77.22.11.2\u0027 per il value set \u0022AllergenNoDrugs\u0022 (- per le allergie non a farmaci \u2013)\n\t\t\t]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore di sintassi.",
+  "detail": "ERROR: -1,-1 cvc-datatype-valid.1.2.3: \u00272.16.840.1.113883.6.XXX\u0027 is not a valid value of union type \u0027uid\u0027.,ERROR: -1,-1 cvc-attribute.3: The value \u00272.16.840.1.113883.6.XXX\u0027 of attribute \u0027codeSystem\u0027 on element \u0027value\u0027 is not valid with respect to its type, \u0027uid\u0027.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-30| L\u0027elemento ClinicalDocument/legalAuthenticator/signatureCode deve essere valorizzato con il codice \u0022S\u0022 ]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore vocabolario.",
+  "detail": "Almeno uno dei seguenti vocaboli non \u00E8 censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 575.6666]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-6| L\u0027elemento ClinicalDocument/confidentialityCode DEVE avere l\u0027attributo @code valorizzato con \u0027N\u0027 o \u0027R\u0027 o \u0027V\u0027, e il @codeSystem=\u00272.16.840.1.113883.5.25\u0027]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-6| L\u0027elemento ClinicalDocument/confidentialityCode DEVE avere l\u0027attributo @code valorizzato con \u0027N\u0027 o \u0027R\u0027 o \u0027V\u0027, e il @codeSystem=\u00272.16.840.1.113883.5.25\u0027],[W002 | Si consiglia di valorizzare l\u0027elemento organizer[CLUSTER]/code]",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Errore semantico.",
+  "detail": "[ERRORE-6| L\u0027elemento ClinicalDocument/confidentialityCode DEVE avere l\u0027attributo @code valorizzato con \u0027N\u0027 o \u0027R\u0027 o \u0027V\u0027, e il @codeSystem=\u00272.16.840.1.113883.5.25\u0027],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO\u0027 contenere l\u0027elemento \u0027entry\u0027 ]",</t>
+  </si>
+  <si>
+    <t>{
+  "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
+  "data": "2025-05-21T15:21:06.5037654Z",
+  "status": 500,
+  "traceID": "417de76c89effbc494fe008633ee91a9",
+  "spanID": "6e6efbba192c6792",
+  "warning": null,
+  "workflowInstanceId": null,
+  "type": "/msg/jwt-validation",
+  "title": "Campo token JWT non valido.",
+  "detail": "Il campo purpose_of_use non \u00E8 corretto",
+  "instance": "28"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Campo token JWT non valido.",
+  "detail": "Il campo purpose_of_use non \u00E8 corretto",</t>
+  </si>
+  <si>
+    <t>{
+  "id": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
+  "data": "2025-05-21T15:25:45.6435744Z",
+  "status": 500,
+  "traceID": "1ceba0e7ccbcf2074d99360e725ed6a7",
+  "spanID": "21f85f652b4b08c5",
+  "warning": null,
+  "workflowInstanceId": null,
+  "type": "/msg/jwt-validation",
+  "title": "Campo token JWT non valido.",
+  "detail": "Il campo action_id non \u00E8 corretto",
+  "instance": "36"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "title": "Campo token JWT non valido.",
+  "detail": "Il campo action_id non \u00E8 corretto",</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Il metodo di test FSEGATEWAY.API.TEST.ValidateLabTest.VALIDAZIONE_LAB_TIMEOUT ha generato un'eccezione: 
+System.Net.Http.HttpRequestException: Host sconosciuto. (auth.giomi.com:443) ---&gt; System.Net.Sockets.SocketException: Host sconosciuto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Il metodo di test FSEGATEWAY.API.TEST.ValidateLdoTest.VALIDAZIONE_LDO_TIMEOUT ha generato un'eccezione: 
+System.Net.Http.HttpRequestException: Host sconosciuto. (auth.giomi.com:443) ---&gt; System.Net.Sockets.SocketException: Host sconosciuto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Il metodo di test FSEGATEWAY.API.TEST.ValidateRadTest.VALIDAZIONE_RAD_TIMEOUT ha generato un'eccezione: 
+System.Net.Http.HttpRequestException: Host sconosciuto. (auth.giomi.com:443) ---&gt; System.Net.Sockets.SocketException: Host sconosciuto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Il metodo di test FSEGATEWAY.API.TEST.ValidateRsaTest.VALIDAZIONE_RSA_TIMEOUT ha generato un'eccezione: 
+System.Net.Http.HttpRequestException: Host sconosciuto. (auth.giomi.com:443) ---&gt; System.Net.Sockets.SocketException: Host sconosciuto.</t>
   </si>
 </sst>
 </file>
@@ -5367,14 +5600,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W755"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
+      <selection pane="bottomRight" activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5455,7 +5687,7 @@
       </c>
       <c r="D3" s="47"/>
       <c r="E3" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -5483,7 +5715,7 @@
       </c>
       <c r="D4" s="47"/>
       <c r="E4" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -5511,7 +5743,7 @@
       </c>
       <c r="D5" s="47"/>
       <c r="E5" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -5752,7 +5984,9 @@
       <c r="N11" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O11" s="38"/>
+      <c r="O11" s="38" t="s">
+        <v>754</v>
+      </c>
       <c r="P11" s="38" t="s">
         <v>64</v>
       </c>
@@ -5763,18 +5997,20 @@
         <v>64</v>
       </c>
       <c r="S11" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T11" s="38" t="s">
         <v>230</v>
       </c>
       <c r="U11" s="39"/>
-      <c r="V11" s="40"/>
+      <c r="V11" s="40" t="s">
+        <v>753</v>
+      </c>
       <c r="W11" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35">
         <v>29</v>
       </c>
@@ -5829,7 +6065,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="35">
         <v>30</v>
       </c>
@@ -5866,7 +6102,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>31</v>
       </c>
@@ -5921,7 +6157,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35">
         <v>32</v>
       </c>
@@ -5976,7 +6212,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35">
         <v>33</v>
       </c>
@@ -6013,7 +6249,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35">
         <v>34</v>
       </c>
@@ -6050,7 +6286,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35">
         <v>35</v>
       </c>
@@ -6120,7 +6356,9 @@
       <c r="N19" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O19" s="38"/>
+      <c r="O19" s="38" t="s">
+        <v>756</v>
+      </c>
       <c r="P19" s="38" t="s">
         <v>64</v>
       </c>
@@ -6131,18 +6369,20 @@
         <v>64</v>
       </c>
       <c r="S19" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T19" s="38" t="s">
         <v>230</v>
       </c>
       <c r="U19" s="39"/>
-      <c r="V19" s="40"/>
+      <c r="V19" s="40" t="s">
+        <v>755</v>
+      </c>
       <c r="W19" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35">
         <v>37</v>
       </c>
@@ -6197,7 +6437,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35">
         <v>38</v>
       </c>
@@ -6234,7 +6474,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35">
         <v>39</v>
       </c>
@@ -6289,7 +6529,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35">
         <v>40</v>
       </c>
@@ -6344,7 +6584,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35">
         <v>41</v>
       </c>
@@ -6381,7 +6621,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35">
         <v>42</v>
       </c>
@@ -6418,7 +6658,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="35">
         <v>43</v>
       </c>
@@ -6490,7 +6730,9 @@
       <c r="N27" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O27" s="38"/>
+      <c r="O27" s="38" t="s">
+        <v>757</v>
+      </c>
       <c r="P27" s="38" t="s">
         <v>64</v>
       </c>
@@ -6501,7 +6743,7 @@
         <v>64</v>
       </c>
       <c r="S27" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T27" s="38" t="s">
         <v>230</v>
@@ -6514,7 +6756,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35">
         <v>45</v>
       </c>
@@ -6549,7 +6791,9 @@
       <c r="N28" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O28" s="38"/>
+      <c r="O28" s="38" t="s">
+        <v>758</v>
+      </c>
       <c r="P28" s="38" t="s">
         <v>64</v>
       </c>
@@ -6573,7 +6817,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="35">
         <v>46</v>
       </c>
@@ -6612,7 +6856,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="35">
         <v>47</v>
       </c>
@@ -6647,7 +6891,9 @@
       <c r="N30" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O30" s="38"/>
+      <c r="O30" s="38" t="s">
+        <v>759</v>
+      </c>
       <c r="P30" s="38" t="s">
         <v>64</v>
       </c>
@@ -6671,7 +6917,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="35">
         <v>48</v>
       </c>
@@ -6706,7 +6952,9 @@
       <c r="N31" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O31" s="38"/>
+      <c r="O31" s="38" t="s">
+        <v>760</v>
+      </c>
       <c r="P31" s="38" t="s">
         <v>64</v>
       </c>
@@ -6730,7 +6978,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35">
         <v>49</v>
       </c>
@@ -6769,7 +7017,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35">
         <v>50</v>
       </c>
@@ -6808,7 +7056,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="35">
         <v>51</v>
       </c>
@@ -6886,7 +7134,9 @@
       <c r="N35" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O35" s="38"/>
+      <c r="O35" s="38" t="s">
+        <v>700</v>
+      </c>
       <c r="P35" s="38" t="s">
         <v>64</v>
       </c>
@@ -6897,7 +7147,7 @@
         <v>64</v>
       </c>
       <c r="S35" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T35" s="38" t="s">
         <v>230</v>
@@ -6949,7 +7199,9 @@
       <c r="N36" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O36" s="38"/>
+      <c r="O36" s="38" t="s">
+        <v>701</v>
+      </c>
       <c r="P36" s="38" t="s">
         <v>64</v>
       </c>
@@ -6960,7 +7212,7 @@
         <v>64</v>
       </c>
       <c r="S36" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T36" s="38" t="s">
         <v>230</v>
@@ -7012,7 +7264,9 @@
       <c r="N37" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O37" s="38"/>
+      <c r="O37" s="38" t="s">
+        <v>702</v>
+      </c>
       <c r="P37" s="38" t="s">
         <v>64</v>
       </c>
@@ -7023,7 +7277,7 @@
         <v>64</v>
       </c>
       <c r="S37" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T37" s="38" t="s">
         <v>230</v>
@@ -7075,7 +7329,9 @@
       <c r="N38" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O38" s="38"/>
+      <c r="O38" s="38" t="s">
+        <v>703</v>
+      </c>
       <c r="P38" s="38" t="s">
         <v>64</v>
       </c>
@@ -7086,7 +7342,7 @@
         <v>64</v>
       </c>
       <c r="S38" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T38" s="38" t="s">
         <v>230</v>
@@ -7116,16 +7372,16 @@
         <v>79</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="G39" s="37" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="H39" s="37" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
       <c r="I39" s="42" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="J39" s="38" t="s">
         <v>64</v>
@@ -7138,7 +7394,9 @@
       <c r="N39" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O39" s="38"/>
+      <c r="O39" s="38" t="s">
+        <v>704</v>
+      </c>
       <c r="P39" s="38" t="s">
         <v>64</v>
       </c>
@@ -7149,14 +7407,14 @@
         <v>64</v>
       </c>
       <c r="S39" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T39" s="38" t="s">
         <v>230</v>
       </c>
       <c r="U39" s="39"/>
       <c r="V39" s="40" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="W39" s="38" t="s">
         <v>44</v>
@@ -7201,7 +7459,9 @@
       <c r="N40" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O40" s="38"/>
+      <c r="O40" s="38" t="s">
+        <v>705</v>
+      </c>
       <c r="P40" s="38" t="s">
         <v>64</v>
       </c>
@@ -7212,7 +7472,7 @@
         <v>64</v>
       </c>
       <c r="S40" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T40" s="38" t="s">
         <v>230</v>
@@ -7264,7 +7524,9 @@
       <c r="N41" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O41" s="38"/>
+      <c r="O41" s="38" t="s">
+        <v>706</v>
+      </c>
       <c r="P41" s="38" t="s">
         <v>64</v>
       </c>
@@ -7275,7 +7537,7 @@
         <v>64</v>
       </c>
       <c r="S41" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T41" s="38" t="s">
         <v>230</v>
@@ -7327,7 +7589,9 @@
       <c r="N42" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O42" s="38"/>
+      <c r="O42" s="38" t="s">
+        <v>707</v>
+      </c>
       <c r="P42" s="38" t="s">
         <v>64</v>
       </c>
@@ -7338,7 +7602,7 @@
         <v>64</v>
       </c>
       <c r="S42" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T42" s="38" t="s">
         <v>230</v>
@@ -7390,7 +7654,9 @@
       <c r="N43" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O43" s="38"/>
+      <c r="O43" s="38" t="s">
+        <v>708</v>
+      </c>
       <c r="P43" s="38" t="s">
         <v>64</v>
       </c>
@@ -7401,7 +7667,7 @@
         <v>64</v>
       </c>
       <c r="S43" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T43" s="38" t="s">
         <v>230</v>
@@ -7414,7 +7680,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35">
         <v>64</v>
       </c>
@@ -7451,7 +7717,9 @@
       <c r="N44" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O44" s="38"/>
+      <c r="O44" s="38" t="s">
+        <v>700</v>
+      </c>
       <c r="P44" s="38" t="s">
         <v>64</v>
       </c>
@@ -7475,7 +7743,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35">
         <v>66</v>
       </c>
@@ -7512,7 +7780,9 @@
       <c r="N45" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O45" s="38"/>
+      <c r="O45" s="38" t="s">
+        <v>709</v>
+      </c>
       <c r="P45" s="38" t="s">
         <v>64</v>
       </c>
@@ -7536,7 +7806,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="35">
         <v>67</v>
       </c>
@@ -7573,7 +7843,9 @@
       <c r="N46" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O46" s="38"/>
+      <c r="O46" s="38" t="s">
+        <v>710</v>
+      </c>
       <c r="P46" s="38" t="s">
         <v>64</v>
       </c>
@@ -7597,7 +7869,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="35">
         <v>68</v>
       </c>
@@ -7634,7 +7906,9 @@
       <c r="N47" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O47" s="38"/>
+      <c r="O47" s="38" t="s">
+        <v>703</v>
+      </c>
       <c r="P47" s="38" t="s">
         <v>64</v>
       </c>
@@ -7658,7 +7932,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="35">
         <v>69</v>
       </c>
@@ -7695,7 +7969,9 @@
       <c r="N48" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O48" s="38"/>
+      <c r="O48" s="38" t="s">
+        <v>711</v>
+      </c>
       <c r="P48" s="38" t="s">
         <v>64</v>
       </c>
@@ -7719,7 +7995,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="35">
         <v>70</v>
       </c>
@@ -7756,7 +8032,9 @@
       <c r="N49" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O49" s="38"/>
+      <c r="O49" s="38" t="s">
+        <v>712</v>
+      </c>
       <c r="P49" s="38" t="s">
         <v>64</v>
       </c>
@@ -7780,7 +8058,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="35">
         <v>71</v>
       </c>
@@ -7817,7 +8095,9 @@
       <c r="N50" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O50" s="38"/>
+      <c r="O50" s="38" t="s">
+        <v>713</v>
+      </c>
       <c r="P50" s="38" t="s">
         <v>64</v>
       </c>
@@ -7841,7 +8121,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="35">
         <v>72</v>
       </c>
@@ -7878,7 +8158,9 @@
       <c r="N51" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O51" s="38"/>
+      <c r="O51" s="38" t="s">
+        <v>714</v>
+      </c>
       <c r="P51" s="38" t="s">
         <v>64</v>
       </c>
@@ -7902,7 +8184,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="35">
         <v>73</v>
       </c>
@@ -7939,7 +8221,9 @@
       <c r="N52" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O52" s="38"/>
+      <c r="O52" s="38" t="s">
+        <v>715</v>
+      </c>
       <c r="P52" s="38" t="s">
         <v>64</v>
       </c>
@@ -7963,7 +8247,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="35">
         <v>74</v>
       </c>
@@ -8000,7 +8284,9 @@
       <c r="N53" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O53" s="38"/>
+      <c r="O53" s="38" t="s">
+        <v>716</v>
+      </c>
       <c r="P53" s="38" t="s">
         <v>64</v>
       </c>
@@ -8024,7 +8310,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="35">
         <v>76</v>
       </c>
@@ -8061,7 +8347,9 @@
       <c r="N54" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O54" s="38"/>
+      <c r="O54" s="38" t="s">
+        <v>700</v>
+      </c>
       <c r="P54" s="38" t="s">
         <v>64</v>
       </c>
@@ -8085,7 +8373,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="35">
         <v>78</v>
       </c>
@@ -8122,7 +8410,9 @@
       <c r="N55" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O55" s="38"/>
+      <c r="O55" s="38" t="s">
+        <v>717</v>
+      </c>
       <c r="P55" s="38" t="s">
         <v>64</v>
       </c>
@@ -8146,7 +8436,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="35">
         <v>79</v>
       </c>
@@ -8183,7 +8473,9 @@
       <c r="N56" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O56" s="38"/>
+      <c r="O56" s="38" t="s">
+        <v>718</v>
+      </c>
       <c r="P56" s="38" t="s">
         <v>64</v>
       </c>
@@ -8207,7 +8499,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="35">
         <v>80</v>
       </c>
@@ -8244,7 +8536,9 @@
       <c r="N57" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O57" s="38"/>
+      <c r="O57" s="38" t="s">
+        <v>703</v>
+      </c>
       <c r="P57" s="38" t="s">
         <v>64</v>
       </c>
@@ -8268,7 +8562,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="35">
         <v>81</v>
       </c>
@@ -8305,7 +8599,9 @@
       <c r="N58" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O58" s="38"/>
+      <c r="O58" s="38" t="s">
+        <v>719</v>
+      </c>
       <c r="P58" s="38" t="s">
         <v>64</v>
       </c>
@@ -8329,7 +8625,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="35">
         <v>82</v>
       </c>
@@ -8346,16 +8642,16 @@
         <v>312</v>
       </c>
       <c r="F59" s="37" t="s">
-        <v>492</v>
+        <v>724</v>
       </c>
       <c r="G59" s="37" t="s">
-        <v>564</v>
+        <v>723</v>
       </c>
       <c r="H59" s="37" t="s">
-        <v>563</v>
+        <v>722</v>
       </c>
       <c r="I59" s="42" t="s">
-        <v>562</v>
+        <v>721</v>
       </c>
       <c r="J59" s="38"/>
       <c r="K59" s="38"/>
@@ -8366,7 +8662,9 @@
       <c r="N59" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O59" s="38"/>
+      <c r="O59" s="38" t="s">
+        <v>704</v>
+      </c>
       <c r="P59" s="38" t="s">
         <v>64</v>
       </c>
@@ -8384,13 +8682,13 @@
       </c>
       <c r="U59" s="39"/>
       <c r="V59" s="40" t="s">
-        <v>561</v>
+        <v>720</v>
       </c>
       <c r="W59" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="35">
         <v>83</v>
       </c>
@@ -8410,13 +8708,13 @@
         <v>492</v>
       </c>
       <c r="G60" s="37" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="H60" s="37" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="I60" s="42" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="J60" s="38"/>
       <c r="K60" s="38"/>
@@ -8427,7 +8725,9 @@
       <c r="N60" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O60" s="38"/>
+      <c r="O60" s="38" t="s">
+        <v>725</v>
+      </c>
       <c r="P60" s="38" t="s">
         <v>64</v>
       </c>
@@ -8445,13 +8745,13 @@
       </c>
       <c r="U60" s="39"/>
       <c r="V60" s="40" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="W60" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="35">
         <v>84</v>
       </c>
@@ -8471,13 +8771,13 @@
         <v>492</v>
       </c>
       <c r="G61" s="37" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="H61" s="37" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="I61" s="42" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="J61" s="38"/>
       <c r="K61" s="38"/>
@@ -8488,7 +8788,9 @@
       <c r="N61" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O61" s="38"/>
+      <c r="O61" s="38" t="s">
+        <v>726</v>
+      </c>
       <c r="P61" s="38" t="s">
         <v>64</v>
       </c>
@@ -8506,13 +8808,13 @@
       </c>
       <c r="U61" s="39"/>
       <c r="V61" s="40" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="W61" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="35">
         <v>85</v>
       </c>
@@ -8532,13 +8834,13 @@
         <v>492</v>
       </c>
       <c r="G62" s="37" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="H62" s="37" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="I62" s="42" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="J62" s="38"/>
       <c r="K62" s="38"/>
@@ -8549,7 +8851,9 @@
       <c r="N62" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O62" s="38"/>
+      <c r="O62" s="38" t="s">
+        <v>727</v>
+      </c>
       <c r="P62" s="38" t="s">
         <v>64</v>
       </c>
@@ -8567,13 +8871,13 @@
       </c>
       <c r="U62" s="39"/>
       <c r="V62" s="40" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="W62" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="35">
         <v>86</v>
       </c>
@@ -8593,13 +8897,13 @@
         <v>492</v>
       </c>
       <c r="G63" s="37" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="H63" s="37" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="I63" s="42" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="J63" s="38"/>
       <c r="K63" s="38"/>
@@ -8610,7 +8914,9 @@
       <c r="N63" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O63" s="38"/>
+      <c r="O63" s="38" t="s">
+        <v>728</v>
+      </c>
       <c r="P63" s="38" t="s">
         <v>64</v>
       </c>
@@ -8628,13 +8934,13 @@
       </c>
       <c r="U63" s="39"/>
       <c r="V63" s="40" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="W63" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="35">
         <v>87</v>
       </c>
@@ -8654,13 +8960,13 @@
         <v>492</v>
       </c>
       <c r="G64" s="37" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="H64" s="37" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="I64" s="42" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="J64" s="38"/>
       <c r="K64" s="38"/>
@@ -8671,7 +8977,9 @@
       <c r="N64" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O64" s="38"/>
+      <c r="O64" s="38" t="s">
+        <v>729</v>
+      </c>
       <c r="P64" s="38" t="s">
         <v>64</v>
       </c>
@@ -8689,13 +8997,13 @@
       </c>
       <c r="U64" s="39"/>
       <c r="V64" s="40" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="W64" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="35">
         <v>88</v>
       </c>
@@ -8715,13 +9023,13 @@
         <v>492</v>
       </c>
       <c r="G65" s="37" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="H65" s="37" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="I65" s="42" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="J65" s="38"/>
       <c r="K65" s="38"/>
@@ -8732,7 +9040,9 @@
       <c r="N65" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O65" s="38"/>
+      <c r="O65" s="38" t="s">
+        <v>730</v>
+      </c>
       <c r="P65" s="38" t="s">
         <v>64</v>
       </c>
@@ -8750,13 +9060,13 @@
       </c>
       <c r="U65" s="39"/>
       <c r="V65" s="40" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="W65" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="35">
         <v>89</v>
       </c>
@@ -8776,13 +9086,13 @@
         <v>492</v>
       </c>
       <c r="G66" s="37" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="H66" s="37" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="I66" s="42" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="J66" s="38"/>
       <c r="K66" s="38"/>
@@ -8793,7 +9103,9 @@
       <c r="N66" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O66" s="38"/>
+      <c r="O66" s="38" t="s">
+        <v>731</v>
+      </c>
       <c r="P66" s="38" t="s">
         <v>64</v>
       </c>
@@ -8811,13 +9123,13 @@
       </c>
       <c r="U66" s="39"/>
       <c r="V66" s="40" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="W66" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="35">
         <v>90</v>
       </c>
@@ -8837,13 +9149,13 @@
         <v>492</v>
       </c>
       <c r="G67" s="37" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="H67" s="37" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="I67" s="42" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="J67" s="38"/>
       <c r="K67" s="38"/>
@@ -8854,7 +9166,9 @@
       <c r="N67" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O67" s="38"/>
+      <c r="O67" s="38" t="s">
+        <v>730</v>
+      </c>
       <c r="P67" s="38" t="s">
         <v>64</v>
       </c>
@@ -8872,13 +9186,13 @@
       </c>
       <c r="U67" s="39"/>
       <c r="V67" s="40" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="W67" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="35">
         <v>91</v>
       </c>
@@ -8898,13 +9212,13 @@
         <v>492</v>
       </c>
       <c r="G68" s="37" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="H68" s="37" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="I68" s="42" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="J68" s="38"/>
       <c r="K68" s="38"/>
@@ -8915,7 +9229,9 @@
       <c r="N68" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O68" s="38"/>
+      <c r="O68" s="38" t="s">
+        <v>732</v>
+      </c>
       <c r="P68" s="38" t="s">
         <v>64</v>
       </c>
@@ -8933,13 +9249,13 @@
       </c>
       <c r="U68" s="39"/>
       <c r="V68" s="40" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="W68" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="35">
         <v>92</v>
       </c>
@@ -8959,13 +9275,13 @@
         <v>492</v>
       </c>
       <c r="G69" s="37" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H69" s="37" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="I69" s="42" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="J69" s="38"/>
       <c r="K69" s="38"/>
@@ -8976,7 +9292,9 @@
       <c r="N69" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O69" s="38"/>
+      <c r="O69" s="38" t="s">
+        <v>733</v>
+      </c>
       <c r="P69" s="38" t="s">
         <v>64</v>
       </c>
@@ -8994,13 +9312,13 @@
       </c>
       <c r="U69" s="39"/>
       <c r="V69" s="40" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="W69" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="35">
         <v>93</v>
       </c>
@@ -9020,13 +9338,13 @@
         <v>492</v>
       </c>
       <c r="G70" s="37" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="H70" s="37" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="I70" s="42" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="J70" s="38"/>
       <c r="K70" s="38"/>
@@ -9037,7 +9355,9 @@
       <c r="N70" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O70" s="38"/>
+      <c r="O70" s="38" t="s">
+        <v>734</v>
+      </c>
       <c r="P70" s="38" t="s">
         <v>64</v>
       </c>
@@ -9055,13 +9375,13 @@
       </c>
       <c r="U70" s="39"/>
       <c r="V70" s="40" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="W70" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="35">
         <v>95</v>
       </c>
@@ -9098,7 +9418,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="35">
         <v>97</v>
       </c>
@@ -9135,7 +9455,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="35">
         <v>98</v>
       </c>
@@ -9172,7 +9492,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="35">
         <v>99</v>
       </c>
@@ -9209,7 +9529,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="35">
         <v>100</v>
       </c>
@@ -9246,7 +9566,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="35">
         <v>101</v>
       </c>
@@ -9283,7 +9603,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="35">
         <v>102</v>
       </c>
@@ -9320,7 +9640,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="35">
         <v>103</v>
       </c>
@@ -9357,7 +9677,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="35">
         <v>104</v>
       </c>
@@ -9394,7 +9714,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="35">
         <v>105</v>
       </c>
@@ -9431,7 +9751,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="35">
         <v>106</v>
       </c>
@@ -9468,7 +9788,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="35">
         <v>108</v>
       </c>
@@ -9505,7 +9825,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="35">
         <v>110</v>
       </c>
@@ -9542,7 +9862,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="35">
         <v>111</v>
       </c>
@@ -9579,7 +9899,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="35">
         <v>112</v>
       </c>
@@ -9616,7 +9936,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="35">
         <v>113</v>
       </c>
@@ -9653,7 +9973,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="35">
         <v>114</v>
       </c>
@@ -9690,7 +10010,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="35">
         <v>115</v>
       </c>
@@ -9727,7 +10047,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="35">
         <v>116</v>
       </c>
@@ -9764,7 +10084,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="35">
         <v>117</v>
       </c>
@@ -9801,7 +10121,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="35">
         <v>118</v>
       </c>
@@ -9838,7 +10158,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="35">
         <v>119</v>
       </c>
@@ -9875,7 +10195,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="35">
         <v>120</v>
       </c>
@@ -9912,7 +10232,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="35">
         <v>121</v>
       </c>
@@ -9949,7 +10269,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="35">
         <v>123</v>
       </c>
@@ -9986,7 +10306,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="35">
         <v>125</v>
       </c>
@@ -10023,7 +10343,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="35">
         <v>126</v>
       </c>
@@ -10060,7 +10380,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="35">
         <v>127</v>
       </c>
@@ -10097,7 +10417,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="35">
         <v>128</v>
       </c>
@@ -10134,7 +10454,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="35">
         <v>129</v>
       </c>
@@ -10171,7 +10491,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="35">
         <v>130</v>
       </c>
@@ -10208,7 +10528,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="35">
         <v>131</v>
       </c>
@@ -10245,7 +10565,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="35">
         <v>132</v>
       </c>
@@ -10282,7 +10602,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="35">
         <v>133</v>
       </c>
@@ -10319,7 +10639,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="35">
         <v>134</v>
       </c>
@@ -10356,7 +10676,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="35">
         <v>135</v>
       </c>
@@ -10393,7 +10713,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="35">
         <v>136</v>
       </c>
@@ -10430,7 +10750,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="35">
         <v>137</v>
       </c>
@@ -10467,7 +10787,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="35">
         <v>138</v>
       </c>
@@ -10504,7 +10824,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="35">
         <v>139</v>
       </c>
@@ -10541,7 +10861,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="35">
         <v>140</v>
       </c>
@@ -10578,7 +10898,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="35">
         <v>141</v>
       </c>
@@ -10615,7 +10935,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="35">
         <v>142</v>
       </c>
@@ -10652,7 +10972,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="35">
         <v>143</v>
       </c>
@@ -10689,7 +11009,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="35">
         <v>144</v>
       </c>
@@ -10726,7 +11046,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="35">
         <v>145</v>
       </c>
@@ -10763,7 +11083,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="35">
         <v>146</v>
       </c>
@@ -10800,7 +11120,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="35">
         <v>152</v>
       </c>
@@ -10817,16 +11137,16 @@
         <v>344</v>
       </c>
       <c r="F118" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G118" s="37" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="H118" s="37" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="I118" s="37" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="J118" s="38"/>
       <c r="K118" s="38"/>
@@ -10837,7 +11157,9 @@
       <c r="N118" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O118" s="38"/>
+      <c r="O118" s="38" t="s">
+        <v>700</v>
+      </c>
       <c r="P118" s="38" t="s">
         <v>64</v>
       </c>
@@ -10855,13 +11177,13 @@
       </c>
       <c r="U118" s="39"/>
       <c r="V118" s="40" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="W118" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="35">
         <v>154</v>
       </c>
@@ -10878,16 +11200,16 @@
         <v>345</v>
       </c>
       <c r="F119" s="37" t="s">
+        <v>621</v>
+      </c>
+      <c r="G119" s="37" t="s">
         <v>625</v>
       </c>
-      <c r="G119" s="37" t="s">
-        <v>629</v>
-      </c>
       <c r="H119" s="37" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="I119" s="42" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="J119" s="38"/>
       <c r="K119" s="38"/>
@@ -10898,7 +11220,9 @@
       <c r="N119" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O119" s="38"/>
+      <c r="O119" s="38" t="s">
+        <v>735</v>
+      </c>
       <c r="P119" s="38" t="s">
         <v>64</v>
       </c>
@@ -10916,13 +11240,13 @@
       </c>
       <c r="U119" s="39"/>
       <c r="V119" s="40" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="W119" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="35">
         <v>155</v>
       </c>
@@ -10939,16 +11263,16 @@
         <v>346</v>
       </c>
       <c r="F120" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G120" s="37" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="H120" s="37" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="I120" s="42" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="J120" s="38"/>
       <c r="K120" s="38"/>
@@ -10959,7 +11283,9 @@
       <c r="N120" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O120" s="38"/>
+      <c r="O120" s="38" t="s">
+        <v>718</v>
+      </c>
       <c r="P120" s="38" t="s">
         <v>64</v>
       </c>
@@ -10977,13 +11303,13 @@
       </c>
       <c r="U120" s="39"/>
       <c r="V120" s="40" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="W120" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="35">
         <v>156</v>
       </c>
@@ -11000,16 +11326,16 @@
         <v>347</v>
       </c>
       <c r="F121" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G121" s="37" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="H121" s="37" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="I121" s="42" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="J121" s="38"/>
       <c r="K121" s="38"/>
@@ -11020,7 +11346,9 @@
       <c r="N121" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O121" s="38"/>
+      <c r="O121" s="38" t="s">
+        <v>703</v>
+      </c>
       <c r="P121" s="38" t="s">
         <v>64</v>
       </c>
@@ -11038,13 +11366,13 @@
       </c>
       <c r="U121" s="39"/>
       <c r="V121" s="40" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="W121" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="35">
         <v>158</v>
       </c>
@@ -11061,16 +11389,16 @@
         <v>348</v>
       </c>
       <c r="F122" s="37" t="s">
-        <v>625</v>
+        <v>724</v>
       </c>
       <c r="G122" s="37" t="s">
-        <v>641</v>
+        <v>739</v>
       </c>
       <c r="H122" s="37" t="s">
-        <v>640</v>
+        <v>738</v>
       </c>
       <c r="I122" s="42" t="s">
-        <v>639</v>
+        <v>737</v>
       </c>
       <c r="J122" s="38"/>
       <c r="K122" s="38"/>
@@ -11081,7 +11409,9 @@
       <c r="N122" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O122" s="38"/>
+      <c r="O122" s="38" t="s">
+        <v>704</v>
+      </c>
       <c r="P122" s="38" t="s">
         <v>64</v>
       </c>
@@ -11099,13 +11429,13 @@
       </c>
       <c r="U122" s="39"/>
       <c r="V122" s="40" t="s">
-        <v>638</v>
+        <v>736</v>
       </c>
       <c r="W122" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="35">
         <v>159</v>
       </c>
@@ -11122,16 +11452,16 @@
         <v>192</v>
       </c>
       <c r="F123" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G123" s="37" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="H123" s="37" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="I123" s="42" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="J123" s="38"/>
       <c r="K123" s="38"/>
@@ -11142,7 +11472,9 @@
       <c r="N123" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O123" s="38"/>
+      <c r="O123" s="38" t="s">
+        <v>725</v>
+      </c>
       <c r="P123" s="38" t="s">
         <v>64</v>
       </c>
@@ -11160,13 +11492,13 @@
       </c>
       <c r="U123" s="39"/>
       <c r="V123" s="40" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="W123" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="35">
         <v>160</v>
       </c>
@@ -11183,16 +11515,16 @@
         <v>194</v>
       </c>
       <c r="F124" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G124" s="37" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="H124" s="37" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="I124" s="42" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="J124" s="38"/>
       <c r="K124" s="38"/>
@@ -11203,7 +11535,9 @@
       <c r="N124" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O124" s="38"/>
+      <c r="O124" s="38" t="s">
+        <v>740</v>
+      </c>
       <c r="P124" s="38" t="s">
         <v>64</v>
       </c>
@@ -11221,13 +11555,13 @@
       </c>
       <c r="U124" s="39"/>
       <c r="V124" s="40" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="W124" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="35">
         <v>161</v>
       </c>
@@ -11244,16 +11578,16 @@
         <v>284</v>
       </c>
       <c r="F125" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G125" s="37" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="H125" s="37" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="I125" s="42" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="J125" s="38"/>
       <c r="K125" s="38"/>
@@ -11264,7 +11598,9 @@
       <c r="N125" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O125" s="38"/>
+      <c r="O125" s="38" t="s">
+        <v>741</v>
+      </c>
       <c r="P125" s="38" t="s">
         <v>64</v>
       </c>
@@ -11282,13 +11618,13 @@
       </c>
       <c r="U125" s="39"/>
       <c r="V125" s="40" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="W125" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="35">
         <v>162</v>
       </c>
@@ -11305,16 +11641,16 @@
         <v>285</v>
       </c>
       <c r="F126" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G126" s="37" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="H126" s="37" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="I126" s="42" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="J126" s="38"/>
       <c r="K126" s="38"/>
@@ -11325,7 +11661,9 @@
       <c r="N126" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O126" s="38"/>
+      <c r="O126" s="38" t="s">
+        <v>742</v>
+      </c>
       <c r="P126" s="38" t="s">
         <v>64</v>
       </c>
@@ -11343,13 +11681,13 @@
       </c>
       <c r="U126" s="39"/>
       <c r="V126" s="40" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="W126" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="35">
         <v>163</v>
       </c>
@@ -11366,16 +11704,16 @@
         <v>286</v>
       </c>
       <c r="F127" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G127" s="37" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="H127" s="37" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="I127" s="42" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="J127" s="38"/>
       <c r="K127" s="38"/>
@@ -11386,7 +11724,9 @@
       <c r="N127" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O127" s="38"/>
+      <c r="O127" s="38" t="s">
+        <v>740</v>
+      </c>
       <c r="P127" s="38" t="s">
         <v>64</v>
       </c>
@@ -11404,13 +11744,13 @@
       </c>
       <c r="U127" s="39"/>
       <c r="V127" s="40" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="W127" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="35">
         <v>164</v>
       </c>
@@ -11427,16 +11767,16 @@
         <v>287</v>
       </c>
       <c r="F128" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G128" s="37" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="H128" s="37" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="I128" s="42" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="J128" s="38"/>
       <c r="K128" s="38"/>
@@ -11447,7 +11787,9 @@
       <c r="N128" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O128" s="38"/>
+      <c r="O128" s="38" t="s">
+        <v>743</v>
+      </c>
       <c r="P128" s="38" t="s">
         <v>64</v>
       </c>
@@ -11465,13 +11807,13 @@
       </c>
       <c r="U128" s="39"/>
       <c r="V128" s="40" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="W128" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="35">
         <v>165</v>
       </c>
@@ -11488,16 +11830,16 @@
         <v>288</v>
       </c>
       <c r="F129" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G129" s="37" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="H129" s="37" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="I129" s="42" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="J129" s="38"/>
       <c r="K129" s="38"/>
@@ -11508,7 +11850,9 @@
       <c r="N129" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O129" s="38"/>
+      <c r="O129" s="38" t="s">
+        <v>744</v>
+      </c>
       <c r="P129" s="38" t="s">
         <v>64</v>
       </c>
@@ -11526,13 +11870,13 @@
       </c>
       <c r="U129" s="39"/>
       <c r="V129" s="40" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="W129" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="35">
         <v>166</v>
       </c>
@@ -11549,16 +11893,16 @@
         <v>289</v>
       </c>
       <c r="F130" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G130" s="37" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="H130" s="37" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="I130" s="42" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="J130" s="38"/>
       <c r="K130" s="38"/>
@@ -11569,7 +11913,9 @@
       <c r="N130" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O130" s="38"/>
+      <c r="O130" s="38" t="s">
+        <v>745</v>
+      </c>
       <c r="P130" s="38" t="s">
         <v>64</v>
       </c>
@@ -11587,13 +11933,13 @@
       </c>
       <c r="U130" s="39"/>
       <c r="V130" s="40" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="W130" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="35">
         <v>167</v>
       </c>
@@ -11610,16 +11956,16 @@
         <v>290</v>
       </c>
       <c r="F131" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G131" s="37" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="H131" s="37" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="I131" s="42" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="J131" s="38"/>
       <c r="K131" s="38"/>
@@ -11630,7 +11976,9 @@
       <c r="N131" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O131" s="38"/>
+      <c r="O131" s="38" t="s">
+        <v>746</v>
+      </c>
       <c r="P131" s="38" t="s">
         <v>64</v>
       </c>
@@ -11648,13 +11996,13 @@
       </c>
       <c r="U131" s="39"/>
       <c r="V131" s="40" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="W131" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="35">
         <v>168</v>
       </c>
@@ -11671,16 +12019,16 @@
         <v>291</v>
       </c>
       <c r="F132" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G132" s="37" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="H132" s="37" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="I132" s="42" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="J132" s="38"/>
       <c r="K132" s="38"/>
@@ -11691,7 +12039,9 @@
       <c r="N132" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O132" s="38"/>
+      <c r="O132" s="38" t="s">
+        <v>747</v>
+      </c>
       <c r="P132" s="38" t="s">
         <v>64</v>
       </c>
@@ -11709,13 +12059,13 @@
       </c>
       <c r="U132" s="39"/>
       <c r="V132" s="40" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="W132" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="35">
         <v>169</v>
       </c>
@@ -11732,16 +12082,16 @@
         <v>293</v>
       </c>
       <c r="F133" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G133" s="37" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="H133" s="37" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="I133" s="42" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="J133" s="38"/>
       <c r="K133" s="38"/>
@@ -11752,7 +12102,9 @@
       <c r="N133" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O133" s="38"/>
+      <c r="O133" s="38" t="s">
+        <v>748</v>
+      </c>
       <c r="P133" s="38" t="s">
         <v>64</v>
       </c>
@@ -11770,13 +12122,13 @@
       </c>
       <c r="U133" s="39"/>
       <c r="V133" s="40" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="W133" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="35">
         <v>175</v>
       </c>
@@ -11813,7 +12165,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="35">
         <v>177</v>
       </c>
@@ -11850,7 +12202,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="35">
         <v>178</v>
       </c>
@@ -11887,7 +12239,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="35">
         <v>179</v>
       </c>
@@ -11924,7 +12276,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="138" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="35">
         <v>180</v>
       </c>
@@ -11961,7 +12313,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="139" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="35">
         <v>181</v>
       </c>
@@ -11998,7 +12350,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="140" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="35">
         <v>182</v>
       </c>
@@ -12035,7 +12387,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="141" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="35">
         <v>183</v>
       </c>
@@ -12072,7 +12424,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="142" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="35">
         <v>184</v>
       </c>
@@ -12109,7 +12461,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="143" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="35">
         <v>185</v>
       </c>
@@ -12146,7 +12498,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="144" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="35">
         <v>186</v>
       </c>
@@ -12183,7 +12535,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="145" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="35">
         <v>187</v>
       </c>
@@ -12220,7 +12572,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="146" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="35">
         <v>188</v>
       </c>
@@ -12257,7 +12609,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="147" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="35">
         <v>189</v>
       </c>
@@ -12294,7 +12646,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="35">
         <v>190</v>
       </c>
@@ -12417,7 +12769,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="35">
         <v>417</v>
       </c>
@@ -12454,7 +12806,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="35">
         <v>418</v>
       </c>
@@ -12491,7 +12843,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="35">
         <v>419</v>
       </c>
@@ -12528,7 +12880,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="35">
         <v>423</v>
       </c>
@@ -12565,7 +12917,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="35">
         <v>424</v>
       </c>
@@ -12602,7 +12954,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="35">
         <v>425</v>
       </c>
@@ -12639,7 +12991,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="35">
         <v>432</v>
       </c>
@@ -12676,7 +13028,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="35">
         <v>433</v>
       </c>
@@ -12713,7 +13065,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="35">
         <v>434</v>
       </c>
@@ -12750,7 +13102,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="35">
         <v>435</v>
       </c>
@@ -12787,7 +13139,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="35">
         <v>437</v>
       </c>
@@ -12824,7 +13176,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="35">
         <v>438</v>
       </c>
@@ -12861,7 +13213,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="35">
         <v>440</v>
       </c>
@@ -12898,7 +13250,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="164" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="35">
         <v>441</v>
       </c>
@@ -12935,7 +13287,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="165" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="35">
         <v>442</v>
       </c>
@@ -12972,7 +13324,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="166" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="35">
         <v>443</v>
       </c>
@@ -13009,7 +13361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="35">
         <v>444</v>
       </c>
@@ -13046,7 +13398,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="35">
         <v>445</v>
       </c>
@@ -13083,7 +13435,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="35">
         <v>448</v>
       </c>
@@ -13100,16 +13452,16 @@
         <v>395</v>
       </c>
       <c r="F169" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G169" s="37" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="H169" s="37" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="I169" s="42" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="J169" s="38"/>
       <c r="K169" s="38"/>
@@ -13138,13 +13490,13 @@
       </c>
       <c r="U169" s="39"/>
       <c r="V169" s="40" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="W169" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="35">
         <v>449</v>
       </c>
@@ -13161,16 +13513,16 @@
         <v>396</v>
       </c>
       <c r="F170" s="37" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G170" s="37" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="H170" s="37" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="I170" s="42" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="J170" s="38"/>
       <c r="K170" s="38"/>
@@ -13199,13 +13551,13 @@
       </c>
       <c r="U170" s="39"/>
       <c r="V170" s="40" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="W170" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="35">
         <v>450</v>
       </c>
@@ -13254,7 +13606,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="35">
         <v>451</v>
       </c>
@@ -13354,7 +13706,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="35">
         <v>454</v>
       </c>
@@ -13391,7 +13743,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="175" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="35">
         <v>455</v>
       </c>
@@ -13428,7 +13780,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="176" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="35">
         <v>456</v>
       </c>
@@ -13465,7 +13817,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="35">
         <v>457</v>
       </c>
@@ -13502,7 +13854,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="35">
         <v>458</v>
       </c>
@@ -13539,7 +13891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="35">
         <v>459</v>
       </c>
@@ -13576,7 +13928,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="35">
         <v>460</v>
       </c>
@@ -13613,7 +13965,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="35">
         <v>461</v>
       </c>
@@ -13630,16 +13982,16 @@
         <v>397</v>
       </c>
       <c r="F181" s="35" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G181" s="35" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="H181" s="35" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="I181" s="35" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="J181" s="38"/>
       <c r="K181" s="38"/>
@@ -13650,7 +14002,9 @@
       <c r="N181" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O181" s="35"/>
+      <c r="O181" s="38" t="s">
+        <v>749</v>
+      </c>
       <c r="P181" s="38" t="s">
         <v>64</v>
       </c>
@@ -13668,13 +14022,13 @@
       </c>
       <c r="U181" s="35"/>
       <c r="V181" s="38" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="W181" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="35">
         <v>462</v>
       </c>
@@ -13694,13 +14048,13 @@
         <v>492</v>
       </c>
       <c r="G182" s="35" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="H182" s="35" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="I182" s="35" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="J182" s="38"/>
       <c r="K182" s="38"/>
@@ -13711,7 +14065,9 @@
       <c r="N182" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O182" s="35"/>
+      <c r="O182" s="38" t="s">
+        <v>750</v>
+      </c>
       <c r="P182" s="38" t="s">
         <v>64</v>
       </c>
@@ -13729,13 +14085,13 @@
       </c>
       <c r="U182" s="35"/>
       <c r="V182" s="38" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="W182" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="35">
         <v>463</v>
       </c>
@@ -13772,7 +14128,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="184" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="35">
         <v>464</v>
       </c>
@@ -13809,7 +14165,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="35">
         <v>465</v>
       </c>
@@ -13885,7 +14241,9 @@
       <c r="N186" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O186" s="38"/>
+      <c r="O186" s="38" t="s">
+        <v>751</v>
+      </c>
       <c r="P186" s="38" t="s">
         <v>64</v>
       </c>
@@ -13896,7 +14254,7 @@
         <v>64</v>
       </c>
       <c r="S186" s="38" t="s">
-        <v>64</v>
+        <v>440</v>
       </c>
       <c r="T186" s="38" t="s">
         <v>230</v>
@@ -13909,7 +14267,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="19.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="35">
         <v>467</v>
       </c>
@@ -13946,7 +14304,9 @@
       <c r="N187" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O187" s="38"/>
+      <c r="O187" s="38" t="s">
+        <v>752</v>
+      </c>
       <c r="P187" s="38" t="s">
         <v>64</v>
       </c>
@@ -13970,7 +14330,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="18.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="35">
         <v>468</v>
       </c>
@@ -13987,16 +14347,16 @@
         <v>412</v>
       </c>
       <c r="F188" s="35" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="G188" s="35" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="H188" s="35" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="I188" s="35" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="J188" s="38"/>
       <c r="K188" s="38"/>
@@ -14007,7 +14367,9 @@
       <c r="N188" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="O188" s="35"/>
+      <c r="O188" s="38" t="s">
+        <v>750</v>
+      </c>
       <c r="P188" s="38" t="s">
         <v>64</v>
       </c>
@@ -14025,13 +14387,13 @@
       </c>
       <c r="U188" s="35"/>
       <c r="V188" s="38" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="W188" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="35">
         <v>469</v>
       </c>
@@ -14068,7 +14430,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="190" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="35">
         <v>470</v>
       </c>
@@ -14105,7 +14467,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="191" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="35">
         <v>471</v>
       </c>
@@ -14125,13 +14487,13 @@
         <v>492</v>
       </c>
       <c r="G191" s="37" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="H191" s="37" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="I191" s="42" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="J191" s="38"/>
       <c r="K191" s="38"/>
@@ -14148,13 +14510,13 @@
       </c>
       <c r="U191" s="39"/>
       <c r="V191" s="40" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="W191" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="192" spans="1:23" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="35">
         <v>472</v>
       </c>
@@ -14174,13 +14536,13 @@
         <v>492</v>
       </c>
       <c r="G192" s="37" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="H192" s="37" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="I192" s="42" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="J192" s="38"/>
       <c r="K192" s="38"/>
@@ -14197,7 +14559,7 @@
       </c>
       <c r="U192" s="39"/>
       <c r="V192" s="40" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="W192" s="38" t="s">
         <v>36</v>
@@ -18280,13 +18642,7 @@
     <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A9:W192" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="LAB"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:W192" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -20570,12 +20926,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20837,21 +21196,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20876,18 +21241,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiornati i test di time out
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111IGCOMSRLXXX/IGCOM/IGSUITE/4.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\igcom\FSE Fascicolo sanitario nazionale\FSE-Accreditamento\it-fse-accreditamento\GATEWAY\A1#111IGCOMSRLXXX\IGCOM\IGSUITE\4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8191BDBE-89A9-4C18-9973-017635BC6C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FCD0A1-990F-44F7-A9B6-81298E84510D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1939" uniqueCount="761">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -5603,10 +5603,10 @@
   <dimension ref="A1:W755"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="P11" sqref="P11:S150"/>
+      <selection pane="bottomRight" activeCell="S27" sqref="S27:S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6652,7 +6652,7 @@
       <c r="H27" s="37"/>
       <c r="I27" s="42"/>
       <c r="J27" s="38" t="s">
-        <v>232</v>
+        <v>64</v>
       </c>
       <c r="K27" s="38" t="s">
         <v>243</v>
@@ -6669,10 +6669,18 @@
       <c r="O27" s="38" t="s">
         <v>757</v>
       </c>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
+      <c r="P27" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q27" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="R27" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S27" s="38" t="s">
+        <v>440</v>
+      </c>
       <c r="T27" s="38" t="s">
         <v>230</v>
       </c>
@@ -6705,7 +6713,7 @@
       <c r="H28" s="37"/>
       <c r="I28" s="42"/>
       <c r="J28" s="38" t="s">
-        <v>232</v>
+        <v>64</v>
       </c>
       <c r="K28" s="38" t="s">
         <v>243</v>
@@ -6722,10 +6730,18 @@
       <c r="O28" s="38" t="s">
         <v>758</v>
       </c>
-      <c r="P28" s="38"/>
-      <c r="Q28" s="38"/>
-      <c r="R28" s="38"/>
-      <c r="S28" s="38"/>
+      <c r="P28" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q28" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="R28" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S28" s="38" t="s">
+        <v>440</v>
+      </c>
       <c r="T28" s="38" t="s">
         <v>230</v>
       </c>
@@ -6797,7 +6813,7 @@
       <c r="H30" s="37"/>
       <c r="I30" s="42"/>
       <c r="J30" s="38" t="s">
-        <v>232</v>
+        <v>64</v>
       </c>
       <c r="K30" s="38" t="s">
         <v>243</v>
@@ -6814,10 +6830,18 @@
       <c r="O30" s="38" t="s">
         <v>759</v>
       </c>
-      <c r="P30" s="38"/>
-      <c r="Q30" s="38"/>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
+      <c r="P30" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q30" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="R30" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S30" s="38" t="s">
+        <v>440</v>
+      </c>
       <c r="T30" s="38" t="s">
         <v>230</v>
       </c>
@@ -6850,7 +6874,7 @@
       <c r="H31" s="37"/>
       <c r="I31" s="42"/>
       <c r="J31" s="38" t="s">
-        <v>232</v>
+        <v>64</v>
       </c>
       <c r="K31" s="38" t="s">
         <v>243</v>
@@ -6867,10 +6891,18 @@
       <c r="O31" s="38" t="s">
         <v>760</v>
       </c>
-      <c r="P31" s="38"/>
-      <c r="Q31" s="38"/>
-      <c r="R31" s="38"/>
-      <c r="S31" s="38"/>
+      <c r="P31" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q31" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="R31" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S31" s="38" t="s">
+        <v>440</v>
+      </c>
       <c r="T31" s="38" t="s">
         <v>230</v>
       </c>
@@ -18567,7 +18599,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J10:J192 P10:R192 M10:N192</xm:sqref>
+          <xm:sqref>J10:J192 M10:N192 P10:R192</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
@@ -20830,12 +20862,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21097,21 +21132,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -21136,18 +21177,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>